<commit_message>
Code updated 23-01-16 11:30:36
</commit_message>
<xml_diff>
--- a/Season_Attack/82.xlsx
+++ b/Season_Attack/82.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G164"/>
+  <dimension ref="A1:I167"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,6 +426,16 @@
           <t>01-14_0</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>01-15_A</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>01-15_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -452,9 +462,15 @@
       <c r="F2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>4604</t>
+      <c r="G2" t="n">
+        <v>4604</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2504</t>
         </is>
       </c>
     </row>
@@ -483,9 +499,15 @@
       <c r="F3" s="3" t="n">
         <v>34</v>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>6101</t>
+      <c r="G3" t="n">
+        <v>6101</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>36</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>2840</t>
         </is>
       </c>
     </row>
@@ -514,9 +536,15 @@
       <c r="F4" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>6583</t>
+      <c r="G4" t="n">
+        <v>6583</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -545,9 +573,15 @@
       <c r="F5" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>6330</t>
+      <c r="G5" t="n">
+        <v>6330</v>
+      </c>
+      <c r="H5" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2820</t>
         </is>
       </c>
     </row>
@@ -576,9 +610,15 @@
       <c r="F6" s="3" t="n">
         <v>32</v>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>6320</t>
+      <c r="G6" t="n">
+        <v>6320</v>
+      </c>
+      <c r="H6" s="3" t="n">
+        <v>33</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>3013</t>
         </is>
       </c>
     </row>
@@ -607,9 +647,15 @@
       <c r="F7" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>5732</t>
+      <c r="G7" t="n">
+        <v>5732</v>
+      </c>
+      <c r="H7" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>2800</t>
         </is>
       </c>
     </row>
@@ -632,15 +678,21 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F8" s="3" t="n">
         <v>32</v>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>6111</t>
+      <c r="G8" t="n">
+        <v>6111</v>
+      </c>
+      <c r="H8" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>2850</t>
         </is>
       </c>
     </row>
@@ -669,9 +721,15 @@
       <c r="F9" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>3534</t>
+      <c r="G9" t="n">
+        <v>3534</v>
+      </c>
+      <c r="H9" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>2471</t>
         </is>
       </c>
     </row>
@@ -700,9 +758,15 @@
       <c r="F10" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>5738</t>
+      <c r="G10" t="n">
+        <v>5738</v>
+      </c>
+      <c r="H10" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>2830</t>
         </is>
       </c>
     </row>
@@ -731,9 +795,15 @@
       <c r="F11" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>7186</t>
+      <c r="G11" t="n">
+        <v>7186</v>
+      </c>
+      <c r="H11" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>2902</t>
         </is>
       </c>
     </row>
@@ -762,9 +832,15 @@
       <c r="F12" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>6075</t>
+      <c r="G12" t="n">
+        <v>6075</v>
+      </c>
+      <c r="H12" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>2797</t>
         </is>
       </c>
     </row>
@@ -793,9 +869,15 @@
       <c r="F13" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>2552</t>
         </is>
       </c>
     </row>
@@ -824,9 +906,15 @@
       <c r="F14" s="3" t="n">
         <v>38</v>
       </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>7281</t>
+      <c r="G14" t="n">
+        <v>7281</v>
+      </c>
+      <c r="H14" s="3" t="n">
+        <v>36</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>2953</t>
         </is>
       </c>
     </row>
@@ -855,9 +943,15 @@
       <c r="F15" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>6108</t>
+      <c r="G15" t="n">
+        <v>6108</v>
+      </c>
+      <c r="H15" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>2852</t>
         </is>
       </c>
     </row>
@@ -886,9 +980,15 @@
       <c r="F16" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>6840</t>
+      <c r="G16" t="n">
+        <v>6840</v>
+      </c>
+      <c r="H16" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>2945</t>
         </is>
       </c>
     </row>
@@ -917,9 +1017,15 @@
       <c r="F17" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>5630</t>
+      <c r="G17" t="n">
+        <v>5630</v>
+      </c>
+      <c r="H17" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>2891</t>
         </is>
       </c>
     </row>
@@ -942,15 +1048,21 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>Chinese</t>
         </is>
       </c>
       <c r="F18" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>6351</t>
+      <c r="G18" t="n">
+        <v>6351</v>
+      </c>
+      <c r="H18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -979,9 +1091,15 @@
       <c r="F19" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>7137</t>
+      <c r="G19" t="n">
+        <v>7137</v>
+      </c>
+      <c r="H19" s="3" t="n">
+        <v>31</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>2968</t>
         </is>
       </c>
     </row>
@@ -1010,9 +1128,15 @@
       <c r="F20" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>5881</t>
+      <c r="G20" t="n">
+        <v>5881</v>
+      </c>
+      <c r="H20" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>2791</t>
         </is>
       </c>
     </row>
@@ -1041,9 +1165,15 @@
       <c r="F21" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>6525</t>
+      <c r="G21" t="n">
+        <v>6525</v>
+      </c>
+      <c r="H21" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>3047</t>
         </is>
       </c>
     </row>
@@ -1072,9 +1202,15 @@
       <c r="F22" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>6196</t>
+      <c r="G22" t="n">
+        <v>6196</v>
+      </c>
+      <c r="H22" s="3" t="n">
+        <v>33</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>2734</t>
         </is>
       </c>
     </row>
@@ -1103,9 +1239,15 @@
       <c r="F23" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>5834</t>
+      <c r="G23" t="n">
+        <v>5834</v>
+      </c>
+      <c r="H23" s="3" t="n">
+        <v>33</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>2971</t>
         </is>
       </c>
     </row>
@@ -1134,7 +1276,13 @@
       <c r="F24" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G24" t="inlineStr">
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1165,9 +1313,15 @@
       <c r="F25" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>6268</t>
+      <c r="G25" t="n">
+        <v>6268</v>
+      </c>
+      <c r="H25" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>3057</t>
         </is>
       </c>
     </row>
@@ -1196,9 +1350,15 @@
       <c r="F26" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>6492</t>
+      <c r="G26" t="n">
+        <v>6492</v>
+      </c>
+      <c r="H26" s="3" t="n">
+        <v>36</v>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>3020</t>
         </is>
       </c>
     </row>
@@ -1221,15 +1381,21 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F27" s="4" t="n">
         <v>28</v>
       </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>6426</t>
+      <c r="G27" t="n">
+        <v>6426</v>
+      </c>
+      <c r="H27" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>2860</t>
         </is>
       </c>
     </row>
@@ -1258,9 +1424,15 @@
       <c r="F28" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>6924</t>
+      <c r="G28" t="n">
+        <v>6924</v>
+      </c>
+      <c r="H28" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>3048</t>
         </is>
       </c>
     </row>
@@ -1289,9 +1461,15 @@
       <c r="F29" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>6182</t>
+      <c r="G29" t="n">
+        <v>6182</v>
+      </c>
+      <c r="H29" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>2906</t>
         </is>
       </c>
     </row>
@@ -1320,9 +1498,15 @@
       <c r="F30" s="3" t="n">
         <v>37</v>
       </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>6388</t>
+      <c r="G30" t="n">
+        <v>6388</v>
+      </c>
+      <c r="H30" s="3" t="n">
+        <v>31</v>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>2978</t>
         </is>
       </c>
     </row>
@@ -1351,9 +1535,15 @@
       <c r="F31" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>7167</t>
+      <c r="G31" t="n">
+        <v>7167</v>
+      </c>
+      <c r="H31" s="3" t="n">
+        <v>36</v>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>2855</t>
         </is>
       </c>
     </row>
@@ -1382,9 +1572,15 @@
       <c r="F32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>2509</t>
         </is>
       </c>
     </row>
@@ -1407,15 +1603,21 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F33" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>6623</t>
+      <c r="G33" t="n">
+        <v>6623</v>
+      </c>
+      <c r="H33" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>2963</t>
         </is>
       </c>
     </row>
@@ -1444,9 +1646,15 @@
       <c r="F34" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>5648</t>
+      <c r="G34" t="n">
+        <v>5648</v>
+      </c>
+      <c r="H34" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>2755</t>
         </is>
       </c>
     </row>
@@ -1475,9 +1683,15 @@
       <c r="F35" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>5194</t>
+      <c r="G35" t="n">
+        <v>5194</v>
+      </c>
+      <c r="H35" s="3" t="n">
+        <v>33</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>2946</t>
         </is>
       </c>
     </row>
@@ -1501,6 +1715,8 @@
       <c r="E36" t="inlineStr"/>
       <c r="F36" s="4" t="inlineStr"/>
       <c r="G36" t="inlineStr"/>
+      <c r="H36" s="4" t="inlineStr"/>
+      <c r="I36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -1527,9 +1743,15 @@
       <c r="F37" s="3" t="n">
         <v>35</v>
       </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>6198</t>
+      <c r="G37" t="n">
+        <v>6198</v>
+      </c>
+      <c r="H37" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>2956</t>
         </is>
       </c>
     </row>
@@ -1558,9 +1780,15 @@
       <c r="F38" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>5695</t>
+      <c r="G38" t="n">
+        <v>5695</v>
+      </c>
+      <c r="H38" s="3" t="n">
+        <v>35</v>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>2874</t>
         </is>
       </c>
     </row>
@@ -1589,9 +1817,15 @@
       <c r="F39" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>7164</t>
+      <c r="G39" t="n">
+        <v>7164</v>
+      </c>
+      <c r="H39" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>2973</t>
         </is>
       </c>
     </row>
@@ -1620,9 +1854,15 @@
       <c r="F40" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>6157</t>
+      <c r="G40" t="n">
+        <v>6157</v>
+      </c>
+      <c r="H40" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>2850</t>
         </is>
       </c>
     </row>
@@ -1651,9 +1891,15 @@
       <c r="F41" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>7138</t>
+      <c r="G41" t="n">
+        <v>7138</v>
+      </c>
+      <c r="H41" s="3" t="n">
+        <v>35</v>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>2993</t>
         </is>
       </c>
     </row>
@@ -1676,15 +1922,21 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F42" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>6021</t>
+      <c r="G42" t="n">
+        <v>6021</v>
+      </c>
+      <c r="H42" s="3" t="n">
+        <v>33</v>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>2946</t>
         </is>
       </c>
     </row>
@@ -1713,9 +1965,15 @@
       <c r="F43" s="3" t="n">
         <v>39</v>
       </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>3205</t>
+      <c r="G43" t="n">
+        <v>3205</v>
+      </c>
+      <c r="H43" s="3" t="n">
+        <v>33</v>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>2552</t>
         </is>
       </c>
     </row>
@@ -1738,15 +1996,21 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F44" s="4" t="n">
         <v>28</v>
       </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>5813</t>
+      <c r="G44" t="n">
+        <v>5813</v>
+      </c>
+      <c r="H44" s="3" t="n">
+        <v>34</v>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>2750</t>
         </is>
       </c>
     </row>
@@ -1775,9 +2039,15 @@
       <c r="F45" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>6207</t>
+      <c r="G45" t="n">
+        <v>6207</v>
+      </c>
+      <c r="H45" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>2798</t>
         </is>
       </c>
     </row>
@@ -1806,9 +2076,15 @@
       <c r="F46" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>5351</t>
+      <c r="G46" t="n">
+        <v>5351</v>
+      </c>
+      <c r="H46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1837,9 +2113,15 @@
       <c r="F47" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>6366</t>
+      <c r="G47" t="n">
+        <v>6366</v>
+      </c>
+      <c r="H47" s="3" t="n">
+        <v>36</v>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>3063</t>
         </is>
       </c>
     </row>
@@ -1868,9 +2150,15 @@
       <c r="F48" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>6152</t>
+      <c r="G48" t="n">
+        <v>6152</v>
+      </c>
+      <c r="H48" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>2987</t>
         </is>
       </c>
     </row>
@@ -1899,9 +2187,15 @@
       <c r="F49" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>6046</t>
+      <c r="G49" t="n">
+        <v>6046</v>
+      </c>
+      <c r="H49" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>2795</t>
         </is>
       </c>
     </row>
@@ -1925,6 +2219,8 @@
       <c r="E50" t="inlineStr"/>
       <c r="F50" s="4" t="inlineStr"/>
       <c r="G50" t="inlineStr"/>
+      <c r="H50" s="4" t="inlineStr"/>
+      <c r="I50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -1951,11 +2247,11 @@
       <c r="F51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>1997</t>
-        </is>
-      </c>
+      <c r="G51" t="n">
+        <v>1997</v>
+      </c>
+      <c r="H51" s="4" t="inlineStr"/>
+      <c r="I51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -1982,9 +2278,15 @@
       <c r="F52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G52" t="n">
+        <v>0</v>
+      </c>
+      <c r="H52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>2485</t>
         </is>
       </c>
     </row>
@@ -2013,9 +2315,15 @@
       <c r="F53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>3380</t>
+      <c r="G53" t="n">
+        <v>3380</v>
+      </c>
+      <c r="H53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2044,9 +2352,15 @@
       <c r="F54" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>4150</t>
+      <c r="G54" t="n">
+        <v>4150</v>
+      </c>
+      <c r="H54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>2511</t>
         </is>
       </c>
     </row>
@@ -2075,9 +2389,15 @@
       <c r="F55" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>5784</t>
+      <c r="G55" t="n">
+        <v>5784</v>
+      </c>
+      <c r="H55" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>2890</t>
         </is>
       </c>
     </row>
@@ -2106,9 +2426,15 @@
       <c r="F56" s="3" t="n">
         <v>34</v>
       </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>4567</t>
+      <c r="G56" t="n">
+        <v>4567</v>
+      </c>
+      <c r="H56" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>2761</t>
         </is>
       </c>
     </row>
@@ -2137,9 +2463,15 @@
       <c r="F57" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>4640</t>
+      <c r="G57" t="n">
+        <v>4640</v>
+      </c>
+      <c r="H57" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>2722</t>
         </is>
       </c>
     </row>
@@ -2168,9 +2500,15 @@
       <c r="F58" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>5366</t>
+      <c r="G58" t="n">
+        <v>5366</v>
+      </c>
+      <c r="H58" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>2767</t>
         </is>
       </c>
     </row>
@@ -2199,9 +2537,15 @@
       <c r="F59" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>4781</t>
+      <c r="G59" t="n">
+        <v>4781</v>
+      </c>
+      <c r="H59" s="3" t="n">
+        <v>33</v>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>2757</t>
         </is>
       </c>
     </row>
@@ -2230,9 +2574,15 @@
       <c r="F60" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>5311</t>
+      <c r="G60" t="n">
+        <v>5311</v>
+      </c>
+      <c r="H60" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>2806</t>
         </is>
       </c>
     </row>
@@ -2261,9 +2611,15 @@
       <c r="F61" s="4" t="n">
         <v>26</v>
       </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>5735</t>
+      <c r="G61" t="n">
+        <v>5735</v>
+      </c>
+      <c r="H61" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>2750</t>
         </is>
       </c>
     </row>
@@ -2292,9 +2648,15 @@
       <c r="F62" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>5722</t>
+      <c r="G62" t="n">
+        <v>5722</v>
+      </c>
+      <c r="H62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>2494</t>
         </is>
       </c>
     </row>
@@ -2323,9 +2685,15 @@
       <c r="F63" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G63" t="n">
+        <v>0</v>
+      </c>
+      <c r="H63" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>2605</t>
         </is>
       </c>
     </row>
@@ -2354,9 +2722,15 @@
       <c r="F64" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>3481</t>
+      <c r="G64" t="n">
+        <v>3481</v>
+      </c>
+      <c r="H64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2385,9 +2759,15 @@
       <c r="F65" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>5316</t>
+      <c r="G65" t="n">
+        <v>5316</v>
+      </c>
+      <c r="H65" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>2724</t>
         </is>
       </c>
     </row>
@@ -2416,9 +2796,15 @@
       <c r="F66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>4787</t>
+      <c r="G66" t="n">
+        <v>4787</v>
+      </c>
+      <c r="H66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2447,9 +2833,15 @@
       <c r="F67" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>5795</t>
+      <c r="G67" t="n">
+        <v>5795</v>
+      </c>
+      <c r="H67" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>2875</t>
         </is>
       </c>
     </row>
@@ -2478,9 +2870,15 @@
       <c r="F68" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>4666</t>
+      <c r="G68" t="n">
+        <v>4666</v>
+      </c>
+      <c r="H68" s="3" t="n">
+        <v>36</v>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>2797</t>
         </is>
       </c>
     </row>
@@ -2509,9 +2907,15 @@
       <c r="F69" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>4553</t>
+      <c r="G69" t="n">
+        <v>4553</v>
+      </c>
+      <c r="H69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2540,9 +2944,15 @@
       <c r="F70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>4475</t>
+      <c r="G70" t="n">
+        <v>4475</v>
+      </c>
+      <c r="H70" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>2722</t>
         </is>
       </c>
     </row>
@@ -2571,9 +2981,15 @@
       <c r="F71" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>4311</t>
+      <c r="G71" t="n">
+        <v>4311</v>
+      </c>
+      <c r="H71" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>2804</t>
         </is>
       </c>
     </row>
@@ -2583,7 +2999,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>"心灵有为 1"</t>
+          <t>心灵有为</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2602,9 +3018,15 @@
       <c r="F72" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>6001</t>
+      <c r="G72" t="n">
+        <v>6001</v>
+      </c>
+      <c r="H72" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>3070</t>
         </is>
       </c>
     </row>
@@ -2633,9 +3055,15 @@
       <c r="F73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>4628</t>
+      <c r="G73" t="n">
+        <v>4628</v>
+      </c>
+      <c r="H73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>2478</t>
         </is>
       </c>
     </row>
@@ -2664,9 +3092,15 @@
       <c r="F74" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>4508</t>
+      <c r="G74" t="n">
+        <v>4508</v>
+      </c>
+      <c r="H74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>2496</t>
         </is>
       </c>
     </row>
@@ -2695,9 +3129,15 @@
       <c r="F75" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>3959</t>
+      <c r="G75" t="n">
+        <v>3959</v>
+      </c>
+      <c r="H75" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>2610</t>
         </is>
       </c>
     </row>
@@ -2726,9 +3166,15 @@
       <c r="F76" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="G76" t="inlineStr">
-        <is>
-          <t>5084</t>
+      <c r="G76" t="n">
+        <v>5084</v>
+      </c>
+      <c r="H76" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>2789</t>
         </is>
       </c>
     </row>
@@ -2757,9 +3203,15 @@
       <c r="F77" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>5763</t>
+      <c r="G77" t="n">
+        <v>5763</v>
+      </c>
+      <c r="H77" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>2870</t>
         </is>
       </c>
     </row>
@@ -2788,9 +3240,15 @@
       <c r="F78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G78" t="inlineStr">
-        <is>
-          <t>3648</t>
+      <c r="G78" t="n">
+        <v>3648</v>
+      </c>
+      <c r="H78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2819,9 +3277,15 @@
       <c r="F79" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>5392</t>
+      <c r="G79" t="n">
+        <v>5392</v>
+      </c>
+      <c r="H79" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>2945</t>
         </is>
       </c>
     </row>
@@ -2850,9 +3314,15 @@
       <c r="F80" s="3" t="n">
         <v>32</v>
       </c>
-      <c r="G80" t="inlineStr">
-        <is>
-          <t>4545</t>
+      <c r="G80" t="n">
+        <v>4545</v>
+      </c>
+      <c r="H80" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>2673</t>
         </is>
       </c>
     </row>
@@ -2881,9 +3351,15 @@
       <c r="F81" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>5042</t>
+      <c r="G81" t="n">
+        <v>5042</v>
+      </c>
+      <c r="H81" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>2846</t>
         </is>
       </c>
     </row>
@@ -2912,9 +3388,15 @@
       <c r="F82" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>5240</t>
+      <c r="G82" t="n">
+        <v>5240</v>
+      </c>
+      <c r="H82" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>2992</t>
         </is>
       </c>
     </row>
@@ -2943,9 +3425,15 @@
       <c r="F83" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>4926</t>
+      <c r="G83" t="n">
+        <v>4926</v>
+      </c>
+      <c r="H83" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>2887</t>
         </is>
       </c>
     </row>
@@ -2974,9 +3462,15 @@
       <c r="F84" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>4938</t>
+      <c r="G84" t="n">
+        <v>4938</v>
+      </c>
+      <c r="H84" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>2876</t>
         </is>
       </c>
     </row>
@@ -3005,9 +3499,15 @@
       <c r="F85" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>4781</t>
+      <c r="G85" t="n">
+        <v>4781</v>
+      </c>
+      <c r="H85" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>2768</t>
         </is>
       </c>
     </row>
@@ -3036,9 +3536,15 @@
       <c r="F86" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>3987</t>
+      <c r="G86" t="n">
+        <v>3987</v>
+      </c>
+      <c r="H86" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>2657</t>
         </is>
       </c>
     </row>
@@ -3067,9 +3573,15 @@
       <c r="F87" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="G87" t="inlineStr">
-        <is>
-          <t>3873</t>
+      <c r="G87" t="n">
+        <v>3873</v>
+      </c>
+      <c r="H87" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>2550</t>
         </is>
       </c>
     </row>
@@ -3098,9 +3610,15 @@
       <c r="F88" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G88" t="inlineStr">
-        <is>
-          <t>5219</t>
+      <c r="G88" t="n">
+        <v>5219</v>
+      </c>
+      <c r="H88" s="3" t="n">
+        <v>33</v>
+      </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>2981</t>
         </is>
       </c>
     </row>
@@ -3129,9 +3647,15 @@
       <c r="F89" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t>3096</t>
+      <c r="G89" t="n">
+        <v>3096</v>
+      </c>
+      <c r="H89" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>2566</t>
         </is>
       </c>
     </row>
@@ -3160,9 +3684,15 @@
       <c r="F90" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>3545</t>
+      <c r="G90" t="n">
+        <v>3545</v>
+      </c>
+      <c r="H90" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>2677</t>
         </is>
       </c>
     </row>
@@ -3191,9 +3721,15 @@
       <c r="F91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>2121</t>
+      <c r="G91" t="n">
+        <v>2121</v>
+      </c>
+      <c r="H91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>2018</t>
         </is>
       </c>
     </row>
@@ -3222,9 +3758,15 @@
       <c r="F92" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>2845</t>
+      <c r="G92" t="n">
+        <v>2845</v>
+      </c>
+      <c r="H92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>2428</t>
         </is>
       </c>
     </row>
@@ -3253,9 +3795,15 @@
       <c r="F93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>3228</t>
+      <c r="G93" t="n">
+        <v>3228</v>
+      </c>
+      <c r="H93" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>2470</t>
         </is>
       </c>
     </row>
@@ -3284,9 +3832,15 @@
       <c r="F94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G94" t="inlineStr">
-        <is>
-          <t>2459</t>
+      <c r="G94" t="n">
+        <v>2459</v>
+      </c>
+      <c r="H94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3315,9 +3869,15 @@
       <c r="F95" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>6055</t>
+      <c r="G95" t="n">
+        <v>6055</v>
+      </c>
+      <c r="H95" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>2945</t>
         </is>
       </c>
     </row>
@@ -3346,9 +3906,15 @@
       <c r="F96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>2681</t>
+      <c r="G96" t="n">
+        <v>2681</v>
+      </c>
+      <c r="H96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3377,9 +3943,15 @@
       <c r="F97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>3383</t>
+      <c r="G97" t="n">
+        <v>3383</v>
+      </c>
+      <c r="H97" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>2514</t>
         </is>
       </c>
     </row>
@@ -3408,9 +3980,15 @@
       <c r="F98" s="4" t="n">
         <v>26</v>
       </c>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>3616</t>
+      <c r="G98" t="n">
+        <v>3616</v>
+      </c>
+      <c r="H98" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>2533</t>
         </is>
       </c>
     </row>
@@ -3439,9 +4017,15 @@
       <c r="F99" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="G99" t="inlineStr">
-        <is>
-          <t>4614</t>
+      <c r="G99" t="n">
+        <v>4614</v>
+      </c>
+      <c r="H99" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>2795</t>
         </is>
       </c>
     </row>
@@ -3470,9 +4054,15 @@
       <c r="F100" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G100" t="inlineStr">
-        <is>
-          <t>4197</t>
+      <c r="G100" t="n">
+        <v>4197</v>
+      </c>
+      <c r="H100" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>2638</t>
         </is>
       </c>
     </row>
@@ -3501,9 +4091,15 @@
       <c r="F101" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="G101" t="inlineStr">
-        <is>
-          <t>4006</t>
+      <c r="G101" t="n">
+        <v>4006</v>
+      </c>
+      <c r="H101" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>2575</t>
         </is>
       </c>
     </row>
@@ -3532,9 +4128,15 @@
       <c r="F102" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="G102" t="inlineStr">
-        <is>
-          <t>4671</t>
+      <c r="G102" t="n">
+        <v>4671</v>
+      </c>
+      <c r="H102" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>2769</t>
         </is>
       </c>
     </row>
@@ -3563,9 +4165,15 @@
       <c r="F103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G103" t="inlineStr">
-        <is>
-          <t>4038</t>
+      <c r="G103" t="n">
+        <v>4038</v>
+      </c>
+      <c r="H103" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>2680</t>
         </is>
       </c>
     </row>
@@ -3594,9 +4202,15 @@
       <c r="F104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G104" t="inlineStr">
-        <is>
-          <t>3011</t>
+      <c r="G104" t="n">
+        <v>3011</v>
+      </c>
+      <c r="H104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3625,9 +4239,15 @@
       <c r="F105" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G105" t="inlineStr">
-        <is>
-          <t>5710</t>
+      <c r="G105" t="n">
+        <v>5710</v>
+      </c>
+      <c r="H105" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>2765</t>
         </is>
       </c>
     </row>
@@ -3656,9 +4276,15 @@
       <c r="F106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G106" t="inlineStr">
-        <is>
-          <t>4124</t>
+      <c r="G106" t="n">
+        <v>4124</v>
+      </c>
+      <c r="H106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3687,9 +4313,15 @@
       <c r="F107" s="4" t="n">
         <v>26</v>
       </c>
-      <c r="G107" t="inlineStr">
-        <is>
-          <t>3670</t>
+      <c r="G107" t="n">
+        <v>3670</v>
+      </c>
+      <c r="H107" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>2569</t>
         </is>
       </c>
     </row>
@@ -3718,9 +4350,15 @@
       <c r="F108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G108" t="inlineStr">
-        <is>
-          <t>2865</t>
+      <c r="G108" t="n">
+        <v>2865</v>
+      </c>
+      <c r="H108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>2519</t>
         </is>
       </c>
     </row>
@@ -3749,9 +4387,15 @@
       <c r="F109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G109" t="inlineStr">
-        <is>
-          <t>4064</t>
+      <c r="G109" t="n">
+        <v>4064</v>
+      </c>
+      <c r="H109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>2502</t>
         </is>
       </c>
     </row>
@@ -3780,9 +4424,15 @@
       <c r="F110" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G110" t="inlineStr">
-        <is>
-          <t>3693</t>
+      <c r="G110" t="n">
+        <v>3693</v>
+      </c>
+      <c r="H110" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>2609</t>
         </is>
       </c>
     </row>
@@ -3811,9 +4461,15 @@
       <c r="F111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G111" t="inlineStr">
-        <is>
-          <t>3998</t>
+      <c r="G111" t="n">
+        <v>3998</v>
+      </c>
+      <c r="H111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>2574</t>
         </is>
       </c>
     </row>
@@ -3842,9 +4498,15 @@
       <c r="F112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G112" t="inlineStr">
-        <is>
-          <t>3825</t>
+      <c r="G112" t="n">
+        <v>3825</v>
+      </c>
+      <c r="H112" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>2772</t>
         </is>
       </c>
     </row>
@@ -3873,9 +4535,15 @@
       <c r="F113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G113" t="inlineStr">
-        <is>
-          <t>2800</t>
+      <c r="G113" t="n">
+        <v>2800</v>
+      </c>
+      <c r="H113" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>2493</t>
         </is>
       </c>
     </row>
@@ -3904,9 +4572,15 @@
       <c r="F114" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="G114" t="inlineStr">
-        <is>
-          <t>2953</t>
+      <c r="G114" t="n">
+        <v>2953</v>
+      </c>
+      <c r="H114" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>2432</t>
         </is>
       </c>
     </row>
@@ -3935,9 +4609,15 @@
       <c r="F115" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="G115" t="inlineStr">
-        <is>
-          <t>3810</t>
+      <c r="G115" t="n">
+        <v>3810</v>
+      </c>
+      <c r="H115" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>2598</t>
         </is>
       </c>
     </row>
@@ -3966,9 +4646,15 @@
       <c r="F116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G116" t="inlineStr">
-        <is>
-          <t>3325</t>
+      <c r="G116" t="n">
+        <v>3325</v>
+      </c>
+      <c r="H116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3997,9 +4683,15 @@
       <c r="F117" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G117" t="inlineStr">
-        <is>
-          <t>3776</t>
+      <c r="G117" t="n">
+        <v>3776</v>
+      </c>
+      <c r="H117" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>2621</t>
         </is>
       </c>
     </row>
@@ -4028,9 +4720,15 @@
       <c r="F118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G118" t="inlineStr">
-        <is>
-          <t>3014</t>
+      <c r="G118" t="n">
+        <v>3014</v>
+      </c>
+      <c r="H118" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>2413</t>
         </is>
       </c>
     </row>
@@ -4059,9 +4757,15 @@
       <c r="F119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G119" t="inlineStr">
-        <is>
-          <t>3836</t>
+      <c r="G119" t="n">
+        <v>3836</v>
+      </c>
+      <c r="H119" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>2767</t>
         </is>
       </c>
     </row>
@@ -4090,9 +4794,15 @@
       <c r="F120" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G120" t="inlineStr">
-        <is>
-          <t>2823</t>
+      <c r="G120" t="n">
+        <v>2823</v>
+      </c>
+      <c r="H120" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>2496</t>
         </is>
       </c>
     </row>
@@ -4121,9 +4831,15 @@
       <c r="F121" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G121" t="inlineStr">
-        <is>
-          <t>3446</t>
+      <c r="G121" t="n">
+        <v>3446</v>
+      </c>
+      <c r="H121" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>2539</t>
         </is>
       </c>
     </row>
@@ -4152,9 +4868,15 @@
       <c r="F122" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G122" t="inlineStr">
-        <is>
-          <t>3386</t>
+      <c r="G122" t="n">
+        <v>3386</v>
+      </c>
+      <c r="H122" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I122" t="inlineStr">
+        <is>
+          <t>2539</t>
         </is>
       </c>
     </row>
@@ -4183,9 +4905,15 @@
       <c r="F123" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G123" t="inlineStr">
-        <is>
-          <t>3923</t>
+      <c r="G123" t="n">
+        <v>3923</v>
+      </c>
+      <c r="H123" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>2720</t>
         </is>
       </c>
     </row>
@@ -4214,9 +4942,15 @@
       <c r="F124" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G124" t="inlineStr">
-        <is>
-          <t>3444</t>
+      <c r="G124" t="n">
+        <v>3444</v>
+      </c>
+      <c r="H124" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>2617</t>
         </is>
       </c>
     </row>
@@ -4245,9 +4979,15 @@
       <c r="F125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G125" t="inlineStr">
-        <is>
-          <t>2247</t>
+      <c r="G125" t="n">
+        <v>2247</v>
+      </c>
+      <c r="H125" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="I125" t="inlineStr">
+        <is>
+          <t>2186</t>
         </is>
       </c>
     </row>
@@ -4276,9 +5016,15 @@
       <c r="F126" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="G126" t="inlineStr">
-        <is>
-          <t>2741</t>
+      <c r="G126" t="n">
+        <v>2741</v>
+      </c>
+      <c r="H126" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="I126" t="inlineStr">
+        <is>
+          <t>2457</t>
         </is>
       </c>
     </row>
@@ -4288,7 +5034,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Player-58340439</t>
+          <t>70qilin</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -4307,9 +5053,15 @@
       <c r="F127" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="G127" t="inlineStr">
-        <is>
-          <t>2637</t>
+      <c r="G127" t="n">
+        <v>2637</v>
+      </c>
+      <c r="H127" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I127" t="inlineStr">
+        <is>
+          <t>2480</t>
         </is>
       </c>
     </row>
@@ -4332,15 +5084,21 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F128" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="G128" t="inlineStr">
-        <is>
-          <t>6015</t>
+      <c r="G128" t="n">
+        <v>6015</v>
+      </c>
+      <c r="H128" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I128" t="inlineStr">
+        <is>
+          <t>2818</t>
         </is>
       </c>
     </row>
@@ -4369,9 +5127,15 @@
       <c r="F129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G129" t="inlineStr">
-        <is>
-          <t>2534</t>
+      <c r="G129" t="n">
+        <v>2534</v>
+      </c>
+      <c r="H129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I129" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4400,9 +5164,15 @@
       <c r="F130" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G130" t="inlineStr">
-        <is>
-          <t>2820</t>
+      <c r="G130" t="n">
+        <v>2820</v>
+      </c>
+      <c r="H130" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="I130" t="inlineStr">
+        <is>
+          <t>2498</t>
         </is>
       </c>
     </row>
@@ -4431,9 +5201,15 @@
       <c r="F131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G131" t="inlineStr">
-        <is>
-          <t>2657</t>
+      <c r="G131" t="n">
+        <v>2657</v>
+      </c>
+      <c r="H131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I131" t="inlineStr">
+        <is>
+          <t>2485</t>
         </is>
       </c>
     </row>
@@ -4462,9 +5238,15 @@
       <c r="F132" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G132" t="inlineStr">
-        <is>
-          <t>3966</t>
+      <c r="G132" t="n">
+        <v>3966</v>
+      </c>
+      <c r="H132" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I132" t="inlineStr">
+        <is>
+          <t>2527</t>
         </is>
       </c>
     </row>
@@ -4493,7 +5275,13 @@
       <c r="F133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G133" t="inlineStr">
+      <c r="G133" t="n">
+        <v>0</v>
+      </c>
+      <c r="H133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I133" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4524,9 +5312,15 @@
       <c r="F134" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G134" t="inlineStr">
-        <is>
-          <t>3040</t>
+      <c r="G134" t="n">
+        <v>3040</v>
+      </c>
+      <c r="H134" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I134" t="inlineStr">
+        <is>
+          <t>2521</t>
         </is>
       </c>
     </row>
@@ -4555,9 +5349,15 @@
       <c r="F135" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G135" t="inlineStr">
-        <is>
-          <t>2901</t>
+      <c r="G135" t="n">
+        <v>2901</v>
+      </c>
+      <c r="H135" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I135" t="inlineStr">
+        <is>
+          <t>2473</t>
         </is>
       </c>
     </row>
@@ -4586,9 +5386,15 @@
       <c r="F136" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="G136" t="inlineStr">
-        <is>
-          <t>2711</t>
+      <c r="G136" t="n">
+        <v>2711</v>
+      </c>
+      <c r="H136" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="I136" t="inlineStr">
+        <is>
+          <t>2497</t>
         </is>
       </c>
     </row>
@@ -4617,9 +5423,15 @@
       <c r="F137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G137" t="inlineStr">
-        <is>
-          <t>2492</t>
+      <c r="G137" t="n">
+        <v>2492</v>
+      </c>
+      <c r="H137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I137" t="inlineStr">
+        <is>
+          <t>1988</t>
         </is>
       </c>
     </row>
@@ -4648,7 +5460,13 @@
       <c r="F138" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G138" t="inlineStr">
+      <c r="G138" t="n">
+        <v>0</v>
+      </c>
+      <c r="H138" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I138" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4679,7 +5497,13 @@
       <c r="F139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G139" t="inlineStr">
+      <c r="G139" t="n">
+        <v>0</v>
+      </c>
+      <c r="H139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I139" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4710,7 +5534,13 @@
       <c r="F140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G140" t="inlineStr">
+      <c r="G140" t="n">
+        <v>0</v>
+      </c>
+      <c r="H140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I140" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4741,9 +5571,15 @@
       <c r="F141" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="G141" t="inlineStr">
-        <is>
-          <t>2164</t>
+      <c r="G141" t="n">
+        <v>2164</v>
+      </c>
+      <c r="H141" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I141" t="inlineStr">
+        <is>
+          <t>2000</t>
         </is>
       </c>
     </row>
@@ -4772,9 +5608,15 @@
       <c r="F142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G142" t="inlineStr">
-        <is>
-          <t>2190</t>
+      <c r="G142" t="n">
+        <v>2190</v>
+      </c>
+      <c r="H142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I142" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4803,7 +5645,13 @@
       <c r="F143" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G143" t="inlineStr">
+      <c r="G143" t="n">
+        <v>0</v>
+      </c>
+      <c r="H143" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I143" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4834,7 +5682,13 @@
       <c r="F144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G144" t="inlineStr">
+      <c r="G144" t="n">
+        <v>0</v>
+      </c>
+      <c r="H144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I144" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4865,7 +5719,13 @@
       <c r="F145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G145" t="inlineStr">
+      <c r="G145" t="n">
+        <v>0</v>
+      </c>
+      <c r="H145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I145" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4896,9 +5756,15 @@
       <c r="F146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G146" t="inlineStr">
-        <is>
-          <t>1648</t>
+      <c r="G146" t="n">
+        <v>1648</v>
+      </c>
+      <c r="H146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I146" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4927,7 +5793,13 @@
       <c r="F147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G147" t="inlineStr">
+      <c r="G147" t="n">
+        <v>0</v>
+      </c>
+      <c r="H147" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I147" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4958,7 +5830,13 @@
       <c r="F148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G148" t="inlineStr">
+      <c r="G148" t="n">
+        <v>0</v>
+      </c>
+      <c r="H148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4989,7 +5867,13 @@
       <c r="F149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G149" t="inlineStr">
+      <c r="G149" t="n">
+        <v>0</v>
+      </c>
+      <c r="H149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I149" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5020,9 +5904,15 @@
       <c r="F150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G150" t="inlineStr">
-        <is>
-          <t>1639</t>
+      <c r="G150" t="n">
+        <v>1639</v>
+      </c>
+      <c r="H150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I150" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -5051,7 +5941,13 @@
       <c r="F151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G151" t="inlineStr">
+      <c r="G151" t="n">
+        <v>0</v>
+      </c>
+      <c r="H151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I151" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5082,7 +5978,13 @@
       <c r="F152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G152" t="inlineStr">
+      <c r="G152" t="n">
+        <v>0</v>
+      </c>
+      <c r="H152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5113,9 +6015,15 @@
       <c r="F153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G153" t="inlineStr">
-        <is>
-          <t>1781</t>
+      <c r="G153" t="n">
+        <v>1781</v>
+      </c>
+      <c r="H153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I153" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -5144,9 +6052,15 @@
       <c r="F154" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="G154" t="inlineStr">
-        <is>
-          <t>1346</t>
+      <c r="G154" t="n">
+        <v>1346</v>
+      </c>
+      <c r="H154" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="I154" t="inlineStr">
+        <is>
+          <t>1460</t>
         </is>
       </c>
     </row>
@@ -5175,9 +6089,15 @@
       <c r="F155" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G155" t="inlineStr">
-        <is>
-          <t>1198</t>
+      <c r="G155" t="n">
+        <v>1198</v>
+      </c>
+      <c r="H155" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="I155" t="inlineStr">
+        <is>
+          <t>1412</t>
         </is>
       </c>
     </row>
@@ -5206,9 +6126,15 @@
       <c r="F156" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="G156" t="inlineStr">
-        <is>
-          <t>5347</t>
+      <c r="G156" t="n">
+        <v>5347</v>
+      </c>
+      <c r="H156" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I156" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -5237,7 +6163,13 @@
       <c r="F157" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G157" t="inlineStr">
+      <c r="G157" t="n">
+        <v>0</v>
+      </c>
+      <c r="H157" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I157" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5268,7 +6200,13 @@
       <c r="F158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G158" t="inlineStr">
+      <c r="G158" t="n">
+        <v>0</v>
+      </c>
+      <c r="H158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5299,9 +6237,15 @@
       <c r="F159" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="G159" t="inlineStr">
-        <is>
-          <t>6220</t>
+      <c r="G159" t="n">
+        <v>6220</v>
+      </c>
+      <c r="H159" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="I159" t="inlineStr">
+        <is>
+          <t>2782</t>
         </is>
       </c>
     </row>
@@ -5330,7 +6274,13 @@
       <c r="F160" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G160" t="inlineStr">
+      <c r="G160" t="n">
+        <v>0</v>
+      </c>
+      <c r="H160" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I160" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5361,9 +6311,15 @@
       <c r="F161" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G161" t="inlineStr">
-        <is>
-          <t>2853</t>
+      <c r="G161" t="n">
+        <v>2853</v>
+      </c>
+      <c r="H161" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I161" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -5392,7 +6348,13 @@
       <c r="F162" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G162" t="inlineStr">
+      <c r="G162" t="n">
+        <v>0</v>
+      </c>
+      <c r="H162" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I162" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5423,17 +6385,21 @@
       <c r="F163" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G163" t="inlineStr">
-        <is>
-          <t>3065</t>
+      <c r="G163" t="n">
+        <v>3065</v>
+      </c>
+      <c r="H163" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I163" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="164">
-      <c r="A164" t="inlineStr">
-        <is>
-          <t>47928278</t>
-        </is>
+      <c r="A164" t="n">
+        <v>47928278</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
@@ -5450,9 +6416,102 @@
       <c r="F164" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="G164" t="inlineStr">
-        <is>
-          <t>7458</t>
+      <c r="G164" t="n">
+        <v>7458</v>
+      </c>
+      <c r="H164" s="3" t="n">
+        <v>37</v>
+      </c>
+      <c r="I164" t="inlineStr">
+        <is>
+          <t>2873</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>23526770</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>"Rauan - ALA"</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr"/>
+      <c r="D165" t="inlineStr"/>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F165" s="4" t="inlineStr"/>
+      <c r="G165" t="inlineStr"/>
+      <c r="H165" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="I165" t="inlineStr">
+        <is>
+          <t>2549</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>28122155</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>晨-----</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr"/>
+      <c r="D166" t="inlineStr"/>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F166" s="4" t="inlineStr"/>
+      <c r="G166" t="inlineStr"/>
+      <c r="H166" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I166" t="inlineStr">
+        <is>
+          <t>2509</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>46415834</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>DroningCruise17</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr"/>
+      <c r="D167" t="inlineStr"/>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F167" s="4" t="inlineStr"/>
+      <c r="G167" t="inlineStr"/>
+      <c r="H167" s="3" t="n">
+        <v>33</v>
+      </c>
+      <c r="I167" t="inlineStr">
+        <is>
+          <t>2504</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-01-17 11:30:32
</commit_message>
<xml_diff>
--- a/Season_Attack/82.xlsx
+++ b/Season_Attack/82.xlsx
@@ -82,8 +82,8 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I167"/>
+  <dimension ref="A1:K167"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,6 +436,16 @@
           <t>01-15_0</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>01-16_A</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>01-16_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -468,9 +478,15 @@
       <c r="H2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>2504</t>
+      <c r="I2" t="n">
+        <v>2504</v>
+      </c>
+      <c r="J2" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>2781</t>
         </is>
       </c>
     </row>
@@ -496,18 +512,24 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F3" s="3" t="n">
+      <c r="F3" s="4" t="n">
         <v>34</v>
       </c>
       <c r="G3" t="n">
         <v>6101</v>
       </c>
-      <c r="H3" s="3" t="n">
+      <c r="H3" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>2840</t>
+      <c r="I3" t="n">
+        <v>2840</v>
+      </c>
+      <c r="J3" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>3195</t>
         </is>
       </c>
     </row>
@@ -530,10 +552,10 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F4" s="4" t="n">
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F4" s="3" t="n">
         <v>20</v>
       </c>
       <c r="G4" t="n">
@@ -542,9 +564,15 @@
       <c r="H4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>2920</t>
         </is>
       </c>
     </row>
@@ -576,10 +604,16 @@
       <c r="G5" t="n">
         <v>6330</v>
       </c>
-      <c r="H5" s="4" t="n">
+      <c r="H5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="I5" t="n">
+        <v>2820</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="inlineStr">
         <is>
           <t>2820</t>
         </is>
@@ -604,21 +638,27 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F6" s="3" t="n">
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F6" s="4" t="n">
         <v>32</v>
       </c>
       <c r="G6" t="n">
         <v>6320</v>
       </c>
-      <c r="H6" s="3" t="n">
+      <c r="H6" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>3013</t>
+      <c r="I6" t="n">
+        <v>3013</v>
+      </c>
+      <c r="J6" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>3380</t>
         </is>
       </c>
     </row>
@@ -641,21 +681,27 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F7" s="4" t="n">
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F7" s="3" t="n">
         <v>20</v>
       </c>
       <c r="G7" t="n">
         <v>5732</v>
       </c>
-      <c r="H7" s="4" t="n">
+      <c r="H7" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>2800</t>
+      <c r="I7" t="n">
+        <v>2800</v>
+      </c>
+      <c r="J7" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>3096</t>
         </is>
       </c>
     </row>
@@ -681,18 +727,24 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F8" s="3" t="n">
+      <c r="F8" s="4" t="n">
         <v>32</v>
       </c>
       <c r="G8" t="n">
         <v>6111</v>
       </c>
-      <c r="H8" s="4" t="n">
+      <c r="H8" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>2850</t>
+      <c r="I8" t="n">
+        <v>2850</v>
+      </c>
+      <c r="J8" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>3076</t>
         </is>
       </c>
     </row>
@@ -718,20 +770,20 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F9" s="4" t="n">
+      <c r="F9" s="3" t="n">
         <v>20</v>
       </c>
       <c r="G9" t="n">
         <v>3534</v>
       </c>
-      <c r="H9" s="4" t="n">
+      <c r="H9" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>2471</t>
-        </is>
-      </c>
+      <c r="I9" t="n">
+        <v>2471</v>
+      </c>
+      <c r="J9" s="3" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -752,21 +804,27 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F10" s="3" t="n">
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F10" s="4" t="n">
         <v>40</v>
       </c>
       <c r="G10" t="n">
         <v>5738</v>
       </c>
-      <c r="H10" s="3" t="n">
+      <c r="H10" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>2830</t>
+      <c r="I10" t="n">
+        <v>2830</v>
+      </c>
+      <c r="J10" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>3108</t>
         </is>
       </c>
     </row>
@@ -789,21 +847,27 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F11" s="3" t="n">
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F11" s="4" t="n">
         <v>33</v>
       </c>
       <c r="G11" t="n">
         <v>7186</v>
       </c>
-      <c r="H11" s="4" t="n">
+      <c r="H11" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>2902</t>
+      <c r="I11" t="n">
+        <v>2902</v>
+      </c>
+      <c r="J11" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>3179</t>
         </is>
       </c>
     </row>
@@ -826,21 +890,27 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F12" s="4" t="n">
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F12" s="3" t="n">
         <v>20</v>
       </c>
       <c r="G12" t="n">
         <v>6075</v>
       </c>
-      <c r="H12" s="4" t="n">
+      <c r="H12" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>2797</t>
+      <c r="I12" t="n">
+        <v>2797</v>
+      </c>
+      <c r="J12" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>3062</t>
         </is>
       </c>
     </row>
@@ -875,9 +945,15 @@
       <c r="H13" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>2552</t>
+      <c r="I13" t="n">
+        <v>2552</v>
+      </c>
+      <c r="J13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>2564</t>
         </is>
       </c>
     </row>
@@ -900,21 +976,27 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F14" s="3" t="n">
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F14" s="4" t="n">
         <v>38</v>
       </c>
       <c r="G14" t="n">
         <v>7281</v>
       </c>
-      <c r="H14" s="3" t="n">
+      <c r="H14" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>2953</t>
+      <c r="I14" t="n">
+        <v>2953</v>
+      </c>
+      <c r="J14" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>3362</t>
         </is>
       </c>
     </row>
@@ -937,21 +1019,27 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F15" s="4" t="n">
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F15" s="3" t="n">
         <v>25</v>
       </c>
       <c r="G15" t="n">
         <v>6108</v>
       </c>
-      <c r="H15" s="4" t="n">
+      <c r="H15" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>2852</t>
+      <c r="I15" t="n">
+        <v>2852</v>
+      </c>
+      <c r="J15" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>3210</t>
         </is>
       </c>
     </row>
@@ -974,21 +1062,27 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F16" s="3" t="n">
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F16" s="4" t="n">
         <v>40</v>
       </c>
       <c r="G16" t="n">
         <v>6840</v>
       </c>
-      <c r="H16" s="4" t="n">
+      <c r="H16" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>2945</t>
+      <c r="I16" t="n">
+        <v>2945</v>
+      </c>
+      <c r="J16" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>3379</t>
         </is>
       </c>
     </row>
@@ -1011,21 +1105,27 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F17" s="4" t="n">
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F17" s="3" t="n">
         <v>30</v>
       </c>
       <c r="G17" t="n">
         <v>5630</v>
       </c>
-      <c r="H17" s="4" t="n">
+      <c r="H17" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>2891</t>
+      <c r="I17" t="n">
+        <v>2891</v>
+      </c>
+      <c r="J17" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>3160</t>
         </is>
       </c>
     </row>
@@ -1051,7 +1151,7 @@
           <t>Chinese</t>
         </is>
       </c>
-      <c r="F18" s="4" t="n">
+      <c r="F18" s="3" t="n">
         <v>29</v>
       </c>
       <c r="G18" t="n">
@@ -1060,9 +1160,15 @@
       <c r="H18" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>2682</t>
         </is>
       </c>
     </row>
@@ -1085,21 +1191,27 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F19" s="3" t="n">
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F19" s="4" t="n">
         <v>40</v>
       </c>
       <c r="G19" t="n">
         <v>7137</v>
       </c>
-      <c r="H19" s="3" t="n">
+      <c r="H19" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>2968</t>
+      <c r="I19" t="n">
+        <v>2968</v>
+      </c>
+      <c r="J19" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>3445</t>
         </is>
       </c>
     </row>
@@ -1122,7 +1234,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="F20" s="5" t="n">
@@ -1131,10 +1243,16 @@
       <c r="G20" t="n">
         <v>5881</v>
       </c>
-      <c r="H20" s="4" t="n">
+      <c r="H20" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I20" t="inlineStr">
+      <c r="I20" t="n">
+        <v>2791</v>
+      </c>
+      <c r="J20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" t="inlineStr">
         <is>
           <t>2791</t>
         </is>
@@ -1162,18 +1280,24 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F21" s="3" t="n">
+      <c r="F21" s="4" t="n">
         <v>40</v>
       </c>
       <c r="G21" t="n">
         <v>6525</v>
       </c>
-      <c r="H21" s="3" t="n">
+      <c r="H21" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>3047</t>
+      <c r="I21" t="n">
+        <v>3047</v>
+      </c>
+      <c r="J21" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>3395</t>
         </is>
       </c>
     </row>
@@ -1196,7 +1320,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F22" s="5" t="n">
@@ -1205,12 +1329,18 @@
       <c r="G22" t="n">
         <v>6196</v>
       </c>
-      <c r="H22" s="3" t="n">
+      <c r="H22" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>2734</t>
+      <c r="I22" t="n">
+        <v>2734</v>
+      </c>
+      <c r="J22" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>2684</t>
         </is>
       </c>
     </row>
@@ -1233,21 +1363,27 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F23" s="4" t="n">
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F23" s="3" t="n">
         <v>30</v>
       </c>
       <c r="G23" t="n">
         <v>5834</v>
       </c>
-      <c r="H23" s="3" t="n">
+      <c r="H23" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>2971</t>
+      <c r="I23" t="n">
+        <v>2971</v>
+      </c>
+      <c r="J23" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>3129</t>
         </is>
       </c>
     </row>
@@ -1282,7 +1418,13 @@
       <c r="H24" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I24" t="inlineStr">
+      <c r="I24" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1307,21 +1449,27 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F25" s="3" t="n">
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F25" s="4" t="n">
         <v>40</v>
       </c>
       <c r="G25" t="n">
         <v>6268</v>
       </c>
-      <c r="H25" s="3" t="n">
+      <c r="H25" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>3057</t>
+      <c r="I25" t="n">
+        <v>3057</v>
+      </c>
+      <c r="J25" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>3405</t>
         </is>
       </c>
     </row>
@@ -1344,21 +1492,27 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F26" s="3" t="n">
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F26" s="4" t="n">
         <v>36</v>
       </c>
       <c r="G26" t="n">
         <v>6492</v>
       </c>
-      <c r="H26" s="3" t="n">
+      <c r="H26" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>3020</t>
+      <c r="I26" t="n">
+        <v>3020</v>
+      </c>
+      <c r="J26" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>3414</t>
         </is>
       </c>
     </row>
@@ -1384,18 +1538,24 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F27" s="4" t="n">
+      <c r="F27" s="3" t="n">
         <v>28</v>
       </c>
       <c r="G27" t="n">
         <v>6426</v>
       </c>
-      <c r="H27" s="4" t="n">
+      <c r="H27" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>2860</t>
+      <c r="I27" t="n">
+        <v>2860</v>
+      </c>
+      <c r="J27" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>2992</t>
         </is>
       </c>
     </row>
@@ -1421,18 +1581,24 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F28" s="3" t="n">
+      <c r="F28" s="4" t="n">
         <v>40</v>
       </c>
       <c r="G28" t="n">
         <v>6924</v>
       </c>
-      <c r="H28" s="3" t="n">
+      <c r="H28" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>3048</t>
+      <c r="I28" t="n">
+        <v>3048</v>
+      </c>
+      <c r="J28" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>3482</t>
         </is>
       </c>
     </row>
@@ -1455,7 +1621,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F29" s="5" t="n">
@@ -1464,12 +1630,18 @@
       <c r="G29" t="n">
         <v>6182</v>
       </c>
-      <c r="H29" s="4" t="n">
+      <c r="H29" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>2906</t>
+      <c r="I29" t="n">
+        <v>2906</v>
+      </c>
+      <c r="J29" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>3241</t>
         </is>
       </c>
     </row>
@@ -1495,18 +1667,24 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F30" s="3" t="n">
+      <c r="F30" s="4" t="n">
         <v>37</v>
       </c>
       <c r="G30" t="n">
         <v>6388</v>
       </c>
-      <c r="H30" s="3" t="n">
+      <c r="H30" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>2978</t>
+      <c r="I30" t="n">
+        <v>2978</v>
+      </c>
+      <c r="J30" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>3421</t>
         </is>
       </c>
     </row>
@@ -1529,21 +1707,27 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F31" s="4" t="n">
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F31" s="3" t="n">
         <v>30</v>
       </c>
       <c r="G31" t="n">
         <v>7167</v>
       </c>
-      <c r="H31" s="3" t="n">
+      <c r="H31" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>2855</t>
+      <c r="I31" t="n">
+        <v>2855</v>
+      </c>
+      <c r="J31" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>3317</t>
         </is>
       </c>
     </row>
@@ -1578,9 +1762,15 @@
       <c r="H32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>2509</t>
+      <c r="I32" t="n">
+        <v>2509</v>
+      </c>
+      <c r="J32" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>2550</t>
         </is>
       </c>
     </row>
@@ -1606,18 +1796,24 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F33" s="3" t="n">
+      <c r="F33" s="4" t="n">
         <v>33</v>
       </c>
       <c r="G33" t="n">
         <v>6623</v>
       </c>
-      <c r="H33" s="3" t="n">
+      <c r="H33" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>2963</t>
+      <c r="I33" t="n">
+        <v>2963</v>
+      </c>
+      <c r="J33" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>3240</t>
         </is>
       </c>
     </row>
@@ -1640,21 +1836,27 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F34" s="4" t="n">
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F34" s="3" t="n">
         <v>22</v>
       </c>
       <c r="G34" t="n">
         <v>5648</v>
       </c>
-      <c r="H34" s="4" t="n">
+      <c r="H34" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="I34" t="inlineStr">
-        <is>
-          <t>2755</t>
+      <c r="I34" t="n">
+        <v>2755</v>
+      </c>
+      <c r="J34" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>2904</t>
         </is>
       </c>
     </row>
@@ -1677,21 +1879,27 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F35" s="4" t="n">
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F35" s="3" t="n">
         <v>29</v>
       </c>
       <c r="G35" t="n">
         <v>5194</v>
       </c>
-      <c r="H35" s="3" t="n">
+      <c r="H35" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>2946</t>
+      <c r="I35" t="n">
+        <v>2946</v>
+      </c>
+      <c r="J35" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>3202</t>
         </is>
       </c>
     </row>
@@ -1713,10 +1921,12 @@
         <v>2915</v>
       </c>
       <c r="E36" t="inlineStr"/>
-      <c r="F36" s="4" t="inlineStr"/>
+      <c r="F36" s="3" t="inlineStr"/>
       <c r="G36" t="inlineStr"/>
-      <c r="H36" s="4" t="inlineStr"/>
+      <c r="H36" s="3" t="inlineStr"/>
       <c r="I36" t="inlineStr"/>
+      <c r="J36" s="3" t="inlineStr"/>
+      <c r="K36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -1737,21 +1947,27 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F37" s="3" t="n">
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F37" s="4" t="n">
         <v>35</v>
       </c>
       <c r="G37" t="n">
         <v>6198</v>
       </c>
-      <c r="H37" s="4" t="n">
+      <c r="H37" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>2956</t>
+      <c r="I37" t="n">
+        <v>2956</v>
+      </c>
+      <c r="J37" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>3258</t>
         </is>
       </c>
     </row>
@@ -1774,21 +1990,27 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F38" s="3" t="n">
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F38" s="4" t="n">
         <v>33</v>
       </c>
       <c r="G38" t="n">
         <v>5695</v>
       </c>
-      <c r="H38" s="3" t="n">
+      <c r="H38" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>2874</t>
+      <c r="I38" t="n">
+        <v>2874</v>
+      </c>
+      <c r="J38" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>3244</t>
         </is>
       </c>
     </row>
@@ -1811,21 +2033,27 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F39" s="4" t="n">
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F39" s="3" t="n">
         <v>30</v>
       </c>
       <c r="G39" t="n">
         <v>7164</v>
       </c>
-      <c r="H39" s="4" t="n">
+      <c r="H39" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>2973</t>
+      <c r="I39" t="n">
+        <v>2973</v>
+      </c>
+      <c r="J39" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>3420</t>
         </is>
       </c>
     </row>
@@ -1857,12 +2085,18 @@
       <c r="G40" t="n">
         <v>6157</v>
       </c>
-      <c r="H40" s="4" t="n">
+      <c r="H40" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>2850</t>
+      <c r="I40" t="n">
+        <v>2850</v>
+      </c>
+      <c r="J40" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>3056</t>
         </is>
       </c>
     </row>
@@ -1885,21 +2119,27 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F41" s="3" t="n">
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F41" s="4" t="n">
         <v>33</v>
       </c>
       <c r="G41" t="n">
         <v>7138</v>
       </c>
-      <c r="H41" s="3" t="n">
+      <c r="H41" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="I41" t="inlineStr">
-        <is>
-          <t>2993</t>
+      <c r="I41" t="n">
+        <v>2993</v>
+      </c>
+      <c r="J41" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>3358</t>
         </is>
       </c>
     </row>
@@ -1925,18 +2165,24 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F42" s="4" t="n">
+      <c r="F42" s="3" t="n">
         <v>27</v>
       </c>
       <c r="G42" t="n">
         <v>6021</v>
       </c>
-      <c r="H42" s="3" t="n">
+      <c r="H42" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>2946</t>
+      <c r="I42" t="n">
+        <v>2946</v>
+      </c>
+      <c r="J42" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>3351</t>
         </is>
       </c>
     </row>
@@ -1962,20 +2208,20 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F43" s="3" t="n">
+      <c r="F43" s="4" t="n">
         <v>39</v>
       </c>
       <c r="G43" t="n">
         <v>3205</v>
       </c>
-      <c r="H43" s="3" t="n">
+      <c r="H43" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>2552</t>
-        </is>
-      </c>
+      <c r="I43" t="n">
+        <v>2552</v>
+      </c>
+      <c r="J43" s="3" t="inlineStr"/>
+      <c r="K43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -1999,18 +2245,24 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F44" s="4" t="n">
+      <c r="F44" s="3" t="n">
         <v>28</v>
       </c>
       <c r="G44" t="n">
         <v>5813</v>
       </c>
-      <c r="H44" s="3" t="n">
+      <c r="H44" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>2750</t>
+      <c r="I44" t="n">
+        <v>2750</v>
+      </c>
+      <c r="J44" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>3068</t>
         </is>
       </c>
     </row>
@@ -2033,21 +2285,27 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F45" s="3" t="n">
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F45" s="4" t="n">
         <v>33</v>
       </c>
       <c r="G45" t="n">
         <v>6207</v>
       </c>
-      <c r="H45" s="4" t="n">
+      <c r="H45" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I45" t="inlineStr">
-        <is>
-          <t>2798</t>
+      <c r="I45" t="n">
+        <v>2798</v>
+      </c>
+      <c r="J45" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>3085</t>
         </is>
       </c>
     </row>
@@ -2073,7 +2331,7 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F46" s="4" t="n">
+      <c r="F46" s="3" t="n">
         <v>21</v>
       </c>
       <c r="G46" t="n">
@@ -2082,9 +2340,15 @@
       <c r="H46" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I46" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I46" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>2662</t>
         </is>
       </c>
     </row>
@@ -2107,21 +2371,27 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F47" s="3" t="n">
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F47" s="4" t="n">
         <v>40</v>
       </c>
       <c r="G47" t="n">
         <v>6366</v>
       </c>
-      <c r="H47" s="3" t="n">
+      <c r="H47" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="I47" t="inlineStr">
-        <is>
-          <t>3063</t>
+      <c r="I47" t="n">
+        <v>3063</v>
+      </c>
+      <c r="J47" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>3389</t>
         </is>
       </c>
     </row>
@@ -2144,21 +2414,27 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F48" s="4" t="n">
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F48" s="3" t="n">
         <v>30</v>
       </c>
       <c r="G48" t="n">
         <v>6152</v>
       </c>
-      <c r="H48" s="3" t="n">
+      <c r="H48" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>2987</t>
+      <c r="I48" t="n">
+        <v>2987</v>
+      </c>
+      <c r="J48" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>3340</t>
         </is>
       </c>
     </row>
@@ -2181,21 +2457,27 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F49" s="3" t="n">
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F49" s="4" t="n">
         <v>33</v>
       </c>
       <c r="G49" t="n">
         <v>6046</v>
       </c>
-      <c r="H49" s="4" t="n">
+      <c r="H49" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I49" t="inlineStr">
-        <is>
-          <t>2795</t>
+      <c r="I49" t="n">
+        <v>2795</v>
+      </c>
+      <c r="J49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>2792</t>
         </is>
       </c>
     </row>
@@ -2217,10 +2499,12 @@
         <v>4684</v>
       </c>
       <c r="E50" t="inlineStr"/>
-      <c r="F50" s="4" t="inlineStr"/>
+      <c r="F50" s="3" t="inlineStr"/>
       <c r="G50" t="inlineStr"/>
-      <c r="H50" s="4" t="inlineStr"/>
+      <c r="H50" s="3" t="inlineStr"/>
       <c r="I50" t="inlineStr"/>
+      <c r="J50" s="3" t="inlineStr"/>
+      <c r="K50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -2250,8 +2534,10 @@
       <c r="G51" t="n">
         <v>1997</v>
       </c>
-      <c r="H51" s="4" t="inlineStr"/>
+      <c r="H51" s="3" t="inlineStr"/>
       <c r="I51" t="inlineStr"/>
+      <c r="J51" s="3" t="inlineStr"/>
+      <c r="K51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -2284,9 +2570,15 @@
       <c r="H52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>2485</t>
+      <c r="I52" t="n">
+        <v>2485</v>
+      </c>
+      <c r="J52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>2502</t>
         </is>
       </c>
     </row>
@@ -2321,7 +2613,13 @@
       <c r="H53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I53" t="inlineStr">
+      <c r="I53" t="n">
+        <v>0</v>
+      </c>
+      <c r="J53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K53" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2358,9 +2656,15 @@
       <c r="H54" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I54" t="inlineStr">
-        <is>
-          <t>2511</t>
+      <c r="I54" t="n">
+        <v>2511</v>
+      </c>
+      <c r="J54" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>2693</t>
         </is>
       </c>
     </row>
@@ -2386,18 +2690,24 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F55" s="4" t="n">
+      <c r="F55" s="3" t="n">
         <v>25</v>
       </c>
       <c r="G55" t="n">
         <v>5784</v>
       </c>
-      <c r="H55" s="4" t="n">
+      <c r="H55" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="I55" t="inlineStr">
-        <is>
-          <t>2890</t>
+      <c r="I55" t="n">
+        <v>2890</v>
+      </c>
+      <c r="J55" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>3245</t>
         </is>
       </c>
     </row>
@@ -2423,18 +2733,24 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F56" s="3" t="n">
+      <c r="F56" s="4" t="n">
         <v>34</v>
       </c>
       <c r="G56" t="n">
         <v>4567</v>
       </c>
-      <c r="H56" s="3" t="n">
+      <c r="H56" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I56" t="inlineStr">
-        <is>
-          <t>2761</t>
+      <c r="I56" t="n">
+        <v>2761</v>
+      </c>
+      <c r="J56" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>2992</t>
         </is>
       </c>
     </row>
@@ -2460,18 +2776,24 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F57" s="4" t="n">
+      <c r="F57" s="3" t="n">
         <v>21</v>
       </c>
       <c r="G57" t="n">
         <v>4640</v>
       </c>
-      <c r="H57" s="4" t="n">
+      <c r="H57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I57" t="inlineStr">
-        <is>
-          <t>2722</t>
+      <c r="I57" t="n">
+        <v>2722</v>
+      </c>
+      <c r="J57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>2931</t>
         </is>
       </c>
     </row>
@@ -2497,18 +2819,24 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F58" s="4" t="n">
+      <c r="F58" s="3" t="n">
         <v>20</v>
       </c>
       <c r="G58" t="n">
         <v>5366</v>
       </c>
-      <c r="H58" s="4" t="n">
+      <c r="H58" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="I58" t="inlineStr">
-        <is>
-          <t>2767</t>
+      <c r="I58" t="n">
+        <v>2767</v>
+      </c>
+      <c r="J58" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>3092</t>
         </is>
       </c>
     </row>
@@ -2534,18 +2862,24 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F59" s="3" t="n">
+      <c r="F59" s="4" t="n">
         <v>33</v>
       </c>
       <c r="G59" t="n">
         <v>4781</v>
       </c>
-      <c r="H59" s="3" t="n">
+      <c r="H59" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I59" t="inlineStr">
-        <is>
-          <t>2757</t>
+      <c r="I59" t="n">
+        <v>2757</v>
+      </c>
+      <c r="J59" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>2962</t>
         </is>
       </c>
     </row>
@@ -2577,12 +2911,18 @@
       <c r="G60" t="n">
         <v>5311</v>
       </c>
-      <c r="H60" s="4" t="n">
+      <c r="H60" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I60" t="inlineStr">
-        <is>
-          <t>2806</t>
+      <c r="I60" t="n">
+        <v>2806</v>
+      </c>
+      <c r="J60" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>3079</t>
         </is>
       </c>
     </row>
@@ -2608,18 +2948,24 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F61" s="4" t="n">
+      <c r="F61" s="3" t="n">
         <v>26</v>
       </c>
       <c r="G61" t="n">
         <v>5735</v>
       </c>
-      <c r="H61" s="4" t="n">
+      <c r="H61" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="I61" t="inlineStr">
-        <is>
-          <t>2750</t>
+      <c r="I61" t="n">
+        <v>2750</v>
+      </c>
+      <c r="J61" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>3160</t>
         </is>
       </c>
     </row>
@@ -2645,7 +2991,7 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F62" s="4" t="n">
+      <c r="F62" s="3" t="n">
         <v>21</v>
       </c>
       <c r="G62" t="n">
@@ -2654,9 +3000,15 @@
       <c r="H62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I62" t="inlineStr">
-        <is>
-          <t>2494</t>
+      <c r="I62" t="n">
+        <v>2494</v>
+      </c>
+      <c r="J62" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>2882</t>
         </is>
       </c>
     </row>
@@ -2691,9 +3043,15 @@
       <c r="H63" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="I63" t="inlineStr">
-        <is>
-          <t>2605</t>
+      <c r="I63" t="n">
+        <v>2605</v>
+      </c>
+      <c r="J63" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>2621</t>
         </is>
       </c>
     </row>
@@ -2719,7 +3077,7 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F64" s="4" t="n">
+      <c r="F64" s="3" t="n">
         <v>20</v>
       </c>
       <c r="G64" t="n">
@@ -2728,9 +3086,15 @@
       <c r="H64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I64" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I64" t="n">
+        <v>0</v>
+      </c>
+      <c r="J64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>2493</t>
         </is>
       </c>
     </row>
@@ -2756,18 +3120,24 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F65" s="4" t="n">
+      <c r="F65" s="3" t="n">
         <v>20</v>
       </c>
       <c r="G65" t="n">
         <v>5316</v>
       </c>
-      <c r="H65" s="4" t="n">
+      <c r="H65" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="I65" t="inlineStr">
-        <is>
-          <t>2724</t>
+      <c r="I65" t="n">
+        <v>2724</v>
+      </c>
+      <c r="J65" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>2995</t>
         </is>
       </c>
     </row>
@@ -2802,9 +3172,15 @@
       <c r="H66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I66" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I66" t="n">
+        <v>0</v>
+      </c>
+      <c r="J66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>2524</t>
         </is>
       </c>
     </row>
@@ -2830,18 +3206,24 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F67" s="4" t="n">
+      <c r="F67" s="3" t="n">
         <v>30</v>
       </c>
       <c r="G67" t="n">
         <v>5795</v>
       </c>
-      <c r="H67" s="4" t="n">
+      <c r="H67" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="I67" t="inlineStr">
-        <is>
-          <t>2875</t>
+      <c r="I67" t="n">
+        <v>2875</v>
+      </c>
+      <c r="J67" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>3215</t>
         </is>
       </c>
     </row>
@@ -2867,18 +3249,24 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F68" s="4" t="n">
+      <c r="F68" s="3" t="n">
         <v>30</v>
       </c>
       <c r="G68" t="n">
         <v>4666</v>
       </c>
-      <c r="H68" s="3" t="n">
+      <c r="H68" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="I68" t="inlineStr">
-        <is>
-          <t>2797</t>
+      <c r="I68" t="n">
+        <v>2797</v>
+      </c>
+      <c r="J68" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>2974</t>
         </is>
       </c>
     </row>
@@ -2904,7 +3292,7 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F69" s="4" t="n">
+      <c r="F69" s="3" t="n">
         <v>22</v>
       </c>
       <c r="G69" t="n">
@@ -2913,9 +3301,15 @@
       <c r="H69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I69" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I69" t="n">
+        <v>0</v>
+      </c>
+      <c r="J69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -2947,12 +3341,18 @@
       <c r="G70" t="n">
         <v>4475</v>
       </c>
-      <c r="H70" s="4" t="n">
+      <c r="H70" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="I70" t="inlineStr">
-        <is>
-          <t>2722</t>
+      <c r="I70" t="n">
+        <v>2722</v>
+      </c>
+      <c r="J70" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>2938</t>
         </is>
       </c>
     </row>
@@ -2984,12 +3384,18 @@
       <c r="G71" t="n">
         <v>4311</v>
       </c>
-      <c r="H71" s="4" t="n">
+      <c r="H71" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="I71" t="inlineStr">
-        <is>
-          <t>2804</t>
+      <c r="I71" t="n">
+        <v>2804</v>
+      </c>
+      <c r="J71" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>2951</t>
         </is>
       </c>
     </row>
@@ -3015,18 +3421,24 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F72" s="3" t="n">
+      <c r="F72" s="4" t="n">
         <v>40</v>
       </c>
       <c r="G72" t="n">
         <v>6001</v>
       </c>
-      <c r="H72" s="3" t="n">
+      <c r="H72" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I72" t="inlineStr">
-        <is>
-          <t>3070</t>
+      <c r="I72" t="n">
+        <v>3070</v>
+      </c>
+      <c r="J72" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>3364</t>
         </is>
       </c>
     </row>
@@ -3061,9 +3473,15 @@
       <c r="H73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I73" t="inlineStr">
-        <is>
-          <t>2478</t>
+      <c r="I73" t="n">
+        <v>2478</v>
+      </c>
+      <c r="J73" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>2815</t>
         </is>
       </c>
     </row>
@@ -3089,7 +3507,7 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F74" s="4" t="n">
+      <c r="F74" s="3" t="n">
         <v>29</v>
       </c>
       <c r="G74" t="n">
@@ -3098,9 +3516,15 @@
       <c r="H74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I74" t="inlineStr">
-        <is>
-          <t>2496</t>
+      <c r="I74" t="n">
+        <v>2496</v>
+      </c>
+      <c r="J74" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>2790</t>
         </is>
       </c>
     </row>
@@ -3126,18 +3550,24 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F75" s="4" t="n">
+      <c r="F75" s="3" t="n">
         <v>25</v>
       </c>
       <c r="G75" t="n">
         <v>3959</v>
       </c>
-      <c r="H75" s="4" t="n">
+      <c r="H75" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="I75" t="inlineStr">
-        <is>
-          <t>2610</t>
+      <c r="I75" t="n">
+        <v>2610</v>
+      </c>
+      <c r="J75" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>2831</t>
         </is>
       </c>
     </row>
@@ -3160,7 +3590,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="F76" s="5" t="n">
@@ -3169,12 +3599,18 @@
       <c r="G76" t="n">
         <v>5084</v>
       </c>
-      <c r="H76" s="4" t="n">
+      <c r="H76" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I76" t="inlineStr">
-        <is>
-          <t>2789</t>
+      <c r="I76" t="n">
+        <v>2789</v>
+      </c>
+      <c r="J76" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>3058</t>
         </is>
       </c>
     </row>
@@ -3206,12 +3642,18 @@
       <c r="G77" t="n">
         <v>5763</v>
       </c>
-      <c r="H77" s="4" t="n">
+      <c r="H77" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I77" t="inlineStr">
-        <is>
-          <t>2870</t>
+      <c r="I77" t="n">
+        <v>2870</v>
+      </c>
+      <c r="J77" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>3117</t>
         </is>
       </c>
     </row>
@@ -3246,7 +3688,13 @@
       <c r="H78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I78" t="inlineStr">
+      <c r="I78" t="n">
+        <v>0</v>
+      </c>
+      <c r="J78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3280,12 +3728,18 @@
       <c r="G79" t="n">
         <v>5392</v>
       </c>
-      <c r="H79" s="4" t="n">
+      <c r="H79" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="I79" t="inlineStr">
-        <is>
-          <t>2945</t>
+      <c r="I79" t="n">
+        <v>2945</v>
+      </c>
+      <c r="J79" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>3256</t>
         </is>
       </c>
     </row>
@@ -3311,7 +3765,7 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F80" s="3" t="n">
+      <c r="F80" s="4" t="n">
         <v>32</v>
       </c>
       <c r="G80" t="n">
@@ -3320,9 +3774,15 @@
       <c r="H80" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="I80" t="inlineStr">
-        <is>
-          <t>2673</t>
+      <c r="I80" t="n">
+        <v>2673</v>
+      </c>
+      <c r="J80" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>2742</t>
         </is>
       </c>
     </row>
@@ -3348,18 +3808,24 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F81" s="4" t="n">
+      <c r="F81" s="3" t="n">
         <v>30</v>
       </c>
       <c r="G81" t="n">
         <v>5042</v>
       </c>
-      <c r="H81" s="4" t="n">
+      <c r="H81" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="I81" t="inlineStr">
-        <is>
-          <t>2846</t>
+      <c r="I81" t="n">
+        <v>2846</v>
+      </c>
+      <c r="J81" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>2950</t>
         </is>
       </c>
     </row>
@@ -3385,18 +3851,24 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F82" s="4" t="n">
+      <c r="F82" s="3" t="n">
         <v>30</v>
       </c>
       <c r="G82" t="n">
         <v>5240</v>
       </c>
-      <c r="H82" s="4" t="n">
+      <c r="H82" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I82" t="inlineStr">
-        <is>
-          <t>2992</t>
+      <c r="I82" t="n">
+        <v>2992</v>
+      </c>
+      <c r="J82" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>3157</t>
         </is>
       </c>
     </row>
@@ -3422,18 +3894,24 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F83" s="4" t="n">
+      <c r="F83" s="3" t="n">
         <v>30</v>
       </c>
       <c r="G83" t="n">
         <v>4926</v>
       </c>
-      <c r="H83" s="3" t="n">
+      <c r="H83" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I83" t="inlineStr">
-        <is>
-          <t>2887</t>
+      <c r="I83" t="n">
+        <v>2887</v>
+      </c>
+      <c r="J83" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>3096</t>
         </is>
       </c>
     </row>
@@ -3459,18 +3937,24 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F84" s="4" t="n">
+      <c r="F84" s="3" t="n">
         <v>27</v>
       </c>
       <c r="G84" t="n">
         <v>4938</v>
       </c>
-      <c r="H84" s="4" t="n">
+      <c r="H84" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="I84" t="inlineStr">
-        <is>
-          <t>2876</t>
+      <c r="I84" t="n">
+        <v>2876</v>
+      </c>
+      <c r="J84" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>2983</t>
         </is>
       </c>
     </row>
@@ -3496,18 +3980,24 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F85" s="4" t="n">
+      <c r="F85" s="3" t="n">
         <v>20</v>
       </c>
       <c r="G85" t="n">
         <v>4781</v>
       </c>
-      <c r="H85" s="4" t="n">
+      <c r="H85" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I85" t="inlineStr">
-        <is>
-          <t>2768</t>
+      <c r="I85" t="n">
+        <v>2768</v>
+      </c>
+      <c r="J85" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>2906</t>
         </is>
       </c>
     </row>
@@ -3539,12 +4029,18 @@
       <c r="G86" t="n">
         <v>3987</v>
       </c>
-      <c r="H86" s="4" t="n">
+      <c r="H86" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I86" t="inlineStr">
-        <is>
-          <t>2657</t>
+      <c r="I86" t="n">
+        <v>2657</v>
+      </c>
+      <c r="J86" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>2878</t>
         </is>
       </c>
     </row>
@@ -3576,12 +4072,18 @@
       <c r="G87" t="n">
         <v>3873</v>
       </c>
-      <c r="H87" s="4" t="n">
+      <c r="H87" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I87" t="inlineStr">
-        <is>
-          <t>2550</t>
+      <c r="I87" t="n">
+        <v>2550</v>
+      </c>
+      <c r="J87" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>2605</t>
         </is>
       </c>
     </row>
@@ -3607,18 +4109,24 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F88" s="4" t="n">
+      <c r="F88" s="3" t="n">
         <v>30</v>
       </c>
       <c r="G88" t="n">
         <v>5219</v>
       </c>
-      <c r="H88" s="3" t="n">
+      <c r="H88" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I88" t="inlineStr">
-        <is>
-          <t>2981</t>
+      <c r="I88" t="n">
+        <v>2981</v>
+      </c>
+      <c r="J88" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>3048</t>
         </is>
       </c>
     </row>
@@ -3644,18 +4152,24 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F89" s="4" t="n">
+      <c r="F89" s="3" t="n">
         <v>20</v>
       </c>
       <c r="G89" t="n">
         <v>3096</v>
       </c>
-      <c r="H89" s="4" t="n">
+      <c r="H89" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I89" t="inlineStr">
-        <is>
-          <t>2566</t>
+      <c r="I89" t="n">
+        <v>2566</v>
+      </c>
+      <c r="J89" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>2600</t>
         </is>
       </c>
     </row>
@@ -3681,18 +4195,24 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F90" s="4" t="n">
+      <c r="F90" s="3" t="n">
         <v>21</v>
       </c>
       <c r="G90" t="n">
         <v>3545</v>
       </c>
-      <c r="H90" s="4" t="n">
+      <c r="H90" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="I90" t="inlineStr">
-        <is>
-          <t>2677</t>
+      <c r="I90" t="n">
+        <v>2677</v>
+      </c>
+      <c r="J90" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>2794</t>
         </is>
       </c>
     </row>
@@ -3727,9 +4247,15 @@
       <c r="H91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I91" t="inlineStr">
-        <is>
-          <t>2018</t>
+      <c r="I91" t="n">
+        <v>2018</v>
+      </c>
+      <c r="J91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>2011</t>
         </is>
       </c>
     </row>
@@ -3764,9 +4290,15 @@
       <c r="H92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I92" t="inlineStr">
-        <is>
-          <t>2428</t>
+      <c r="I92" t="n">
+        <v>2428</v>
+      </c>
+      <c r="J92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>2395</t>
         </is>
       </c>
     </row>
@@ -3801,9 +4333,15 @@
       <c r="H93" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="I93" t="inlineStr">
-        <is>
-          <t>2470</t>
+      <c r="I93" t="n">
+        <v>2470</v>
+      </c>
+      <c r="J93" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>2524</t>
         </is>
       </c>
     </row>
@@ -3838,9 +4376,15 @@
       <c r="H94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I94" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I94" t="n">
+        <v>0</v>
+      </c>
+      <c r="J94" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>2347</t>
         </is>
       </c>
     </row>
@@ -3872,12 +4416,18 @@
       <c r="G95" t="n">
         <v>6055</v>
       </c>
-      <c r="H95" s="4" t="n">
+      <c r="H95" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I95" t="inlineStr">
-        <is>
-          <t>2945</t>
+      <c r="I95" t="n">
+        <v>2945</v>
+      </c>
+      <c r="J95" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>3321</t>
         </is>
       </c>
     </row>
@@ -3912,9 +4462,15 @@
       <c r="H96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I96" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I96" t="n">
+        <v>0</v>
+      </c>
+      <c r="J96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>2468</t>
         </is>
       </c>
     </row>
@@ -3949,9 +4505,15 @@
       <c r="H97" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="I97" t="inlineStr">
-        <is>
-          <t>2514</t>
+      <c r="I97" t="n">
+        <v>2514</v>
+      </c>
+      <c r="J97" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K97" t="inlineStr">
+        <is>
+          <t>2525</t>
         </is>
       </c>
     </row>
@@ -3977,18 +4539,24 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F98" s="4" t="n">
+      <c r="F98" s="3" t="n">
         <v>26</v>
       </c>
       <c r="G98" t="n">
         <v>3616</v>
       </c>
-      <c r="H98" s="4" t="n">
+      <c r="H98" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I98" t="inlineStr">
-        <is>
-          <t>2533</t>
+      <c r="I98" t="n">
+        <v>2533</v>
+      </c>
+      <c r="J98" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>2584</t>
         </is>
       </c>
     </row>
@@ -4020,12 +4588,18 @@
       <c r="G99" t="n">
         <v>4614</v>
       </c>
-      <c r="H99" s="4" t="n">
+      <c r="H99" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I99" t="inlineStr">
-        <is>
-          <t>2795</t>
+      <c r="I99" t="n">
+        <v>2795</v>
+      </c>
+      <c r="J99" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K99" t="inlineStr">
+        <is>
+          <t>2995</t>
         </is>
       </c>
     </row>
@@ -4051,18 +4625,24 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F100" s="4" t="n">
+      <c r="F100" s="3" t="n">
         <v>20</v>
       </c>
       <c r="G100" t="n">
         <v>4197</v>
       </c>
-      <c r="H100" s="4" t="n">
+      <c r="H100" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I100" t="inlineStr">
-        <is>
-          <t>2638</t>
+      <c r="I100" t="n">
+        <v>2638</v>
+      </c>
+      <c r="J100" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>2865</t>
         </is>
       </c>
     </row>
@@ -4094,12 +4674,18 @@
       <c r="G101" t="n">
         <v>4006</v>
       </c>
-      <c r="H101" s="4" t="n">
+      <c r="H101" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="I101" t="inlineStr">
-        <is>
-          <t>2575</t>
+      <c r="I101" t="n">
+        <v>2575</v>
+      </c>
+      <c r="J101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>2535</t>
         </is>
       </c>
     </row>
@@ -4131,12 +4717,18 @@
       <c r="G102" t="n">
         <v>4671</v>
       </c>
-      <c r="H102" s="4" t="n">
+      <c r="H102" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I102" t="inlineStr">
-        <is>
-          <t>2769</t>
+      <c r="I102" t="n">
+        <v>2769</v>
+      </c>
+      <c r="J102" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>3047</t>
         </is>
       </c>
     </row>
@@ -4168,12 +4760,18 @@
       <c r="G103" t="n">
         <v>4038</v>
       </c>
-      <c r="H103" s="4" t="n">
+      <c r="H103" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="I103" t="inlineStr">
-        <is>
-          <t>2680</t>
+      <c r="I103" t="n">
+        <v>2680</v>
+      </c>
+      <c r="J103" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>2876</t>
         </is>
       </c>
     </row>
@@ -4208,9 +4806,15 @@
       <c r="H104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I104" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I104" t="n">
+        <v>0</v>
+      </c>
+      <c r="J104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K104" t="inlineStr">
+        <is>
+          <t>2484</t>
         </is>
       </c>
     </row>
@@ -4236,18 +4840,24 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F105" s="4" t="n">
+      <c r="F105" s="3" t="n">
         <v>20</v>
       </c>
       <c r="G105" t="n">
         <v>5710</v>
       </c>
-      <c r="H105" s="4" t="n">
+      <c r="H105" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I105" t="inlineStr">
-        <is>
-          <t>2765</t>
+      <c r="I105" t="n">
+        <v>2765</v>
+      </c>
+      <c r="J105" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="K105" t="inlineStr">
+        <is>
+          <t>2993</t>
         </is>
       </c>
     </row>
@@ -4282,9 +4892,15 @@
       <c r="H106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I106" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I106" t="n">
+        <v>0</v>
+      </c>
+      <c r="J106" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K106" t="inlineStr">
+        <is>
+          <t>2806</t>
         </is>
       </c>
     </row>
@@ -4310,18 +4926,24 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F107" s="4" t="n">
+      <c r="F107" s="3" t="n">
         <v>26</v>
       </c>
       <c r="G107" t="n">
         <v>3670</v>
       </c>
-      <c r="H107" s="4" t="n">
+      <c r="H107" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I107" t="inlineStr">
-        <is>
-          <t>2569</t>
+      <c r="I107" t="n">
+        <v>2569</v>
+      </c>
+      <c r="J107" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K107" t="inlineStr">
+        <is>
+          <t>2732</t>
         </is>
       </c>
     </row>
@@ -4356,9 +4978,15 @@
       <c r="H108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I108" t="inlineStr">
-        <is>
-          <t>2519</t>
+      <c r="I108" t="n">
+        <v>2519</v>
+      </c>
+      <c r="J108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K108" t="inlineStr">
+        <is>
+          <t>2518</t>
         </is>
       </c>
     </row>
@@ -4393,9 +5021,15 @@
       <c r="H109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I109" t="inlineStr">
-        <is>
-          <t>2502</t>
+      <c r="I109" t="n">
+        <v>2502</v>
+      </c>
+      <c r="J109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>2528</t>
         </is>
       </c>
     </row>
@@ -4421,18 +5055,24 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F110" s="4" t="n">
+      <c r="F110" s="3" t="n">
         <v>20</v>
       </c>
       <c r="G110" t="n">
         <v>3693</v>
       </c>
-      <c r="H110" s="4" t="n">
+      <c r="H110" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I110" t="inlineStr">
-        <is>
-          <t>2609</t>
+      <c r="I110" t="n">
+        <v>2609</v>
+      </c>
+      <c r="J110" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K110" t="inlineStr">
+        <is>
+          <t>2777</t>
         </is>
       </c>
     </row>
@@ -4467,9 +5107,15 @@
       <c r="H111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I111" t="inlineStr">
-        <is>
-          <t>2574</t>
+      <c r="I111" t="n">
+        <v>2574</v>
+      </c>
+      <c r="J111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K111" t="inlineStr">
+        <is>
+          <t>2764</t>
         </is>
       </c>
     </row>
@@ -4501,12 +5147,18 @@
       <c r="G112" t="n">
         <v>3825</v>
       </c>
-      <c r="H112" s="4" t="n">
+      <c r="H112" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I112" t="inlineStr">
-        <is>
-          <t>2772</t>
+      <c r="I112" t="n">
+        <v>2772</v>
+      </c>
+      <c r="J112" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K112" t="inlineStr">
+        <is>
+          <t>2926</t>
         </is>
       </c>
     </row>
@@ -4541,9 +5193,15 @@
       <c r="H113" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="I113" t="inlineStr">
-        <is>
-          <t>2493</t>
+      <c r="I113" t="n">
+        <v>2493</v>
+      </c>
+      <c r="J113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>2431</t>
         </is>
       </c>
     </row>
@@ -4578,9 +5236,15 @@
       <c r="H114" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="I114" t="inlineStr">
-        <is>
-          <t>2432</t>
+      <c r="I114" t="n">
+        <v>2432</v>
+      </c>
+      <c r="J114" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="K114" t="inlineStr">
+        <is>
+          <t>2434</t>
         </is>
       </c>
     </row>
@@ -4606,18 +5270,24 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F115" s="4" t="n">
+      <c r="F115" s="3" t="n">
         <v>21</v>
       </c>
       <c r="G115" t="n">
         <v>3810</v>
       </c>
-      <c r="H115" s="4" t="n">
+      <c r="H115" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="I115" t="inlineStr">
-        <is>
-          <t>2598</t>
+      <c r="I115" t="n">
+        <v>2598</v>
+      </c>
+      <c r="J115" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>2812</t>
         </is>
       </c>
     </row>
@@ -4652,9 +5322,15 @@
       <c r="H116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I116" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I116" t="n">
+        <v>0</v>
+      </c>
+      <c r="J116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K116" t="inlineStr">
+        <is>
+          <t>2533</t>
         </is>
       </c>
     </row>
@@ -4680,18 +5356,24 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F117" s="4" t="n">
+      <c r="F117" s="3" t="n">
         <v>20</v>
       </c>
       <c r="G117" t="n">
         <v>3776</v>
       </c>
-      <c r="H117" s="4" t="n">
+      <c r="H117" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I117" t="inlineStr">
-        <is>
-          <t>2621</t>
+      <c r="I117" t="n">
+        <v>2621</v>
+      </c>
+      <c r="J117" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>2677</t>
         </is>
       </c>
     </row>
@@ -4726,9 +5408,15 @@
       <c r="H118" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="I118" t="inlineStr">
-        <is>
-          <t>2413</t>
+      <c r="I118" t="n">
+        <v>2413</v>
+      </c>
+      <c r="J118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K118" t="inlineStr">
+        <is>
+          <t>2356</t>
         </is>
       </c>
     </row>
@@ -4760,12 +5448,18 @@
       <c r="G119" t="n">
         <v>3836</v>
       </c>
-      <c r="H119" s="4" t="n">
+      <c r="H119" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="I119" t="inlineStr">
-        <is>
-          <t>2767</t>
+      <c r="I119" t="n">
+        <v>2767</v>
+      </c>
+      <c r="J119" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="K119" t="inlineStr">
+        <is>
+          <t>2872</t>
         </is>
       </c>
     </row>
@@ -4791,18 +5485,24 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F120" s="4" t="n">
+      <c r="F120" s="3" t="n">
         <v>30</v>
       </c>
       <c r="G120" t="n">
         <v>2823</v>
       </c>
-      <c r="H120" s="4" t="n">
+      <c r="H120" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I120" t="inlineStr">
-        <is>
-          <t>2496</t>
+      <c r="I120" t="n">
+        <v>2496</v>
+      </c>
+      <c r="J120" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="K120" t="inlineStr">
+        <is>
+          <t>2548</t>
         </is>
       </c>
     </row>
@@ -4828,18 +5528,24 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F121" s="4" t="n">
+      <c r="F121" s="3" t="n">
         <v>20</v>
       </c>
       <c r="G121" t="n">
         <v>3446</v>
       </c>
-      <c r="H121" s="4" t="n">
+      <c r="H121" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I121" t="inlineStr">
-        <is>
-          <t>2539</t>
+      <c r="I121" t="n">
+        <v>2539</v>
+      </c>
+      <c r="J121" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="K121" t="inlineStr">
+        <is>
+          <t>2665</t>
         </is>
       </c>
     </row>
@@ -4865,18 +5571,24 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F122" s="4" t="n">
+      <c r="F122" s="3" t="n">
         <v>20</v>
       </c>
       <c r="G122" t="n">
         <v>3386</v>
       </c>
-      <c r="H122" s="4" t="n">
+      <c r="H122" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I122" t="inlineStr">
-        <is>
-          <t>2539</t>
+      <c r="I122" t="n">
+        <v>2539</v>
+      </c>
+      <c r="J122" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K122" t="inlineStr">
+        <is>
+          <t>2590</t>
         </is>
       </c>
     </row>
@@ -4902,18 +5614,24 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F123" s="4" t="n">
+      <c r="F123" s="3" t="n">
         <v>20</v>
       </c>
       <c r="G123" t="n">
         <v>3923</v>
       </c>
-      <c r="H123" s="4" t="n">
+      <c r="H123" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I123" t="inlineStr">
-        <is>
-          <t>2720</t>
+      <c r="I123" t="n">
+        <v>2720</v>
+      </c>
+      <c r="J123" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K123" t="inlineStr">
+        <is>
+          <t>2625</t>
         </is>
       </c>
     </row>
@@ -4939,18 +5657,24 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F124" s="4" t="n">
+      <c r="F124" s="3" t="n">
         <v>20</v>
       </c>
       <c r="G124" t="n">
         <v>3444</v>
       </c>
-      <c r="H124" s="4" t="n">
+      <c r="H124" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I124" t="inlineStr">
-        <is>
-          <t>2617</t>
+      <c r="I124" t="n">
+        <v>2617</v>
+      </c>
+      <c r="J124" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K124" t="inlineStr">
+        <is>
+          <t>2694</t>
         </is>
       </c>
     </row>
@@ -4985,9 +5709,15 @@
       <c r="H125" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="I125" t="inlineStr">
-        <is>
-          <t>2186</t>
+      <c r="I125" t="n">
+        <v>2186</v>
+      </c>
+      <c r="J125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K125" t="inlineStr">
+        <is>
+          <t>2156</t>
         </is>
       </c>
     </row>
@@ -5022,9 +5752,15 @@
       <c r="H126" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="I126" t="inlineStr">
-        <is>
-          <t>2457</t>
+      <c r="I126" t="n">
+        <v>2457</v>
+      </c>
+      <c r="J126" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="K126" t="inlineStr">
+        <is>
+          <t>2465</t>
         </is>
       </c>
     </row>
@@ -5056,12 +5792,18 @@
       <c r="G127" t="n">
         <v>2637</v>
       </c>
-      <c r="H127" s="4" t="n">
+      <c r="H127" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I127" t="inlineStr">
-        <is>
-          <t>2480</t>
+      <c r="I127" t="n">
+        <v>2480</v>
+      </c>
+      <c r="J127" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K127" t="inlineStr">
+        <is>
+          <t>2502</t>
         </is>
       </c>
     </row>
@@ -5084,21 +5826,27 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F128" s="4" t="n">
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F128" s="3" t="n">
         <v>23</v>
       </c>
       <c r="G128" t="n">
         <v>6015</v>
       </c>
-      <c r="H128" s="4" t="n">
+      <c r="H128" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I128" t="inlineStr">
-        <is>
-          <t>2818</t>
+      <c r="I128" t="n">
+        <v>2818</v>
+      </c>
+      <c r="J128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K128" t="inlineStr">
+        <is>
+          <t>2814</t>
         </is>
       </c>
     </row>
@@ -5133,11 +5881,11 @@
       <c r="H129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I129" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="I129" t="n">
+        <v>0</v>
+      </c>
+      <c r="J129" s="3" t="inlineStr"/>
+      <c r="K129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="n">
@@ -5170,9 +5918,15 @@
       <c r="H130" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="I130" t="inlineStr">
-        <is>
-          <t>2498</t>
+      <c r="I130" t="n">
+        <v>2498</v>
+      </c>
+      <c r="J130" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="K130" t="inlineStr">
+        <is>
+          <t>2591</t>
         </is>
       </c>
     </row>
@@ -5195,7 +5949,7 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F131" s="2" t="n">
@@ -5207,9 +5961,15 @@
       <c r="H131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I131" t="inlineStr">
-        <is>
-          <t>2485</t>
+      <c r="I131" t="n">
+        <v>2485</v>
+      </c>
+      <c r="J131" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K131" t="inlineStr">
+        <is>
+          <t>2685</t>
         </is>
       </c>
     </row>
@@ -5235,18 +5995,24 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F132" s="4" t="n">
+      <c r="F132" s="3" t="n">
         <v>20</v>
       </c>
       <c r="G132" t="n">
         <v>3966</v>
       </c>
-      <c r="H132" s="4" t="n">
+      <c r="H132" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I132" t="inlineStr">
-        <is>
-          <t>2527</t>
+      <c r="I132" t="n">
+        <v>2527</v>
+      </c>
+      <c r="J132" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K132" t="inlineStr">
+        <is>
+          <t>2688</t>
         </is>
       </c>
     </row>
@@ -5281,11 +6047,11 @@
       <c r="H133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I133" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="I133" t="n">
+        <v>0</v>
+      </c>
+      <c r="J133" s="3" t="inlineStr"/>
+      <c r="K133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="n">
@@ -5315,12 +6081,18 @@
       <c r="G134" t="n">
         <v>3040</v>
       </c>
-      <c r="H134" s="4" t="n">
+      <c r="H134" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I134" t="inlineStr">
-        <is>
-          <t>2521</t>
+      <c r="I134" t="n">
+        <v>2521</v>
+      </c>
+      <c r="J134" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="K134" t="inlineStr">
+        <is>
+          <t>2596</t>
         </is>
       </c>
     </row>
@@ -5355,9 +6127,15 @@
       <c r="H135" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I135" t="inlineStr">
-        <is>
-          <t>2473</t>
+      <c r="I135" t="n">
+        <v>2473</v>
+      </c>
+      <c r="J135" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K135" t="inlineStr">
+        <is>
+          <t>2492</t>
         </is>
       </c>
     </row>
@@ -5392,9 +6170,15 @@
       <c r="H136" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="I136" t="inlineStr">
-        <is>
-          <t>2497</t>
+      <c r="I136" t="n">
+        <v>2497</v>
+      </c>
+      <c r="J136" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="K136" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -5429,9 +6213,15 @@
       <c r="H137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I137" t="inlineStr">
-        <is>
-          <t>1988</t>
+      <c r="I137" t="n">
+        <v>1988</v>
+      </c>
+      <c r="J137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K137" t="inlineStr">
+        <is>
+          <t>1982</t>
         </is>
       </c>
     </row>
@@ -5466,11 +6256,11 @@
       <c r="H138" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I138" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="I138" t="n">
+        <v>0</v>
+      </c>
+      <c r="J138" s="3" t="inlineStr"/>
+      <c r="K138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -5503,11 +6293,11 @@
       <c r="H139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I139" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="I139" t="n">
+        <v>0</v>
+      </c>
+      <c r="J139" s="3" t="inlineStr"/>
+      <c r="K139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -5540,11 +6330,11 @@
       <c r="H140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I140" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="I140" t="n">
+        <v>0</v>
+      </c>
+      <c r="J140" s="3" t="inlineStr"/>
+      <c r="K140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="n">
@@ -5577,9 +6367,15 @@
       <c r="H141" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I141" t="inlineStr">
-        <is>
-          <t>2000</t>
+      <c r="I141" t="n">
+        <v>2000</v>
+      </c>
+      <c r="J141" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K141" t="inlineStr">
+        <is>
+          <t>1995</t>
         </is>
       </c>
     </row>
@@ -5614,11 +6410,11 @@
       <c r="H142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I142" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="I142" t="n">
+        <v>0</v>
+      </c>
+      <c r="J142" s="3" t="inlineStr"/>
+      <c r="K142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="n">
@@ -5651,11 +6447,11 @@
       <c r="H143" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I143" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="I143" t="n">
+        <v>0</v>
+      </c>
+      <c r="J143" s="3" t="inlineStr"/>
+      <c r="K143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -5688,11 +6484,11 @@
       <c r="H144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I144" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="I144" t="n">
+        <v>0</v>
+      </c>
+      <c r="J144" s="3" t="inlineStr"/>
+      <c r="K144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -5725,11 +6521,11 @@
       <c r="H145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I145" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="I145" t="n">
+        <v>0</v>
+      </c>
+      <c r="J145" s="3" t="inlineStr"/>
+      <c r="K145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -5762,11 +6558,11 @@
       <c r="H146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I146" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="I146" t="n">
+        <v>0</v>
+      </c>
+      <c r="J146" s="3" t="inlineStr"/>
+      <c r="K146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -5799,11 +6595,11 @@
       <c r="H147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I147" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="I147" t="n">
+        <v>0</v>
+      </c>
+      <c r="J147" s="3" t="inlineStr"/>
+      <c r="K147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -5836,11 +6632,11 @@
       <c r="H148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I148" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="I148" t="n">
+        <v>0</v>
+      </c>
+      <c r="J148" s="3" t="inlineStr"/>
+      <c r="K148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="n">
@@ -5873,11 +6669,11 @@
       <c r="H149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I149" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="I149" t="n">
+        <v>0</v>
+      </c>
+      <c r="J149" s="3" t="inlineStr"/>
+      <c r="K149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="n">
@@ -5910,11 +6706,11 @@
       <c r="H150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I150" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="I150" t="n">
+        <v>0</v>
+      </c>
+      <c r="J150" s="3" t="inlineStr"/>
+      <c r="K150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="n">
@@ -5947,11 +6743,11 @@
       <c r="H151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I151" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="I151" t="n">
+        <v>0</v>
+      </c>
+      <c r="J151" s="3" t="inlineStr"/>
+      <c r="K151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="n">
@@ -5984,11 +6780,11 @@
       <c r="H152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I152" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="I152" t="n">
+        <v>0</v>
+      </c>
+      <c r="J152" s="3" t="inlineStr"/>
+      <c r="K152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" t="n">
@@ -6021,11 +6817,11 @@
       <c r="H153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I153" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="I153" t="n">
+        <v>0</v>
+      </c>
+      <c r="J153" s="3" t="inlineStr"/>
+      <c r="K153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" t="n">
@@ -6058,9 +6854,15 @@
       <c r="H154" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="I154" t="inlineStr">
-        <is>
-          <t>1460</t>
+      <c r="I154" t="n">
+        <v>1460</v>
+      </c>
+      <c r="J154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K154" t="inlineStr">
+        <is>
+          <t>1498</t>
         </is>
       </c>
     </row>
@@ -6086,20 +6888,20 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F155" s="4" t="n">
+      <c r="F155" s="3" t="n">
         <v>20</v>
       </c>
       <c r="G155" t="n">
         <v>1198</v>
       </c>
-      <c r="H155" s="4" t="n">
+      <c r="H155" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="I155" t="inlineStr">
-        <is>
-          <t>1412</t>
-        </is>
-      </c>
+      <c r="I155" t="n">
+        <v>1412</v>
+      </c>
+      <c r="J155" s="3" t="inlineStr"/>
+      <c r="K155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="n">
@@ -6132,9 +6934,15 @@
       <c r="H156" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I156" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I156" t="n">
+        <v>0</v>
+      </c>
+      <c r="J156" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K156" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -6169,7 +6977,13 @@
       <c r="H157" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I157" t="inlineStr">
+      <c r="I157" t="n">
+        <v>0</v>
+      </c>
+      <c r="J157" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K157" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6206,7 +7020,13 @@
       <c r="H158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I158" t="inlineStr">
+      <c r="I158" t="n">
+        <v>0</v>
+      </c>
+      <c r="J158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6234,7 +7054,7 @@
           <t>Chinese</t>
         </is>
       </c>
-      <c r="F159" s="4" t="n">
+      <c r="F159" s="3" t="n">
         <v>29</v>
       </c>
       <c r="G159" t="n">
@@ -6243,9 +7063,15 @@
       <c r="H159" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="I159" t="inlineStr">
-        <is>
-          <t>2782</t>
+      <c r="I159" t="n">
+        <v>2782</v>
+      </c>
+      <c r="J159" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K159" t="inlineStr">
+        <is>
+          <t>3047</t>
         </is>
       </c>
     </row>
@@ -6280,7 +7106,13 @@
       <c r="H160" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I160" t="inlineStr">
+      <c r="I160" t="n">
+        <v>0</v>
+      </c>
+      <c r="J160" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K160" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6317,9 +7149,15 @@
       <c r="H161" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I161" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I161" t="n">
+        <v>0</v>
+      </c>
+      <c r="J161" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K161" t="inlineStr">
+        <is>
+          <t>2475</t>
         </is>
       </c>
     </row>
@@ -6354,7 +7192,13 @@
       <c r="H162" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I162" t="inlineStr">
+      <c r="I162" t="n">
+        <v>0</v>
+      </c>
+      <c r="J162" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K162" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6391,7 +7235,13 @@
       <c r="H163" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I163" t="inlineStr">
+      <c r="I163" t="n">
+        <v>0</v>
+      </c>
+      <c r="J163" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K163" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6410,29 +7260,33 @@
       <c r="D164" t="inlineStr"/>
       <c r="E164" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F164" s="3" t="n">
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F164" s="4" t="n">
         <v>40</v>
       </c>
       <c r="G164" t="n">
         <v>7458</v>
       </c>
-      <c r="H164" s="3" t="n">
+      <c r="H164" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="I164" t="inlineStr">
-        <is>
-          <t>2873</t>
+      <c r="I164" t="n">
+        <v>2873</v>
+      </c>
+      <c r="J164" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="K164" t="inlineStr">
+        <is>
+          <t>3281</t>
         </is>
       </c>
     </row>
     <row r="165">
-      <c r="A165" t="inlineStr">
-        <is>
-          <t>23526770</t>
-        </is>
+      <c r="A165" t="n">
+        <v>23526770</v>
       </c>
       <c r="B165" t="inlineStr">
         <is>
@@ -6446,22 +7300,20 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F165" s="4" t="inlineStr"/>
+      <c r="F165" s="3" t="inlineStr"/>
       <c r="G165" t="inlineStr"/>
-      <c r="H165" s="4" t="n">
+      <c r="H165" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="I165" t="inlineStr">
-        <is>
-          <t>2549</t>
-        </is>
-      </c>
+      <c r="I165" t="n">
+        <v>2549</v>
+      </c>
+      <c r="J165" s="3" t="inlineStr"/>
+      <c r="K165" t="inlineStr"/>
     </row>
     <row r="166">
-      <c r="A166" t="inlineStr">
-        <is>
-          <t>28122155</t>
-        </is>
+      <c r="A166" t="n">
+        <v>28122155</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>
@@ -6475,22 +7327,20 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F166" s="4" t="inlineStr"/>
+      <c r="F166" s="3" t="inlineStr"/>
       <c r="G166" t="inlineStr"/>
       <c r="H166" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I166" t="inlineStr">
-        <is>
-          <t>2509</t>
-        </is>
-      </c>
+      <c r="I166" t="n">
+        <v>2509</v>
+      </c>
+      <c r="J166" s="3" t="inlineStr"/>
+      <c r="K166" t="inlineStr"/>
     </row>
     <row r="167">
-      <c r="A167" t="inlineStr">
-        <is>
-          <t>46415834</t>
-        </is>
+      <c r="A167" t="n">
+        <v>46415834</v>
       </c>
       <c r="B167" t="inlineStr">
         <is>
@@ -6504,16 +7354,16 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F167" s="4" t="inlineStr"/>
+      <c r="F167" s="3" t="inlineStr"/>
       <c r="G167" t="inlineStr"/>
-      <c r="H167" s="3" t="n">
+      <c r="H167" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I167" t="inlineStr">
-        <is>
-          <t>2504</t>
-        </is>
-      </c>
+      <c r="I167" t="n">
+        <v>2504</v>
+      </c>
+      <c r="J167" s="3" t="inlineStr"/>
+      <c r="K167" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Code updated 23-01-20 11:30:29
</commit_message>
<xml_diff>
--- a/Season_Attack/82.xlsx
+++ b/Season_Attack/82.xlsx
@@ -82,9 +82,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G170"/>
+  <dimension ref="A1:I172"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,6 +426,16 @@
           <t>01-18_0</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>01-19_A</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>01-19_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -452,9 +462,15 @@
       <c r="F2" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>3309</t>
+      <c r="G2" t="n">
+        <v>3309</v>
+      </c>
+      <c r="H2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>3336</t>
         </is>
       </c>
     </row>
@@ -480,12 +496,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F3" s="3" t="n">
+      <c r="F3" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>3810</t>
+      <c r="G3" t="n">
+        <v>3810</v>
+      </c>
+      <c r="H3" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>4143</t>
         </is>
       </c>
     </row>
@@ -511,12 +533,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F4" s="4" t="n">
+      <c r="F4" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>3431</t>
+      <c r="G4" t="n">
+        <v>3431</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>3764</t>
         </is>
       </c>
     </row>
@@ -545,9 +573,15 @@
       <c r="F5" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>3482</t>
+      <c r="G5" t="n">
+        <v>3482</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>3795</t>
         </is>
       </c>
     </row>
@@ -573,12 +607,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F6" s="3" t="n">
+      <c r="F6" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>4089</t>
+      <c r="G6" t="n">
+        <v>4089</v>
+      </c>
+      <c r="H6" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>4120</t>
         </is>
       </c>
     </row>
@@ -607,9 +647,15 @@
       <c r="F7" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>3631</t>
+      <c r="G7" t="n">
+        <v>3631</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>3923</t>
         </is>
       </c>
     </row>
@@ -632,15 +678,21 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="F8" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>3455</t>
+      <c r="G8" t="n">
+        <v>3455</v>
+      </c>
+      <c r="H8" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>3605</t>
         </is>
       </c>
     </row>
@@ -664,6 +716,8 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" s="2" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
+      <c r="H9" s="2" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -687,12 +741,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F10" s="3" t="n">
+      <c r="F10" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>3657</t>
+      <c r="G10" t="n">
+        <v>3657</v>
+      </c>
+      <c r="H10" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>3932</t>
         </is>
       </c>
     </row>
@@ -715,15 +775,21 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="F11" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>3769</t>
+      <c r="G11" t="n">
+        <v>3769</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>3960</t>
         </is>
       </c>
     </row>
@@ -752,9 +818,15 @@
       <c r="F12" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>3471</t>
+      <c r="G12" t="n">
+        <v>3471</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>3740</t>
         </is>
       </c>
     </row>
@@ -780,12 +852,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F13" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>2564</t>
+      <c r="F13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>2564</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>2682</t>
         </is>
       </c>
     </row>
@@ -811,12 +889,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F14" s="3" t="n">
+      <c r="F14" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>4174</t>
+      <c r="G14" t="n">
+        <v>4174</v>
+      </c>
+      <c r="H14" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>4586</t>
         </is>
       </c>
     </row>
@@ -845,9 +929,15 @@
       <c r="F15" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>3692</t>
+      <c r="G15" t="n">
+        <v>3692</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>4023</t>
         </is>
       </c>
     </row>
@@ -873,12 +963,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F16" s="3" t="n">
+      <c r="F16" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>4037</t>
+      <c r="G16" t="n">
+        <v>4037</v>
+      </c>
+      <c r="H16" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>4335</t>
         </is>
       </c>
     </row>
@@ -907,9 +1003,15 @@
       <c r="F17" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>3664</t>
+      <c r="G17" t="n">
+        <v>3664</v>
+      </c>
+      <c r="H17" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>3837</t>
         </is>
       </c>
     </row>
@@ -935,12 +1037,18 @@
           <t>Chinese</t>
         </is>
       </c>
-      <c r="F18" s="4" t="n">
+      <c r="F18" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>3206</t>
+      <c r="G18" t="n">
+        <v>3206</v>
+      </c>
+      <c r="H18" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>3609</t>
         </is>
       </c>
     </row>
@@ -966,12 +1074,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F19" s="3" t="n">
+      <c r="F19" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>4187</t>
+      <c r="G19" t="n">
+        <v>4187</v>
+      </c>
+      <c r="H19" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>4525</t>
         </is>
       </c>
     </row>
@@ -1000,9 +1114,15 @@
       <c r="F20" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>3393</t>
+      <c r="G20" t="n">
+        <v>3393</v>
+      </c>
+      <c r="H20" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>3720</t>
         </is>
       </c>
     </row>
@@ -1028,12 +1148,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F21" s="3" t="n">
+      <c r="F21" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>3661</t>
+      <c r="G21" t="n">
+        <v>3661</v>
+      </c>
+      <c r="H21" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>4068</t>
         </is>
       </c>
     </row>
@@ -1059,12 +1185,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F22" s="3" t="n">
+      <c r="F22" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>2787</t>
+      <c r="G22" t="n">
+        <v>2787</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>2745</t>
         </is>
       </c>
     </row>
@@ -1090,12 +1222,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F23" s="3" t="n">
+      <c r="F23" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>3669</t>
+      <c r="G23" t="n">
+        <v>3669</v>
+      </c>
+      <c r="H23" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>3916</t>
         </is>
       </c>
     </row>
@@ -1121,10 +1259,16 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F24" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G24" t="inlineStr">
+      <c r="F24" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1152,12 +1296,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F25" s="3" t="n">
+      <c r="F25" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>3849</t>
+      <c r="G25" t="n">
+        <v>3849</v>
+      </c>
+      <c r="H25" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>4027</t>
         </is>
       </c>
     </row>
@@ -1183,12 +1333,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F26" s="3" t="n">
+      <c r="F26" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>4127</t>
+      <c r="G26" t="n">
+        <v>4127</v>
+      </c>
+      <c r="H26" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>4308</t>
         </is>
       </c>
     </row>
@@ -1211,15 +1367,21 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="F27" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>3412</t>
+      <c r="G27" t="n">
+        <v>3412</v>
+      </c>
+      <c r="H27" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>3503</t>
         </is>
       </c>
     </row>
@@ -1245,12 +1407,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F28" s="3" t="n">
+      <c r="F28" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>4074</t>
+      <c r="G28" t="n">
+        <v>4074</v>
+      </c>
+      <c r="H28" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>4424</t>
         </is>
       </c>
     </row>
@@ -1273,15 +1441,21 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="F29" s="2" t="n">
         <v>28</v>
       </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>3748</t>
+      <c r="G29" t="n">
+        <v>3748</v>
+      </c>
+      <c r="H29" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>4068</t>
         </is>
       </c>
     </row>
@@ -1307,12 +1481,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F30" s="3" t="n">
+      <c r="F30" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>3904</t>
+      <c r="G30" t="n">
+        <v>3904</v>
+      </c>
+      <c r="H30" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>4341</t>
         </is>
       </c>
     </row>
@@ -1338,12 +1518,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F31" s="3" t="n">
+      <c r="F31" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>4108</t>
+      <c r="G31" t="n">
+        <v>4108</v>
+      </c>
+      <c r="H31" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>4464</t>
         </is>
       </c>
     </row>
@@ -1369,12 +1555,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F32" s="4" t="n">
+      <c r="F32" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>2784</t>
+      <c r="G32" t="n">
+        <v>2784</v>
+      </c>
+      <c r="H32" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>2813</t>
         </is>
       </c>
     </row>
@@ -1400,12 +1592,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F33" s="3" t="n">
+      <c r="F33" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>4029</t>
+      <c r="G33" t="n">
+        <v>4029</v>
+      </c>
+      <c r="H33" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>4227</t>
         </is>
       </c>
     </row>
@@ -1434,9 +1632,15 @@
       <c r="F34" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>3496</t>
+      <c r="G34" t="n">
+        <v>3496</v>
+      </c>
+      <c r="H34" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>3803</t>
         </is>
       </c>
     </row>
@@ -1462,12 +1666,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F35" s="3" t="n">
+      <c r="F35" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>3591</t>
+      <c r="G35" t="n">
+        <v>3591</v>
+      </c>
+      <c r="H35" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>3753</t>
         </is>
       </c>
     </row>
@@ -1491,6 +1701,8 @@
       <c r="E36" t="inlineStr"/>
       <c r="F36" s="2" t="inlineStr"/>
       <c r="G36" t="inlineStr"/>
+      <c r="H36" s="2" t="inlineStr"/>
+      <c r="I36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -1514,12 +1726,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F37" s="3" t="n">
+      <c r="F37" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>3843</t>
+      <c r="G37" t="n">
+        <v>3843</v>
+      </c>
+      <c r="H37" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>4054</t>
         </is>
       </c>
     </row>
@@ -1545,12 +1763,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F38" s="3" t="n">
+      <c r="F38" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>3810</t>
+      <c r="G38" t="n">
+        <v>3810</v>
+      </c>
+      <c r="H38" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>3883</t>
         </is>
       </c>
     </row>
@@ -1576,12 +1800,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F39" s="3" t="n">
+      <c r="F39" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>4321</t>
+      <c r="G39" t="n">
+        <v>4321</v>
+      </c>
+      <c r="H39" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>4642</t>
         </is>
       </c>
     </row>
@@ -1610,9 +1840,15 @@
       <c r="F40" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>3594</t>
+      <c r="G40" t="n">
+        <v>3594</v>
+      </c>
+      <c r="H40" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>3886</t>
         </is>
       </c>
     </row>
@@ -1638,12 +1874,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F41" s="3" t="n">
+      <c r="F41" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>4179</t>
+      <c r="G41" t="n">
+        <v>4179</v>
+      </c>
+      <c r="H41" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>4430</t>
         </is>
       </c>
     </row>
@@ -1669,12 +1911,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F42" s="3" t="n">
+      <c r="F42" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>3890</t>
+      <c r="G42" t="n">
+        <v>3890</v>
+      </c>
+      <c r="H42" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>4198</t>
         </is>
       </c>
     </row>
@@ -1698,6 +1946,8 @@
       <c r="E43" t="inlineStr"/>
       <c r="F43" s="2" t="inlineStr"/>
       <c r="G43" t="inlineStr"/>
+      <c r="H43" s="2" t="inlineStr"/>
+      <c r="I43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -1721,12 +1971,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F44" s="3" t="n">
+      <c r="F44" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>3567</t>
+      <c r="G44" t="n">
+        <v>3567</v>
+      </c>
+      <c r="H44" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>3724</t>
         </is>
       </c>
     </row>
@@ -1755,9 +2011,15 @@
       <c r="F45" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>3578</t>
+      <c r="G45" t="n">
+        <v>3578</v>
+      </c>
+      <c r="H45" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>3744</t>
         </is>
       </c>
     </row>
@@ -1783,10 +2045,16 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F46" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G46" t="inlineStr">
+      <c r="F46" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" t="n">
+        <v>2662</v>
+      </c>
+      <c r="H46" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I46" t="inlineStr">
         <is>
           <t>2662</t>
         </is>
@@ -1814,12 +2082,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F47" s="3" t="n">
+      <c r="F47" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>3962</t>
+      <c r="G47" t="n">
+        <v>3962</v>
+      </c>
+      <c r="H47" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>4274</t>
         </is>
       </c>
     </row>
@@ -1848,9 +2122,15 @@
       <c r="F48" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>3919</t>
+      <c r="G48" t="n">
+        <v>3919</v>
+      </c>
+      <c r="H48" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>4205</t>
         </is>
       </c>
     </row>
@@ -1879,9 +2159,15 @@
       <c r="F49" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>3381</t>
+      <c r="G49" t="n">
+        <v>3381</v>
+      </c>
+      <c r="H49" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>3394</t>
         </is>
       </c>
     </row>
@@ -1905,6 +2191,8 @@
       <c r="E50" t="inlineStr"/>
       <c r="F50" s="2" t="inlineStr"/>
       <c r="G50" t="inlineStr"/>
+      <c r="H50" s="2" t="inlineStr"/>
+      <c r="I50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -1926,6 +2214,8 @@
       <c r="E51" t="inlineStr"/>
       <c r="F51" s="2" t="inlineStr"/>
       <c r="G51" t="inlineStr"/>
+      <c r="H51" s="2" t="inlineStr"/>
+      <c r="I51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -1949,12 +2239,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F52" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>2485</t>
+      <c r="F52" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G52" t="n">
+        <v>2485</v>
+      </c>
+      <c r="H52" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>2537</t>
         </is>
       </c>
     </row>
@@ -1983,9 +2279,15 @@
       <c r="F53" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>2844</t>
+      <c r="G53" t="n">
+        <v>2844</v>
+      </c>
+      <c r="H53" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>2938</t>
         </is>
       </c>
     </row>
@@ -2011,12 +2313,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F54" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>2732</t>
+      <c r="F54" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" t="n">
+        <v>2732</v>
+      </c>
+      <c r="H54" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>2827</t>
         </is>
       </c>
     </row>
@@ -2045,9 +2353,15 @@
       <c r="F55" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>3825</t>
+      <c r="G55" t="n">
+        <v>3825</v>
+      </c>
+      <c r="H55" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>4062</t>
         </is>
       </c>
     </row>
@@ -2073,12 +2387,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F56" s="3" t="n">
+      <c r="F56" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>3267</t>
+      <c r="G56" t="n">
+        <v>3267</v>
+      </c>
+      <c r="H56" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>3378</t>
         </is>
       </c>
     </row>
@@ -2107,9 +2427,15 @@
       <c r="F57" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>3336</t>
+      <c r="G57" t="n">
+        <v>3336</v>
+      </c>
+      <c r="H57" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>3533</t>
         </is>
       </c>
     </row>
@@ -2138,9 +2464,15 @@
       <c r="F58" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>3438</t>
+      <c r="G58" t="n">
+        <v>3438</v>
+      </c>
+      <c r="H58" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>3721</t>
         </is>
       </c>
     </row>
@@ -2166,12 +2498,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F59" s="3" t="n">
+      <c r="F59" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>3237</t>
+      <c r="G59" t="n">
+        <v>3237</v>
+      </c>
+      <c r="H59" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>3459</t>
         </is>
       </c>
     </row>
@@ -2200,9 +2538,15 @@
       <c r="F60" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>3536</t>
+      <c r="G60" t="n">
+        <v>3536</v>
+      </c>
+      <c r="H60" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>3828</t>
         </is>
       </c>
     </row>
@@ -2228,10 +2572,16 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F61" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G61" t="inlineStr">
+      <c r="F61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" t="n">
+        <v>3153</v>
+      </c>
+      <c r="H61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I61" t="inlineStr">
         <is>
           <t>3153</t>
         </is>
@@ -2262,9 +2612,15 @@
       <c r="F62" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>3568</t>
+      <c r="G62" t="n">
+        <v>3568</v>
+      </c>
+      <c r="H62" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>3892</t>
         </is>
       </c>
     </row>
@@ -2290,10 +2646,16 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F63" s="4" t="n">
+      <c r="F63" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="G63" t="inlineStr">
+      <c r="G63" t="n">
+        <v>2898</v>
+      </c>
+      <c r="H63" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I63" t="inlineStr">
         <is>
           <t>2898</t>
         </is>
@@ -2324,9 +2686,15 @@
       <c r="F64" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>2759</t>
+      <c r="G64" t="n">
+        <v>2759</v>
+      </c>
+      <c r="H64" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>2909</t>
         </is>
       </c>
     </row>
@@ -2355,9 +2723,15 @@
       <c r="F65" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>3543</t>
+      <c r="G65" t="n">
+        <v>3543</v>
+      </c>
+      <c r="H65" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>3728</t>
         </is>
       </c>
     </row>
@@ -2383,12 +2757,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F66" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>2543</t>
+      <c r="F66" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G66" t="n">
+        <v>2543</v>
+      </c>
+      <c r="H66" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>2643</t>
         </is>
       </c>
     </row>
@@ -2417,9 +2797,15 @@
       <c r="F67" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>3739</t>
+      <c r="G67" t="n">
+        <v>3739</v>
+      </c>
+      <c r="H67" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>3960</t>
         </is>
       </c>
     </row>
@@ -2445,12 +2831,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F68" s="3" t="n">
+      <c r="F68" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>3388</t>
+      <c r="G68" t="n">
+        <v>3388</v>
+      </c>
+      <c r="H68" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>3519</t>
         </is>
       </c>
     </row>
@@ -2476,12 +2868,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F69" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>2816</t>
+      <c r="F69" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G69" t="n">
+        <v>2816</v>
+      </c>
+      <c r="H69" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>3152</t>
         </is>
       </c>
     </row>
@@ -2510,9 +2908,15 @@
       <c r="F70" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>3224</t>
+      <c r="G70" t="n">
+        <v>3224</v>
+      </c>
+      <c r="H70" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>3302</t>
         </is>
       </c>
     </row>
@@ -2538,12 +2942,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F71" s="4" t="n">
+      <c r="F71" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>3192</t>
+      <c r="G71" t="n">
+        <v>3192</v>
+      </c>
+      <c r="H71" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>3430</t>
         </is>
       </c>
     </row>
@@ -2569,12 +2979,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F72" s="3" t="n">
+      <c r="F72" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>3958</t>
+      <c r="G72" t="n">
+        <v>3958</v>
+      </c>
+      <c r="H72" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>3999</t>
         </is>
       </c>
     </row>
@@ -2603,9 +3019,15 @@
       <c r="F73" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>3238</t>
+      <c r="G73" t="n">
+        <v>3238</v>
+      </c>
+      <c r="H73" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>3306</t>
         </is>
       </c>
     </row>
@@ -2631,12 +3053,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F74" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>2842</t>
+      <c r="F74" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G74" t="n">
+        <v>2842</v>
+      </c>
+      <c r="H74" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>3177</t>
         </is>
       </c>
     </row>
@@ -2665,9 +3093,15 @@
       <c r="F75" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>3115</t>
+      <c r="G75" t="n">
+        <v>3115</v>
+      </c>
+      <c r="H75" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>3180</t>
         </is>
       </c>
     </row>
@@ -2696,9 +3130,15 @@
       <c r="F76" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="G76" t="inlineStr">
-        <is>
-          <t>3533</t>
+      <c r="G76" t="n">
+        <v>3533</v>
+      </c>
+      <c r="H76" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>3762</t>
         </is>
       </c>
     </row>
@@ -2727,9 +3167,15 @@
       <c r="F77" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>3734</t>
+      <c r="G77" t="n">
+        <v>3734</v>
+      </c>
+      <c r="H77" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>3996</t>
         </is>
       </c>
     </row>
@@ -2755,10 +3201,16 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F78" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G78" t="inlineStr">
+      <c r="F78" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G78" t="n">
+        <v>0</v>
+      </c>
+      <c r="H78" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2789,9 +3241,15 @@
       <c r="F79" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>3684</t>
+      <c r="G79" t="n">
+        <v>3684</v>
+      </c>
+      <c r="H79" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>3875</t>
         </is>
       </c>
     </row>
@@ -2820,9 +3278,15 @@
       <c r="F80" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="G80" t="inlineStr">
-        <is>
-          <t>3277</t>
+      <c r="G80" t="n">
+        <v>3277</v>
+      </c>
+      <c r="H80" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>3581</t>
         </is>
       </c>
     </row>
@@ -2851,9 +3315,15 @@
       <c r="F81" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>3494</t>
+      <c r="G81" t="n">
+        <v>3494</v>
+      </c>
+      <c r="H81" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>3701</t>
         </is>
       </c>
     </row>
@@ -2882,9 +3352,15 @@
       <c r="F82" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>3524</t>
+      <c r="G82" t="n">
+        <v>3524</v>
+      </c>
+      <c r="H82" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>3716</t>
         </is>
       </c>
     </row>
@@ -2910,12 +3386,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F83" s="3" t="n">
+      <c r="F83" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>3646</t>
+      <c r="G83" t="n">
+        <v>3646</v>
+      </c>
+      <c r="H83" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>3596</t>
         </is>
       </c>
     </row>
@@ -2944,9 +3426,15 @@
       <c r="F84" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>3361</t>
+      <c r="G84" t="n">
+        <v>3361</v>
+      </c>
+      <c r="H84" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>3540</t>
         </is>
       </c>
     </row>
@@ -2975,9 +3463,15 @@
       <c r="F85" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>3307</t>
+      <c r="G85" t="n">
+        <v>3307</v>
+      </c>
+      <c r="H85" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>3541</t>
         </is>
       </c>
     </row>
@@ -3006,9 +3500,15 @@
       <c r="F86" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>3036</t>
+      <c r="G86" t="n">
+        <v>3036</v>
+      </c>
+      <c r="H86" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>3146</t>
         </is>
       </c>
     </row>
@@ -3034,12 +3534,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F87" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G87" t="inlineStr">
-        <is>
-          <t>2719</t>
+      <c r="F87" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G87" t="n">
+        <v>2719</v>
+      </c>
+      <c r="H87" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>2990</t>
         </is>
       </c>
     </row>
@@ -3065,12 +3571,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F88" s="3" t="n">
+      <c r="F88" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G88" t="inlineStr">
-        <is>
-          <t>3440</t>
+      <c r="G88" t="n">
+        <v>3440</v>
+      </c>
+      <c r="H88" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>3561</t>
         </is>
       </c>
     </row>
@@ -3099,9 +3611,15 @@
       <c r="F89" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t>2712</t>
+      <c r="G89" t="n">
+        <v>2712</v>
+      </c>
+      <c r="H89" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>2770</t>
         </is>
       </c>
     </row>
@@ -3130,9 +3648,15 @@
       <c r="F90" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>2961</t>
+      <c r="G90" t="n">
+        <v>2961</v>
+      </c>
+      <c r="H90" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>3050</t>
         </is>
       </c>
     </row>
@@ -3158,12 +3682,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F91" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>1991</t>
+      <c r="F91" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G91" t="n">
+        <v>1991</v>
+      </c>
+      <c r="H91" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>2005</t>
         </is>
       </c>
     </row>
@@ -3192,9 +3722,15 @@
       <c r="F92" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>2625</t>
+      <c r="G92" t="n">
+        <v>2625</v>
+      </c>
+      <c r="H92" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>2707</t>
         </is>
       </c>
     </row>
@@ -3220,12 +3756,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F93" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>2633</t>
+      <c r="F93" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G93" t="n">
+        <v>2633</v>
+      </c>
+      <c r="H93" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>2711</t>
         </is>
       </c>
     </row>
@@ -3251,12 +3793,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F94" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G94" t="inlineStr">
-        <is>
-          <t>2306</t>
+      <c r="F94" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G94" t="n">
+        <v>2306</v>
+      </c>
+      <c r="H94" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>2286</t>
         </is>
       </c>
     </row>
@@ -3280,6 +3828,8 @@
       <c r="E95" t="inlineStr"/>
       <c r="F95" s="2" t="inlineStr"/>
       <c r="G95" t="inlineStr"/>
+      <c r="H95" s="2" t="inlineStr"/>
+      <c r="I95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -3303,12 +3853,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F96" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>2422</t>
+      <c r="F96" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G96" t="n">
+        <v>2422</v>
+      </c>
+      <c r="H96" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>2408</t>
         </is>
       </c>
     </row>
@@ -3334,12 +3890,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F97" s="4" t="n">
+      <c r="F97" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>2647</t>
+      <c r="G97" t="n">
+        <v>2647</v>
+      </c>
+      <c r="H97" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>2866</t>
         </is>
       </c>
     </row>
@@ -3368,9 +3930,15 @@
       <c r="F98" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>2913</t>
+      <c r="G98" t="n">
+        <v>2913</v>
+      </c>
+      <c r="H98" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>2988</t>
         </is>
       </c>
     </row>
@@ -3399,9 +3967,15 @@
       <c r="F99" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="G99" t="inlineStr">
-        <is>
-          <t>3398</t>
+      <c r="G99" t="n">
+        <v>3398</v>
+      </c>
+      <c r="H99" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>3601</t>
         </is>
       </c>
     </row>
@@ -3430,9 +4004,15 @@
       <c r="F100" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G100" t="inlineStr">
-        <is>
-          <t>3193</t>
+      <c r="G100" t="n">
+        <v>3193</v>
+      </c>
+      <c r="H100" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>3323</t>
         </is>
       </c>
     </row>
@@ -3461,9 +4041,15 @@
       <c r="F101" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="G101" t="inlineStr">
-        <is>
-          <t>2879</t>
+      <c r="G101" t="n">
+        <v>2879</v>
+      </c>
+      <c r="H101" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>2945</t>
         </is>
       </c>
     </row>
@@ -3492,9 +4078,15 @@
       <c r="F102" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="G102" t="inlineStr">
-        <is>
-          <t>3426</t>
+      <c r="G102" t="n">
+        <v>3426</v>
+      </c>
+      <c r="H102" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>3614</t>
         </is>
       </c>
     </row>
@@ -3520,12 +4112,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F103" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G103" t="inlineStr">
-        <is>
-          <t>3001</t>
+      <c r="F103" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G103" t="n">
+        <v>3001</v>
+      </c>
+      <c r="H103" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>3296</t>
         </is>
       </c>
     </row>
@@ -3551,12 +4149,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F104" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G104" t="inlineStr">
-        <is>
-          <t>2455</t>
+      <c r="F104" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G104" t="n">
+        <v>2455</v>
+      </c>
+      <c r="H104" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>2444</t>
         </is>
       </c>
     </row>
@@ -3585,9 +4189,15 @@
       <c r="F105" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G105" t="inlineStr">
-        <is>
-          <t>3287</t>
+      <c r="G105" t="n">
+        <v>3287</v>
+      </c>
+      <c r="H105" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>3420</t>
         </is>
       </c>
     </row>
@@ -3613,12 +4223,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F106" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G106" t="inlineStr">
-        <is>
-          <t>2992</t>
+      <c r="F106" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G106" t="n">
+        <v>2992</v>
+      </c>
+      <c r="H106" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>3236</t>
         </is>
       </c>
     </row>
@@ -3647,9 +4263,15 @@
       <c r="F107" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="G107" t="inlineStr">
-        <is>
-          <t>3005</t>
+      <c r="G107" t="n">
+        <v>3005</v>
+      </c>
+      <c r="H107" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>3072</t>
         </is>
       </c>
     </row>
@@ -3675,12 +4297,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F108" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G108" t="inlineStr">
-        <is>
-          <t>2547</t>
+      <c r="F108" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G108" t="n">
+        <v>2547</v>
+      </c>
+      <c r="H108" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>2603</t>
         </is>
       </c>
     </row>
@@ -3706,12 +4334,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F109" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G109" t="inlineStr">
-        <is>
-          <t>2806</t>
+      <c r="F109" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G109" t="n">
+        <v>2806</v>
+      </c>
+      <c r="H109" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>3100</t>
         </is>
       </c>
     </row>
@@ -3740,9 +4374,15 @@
       <c r="F110" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G110" t="inlineStr">
-        <is>
-          <t>2956</t>
+      <c r="G110" t="n">
+        <v>2956</v>
+      </c>
+      <c r="H110" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>3018</t>
         </is>
       </c>
     </row>
@@ -3768,12 +4408,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F111" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G111" t="inlineStr">
-        <is>
-          <t>3061</t>
+      <c r="F111" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G111" t="n">
+        <v>3061</v>
+      </c>
+      <c r="H111" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>3113</t>
         </is>
       </c>
     </row>
@@ -3799,12 +4445,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F112" s="4" t="n">
+      <c r="F112" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="G112" t="inlineStr">
-        <is>
-          <t>3164</t>
+      <c r="G112" t="n">
+        <v>3164</v>
+      </c>
+      <c r="H112" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>3377</t>
         </is>
       </c>
     </row>
@@ -3830,12 +4482,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F113" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G113" t="inlineStr">
-        <is>
-          <t>2501</t>
+      <c r="F113" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G113" t="n">
+        <v>2501</v>
+      </c>
+      <c r="H113" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>2514</t>
         </is>
       </c>
     </row>
@@ -3861,12 +4519,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F114" s="4" t="n">
+      <c r="F114" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="G114" t="inlineStr">
-        <is>
-          <t>2472</t>
+      <c r="G114" t="n">
+        <v>2472</v>
+      </c>
+      <c r="H114" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>2521</t>
         </is>
       </c>
     </row>
@@ -3895,9 +4559,15 @@
       <c r="F115" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="G115" t="inlineStr">
-        <is>
-          <t>3026</t>
+      <c r="G115" t="n">
+        <v>3026</v>
+      </c>
+      <c r="H115" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>3048</t>
         </is>
       </c>
     </row>
@@ -3923,12 +4593,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F116" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G116" t="inlineStr">
-        <is>
-          <t>2630</t>
+      <c r="F116" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G116" t="n">
+        <v>2630</v>
+      </c>
+      <c r="H116" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>2673</t>
         </is>
       </c>
     </row>
@@ -3957,9 +4633,15 @@
       <c r="F117" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="G117" t="inlineStr">
-        <is>
-          <t>2998</t>
+      <c r="G117" t="n">
+        <v>2998</v>
+      </c>
+      <c r="H117" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>3022</t>
         </is>
       </c>
     </row>
@@ -3988,9 +4670,15 @@
       <c r="F118" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G118" t="inlineStr">
-        <is>
-          <t>2615</t>
+      <c r="G118" t="n">
+        <v>2615</v>
+      </c>
+      <c r="H118" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>2808</t>
         </is>
       </c>
     </row>
@@ -4019,9 +4707,15 @@
       <c r="F119" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="G119" t="inlineStr">
-        <is>
-          <t>3054</t>
+      <c r="G119" t="n">
+        <v>3054</v>
+      </c>
+      <c r="H119" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>3197</t>
         </is>
       </c>
     </row>
@@ -4047,12 +4741,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F120" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G120" t="inlineStr">
-        <is>
-          <t>2548</t>
+      <c r="F120" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G120" t="n">
+        <v>2548</v>
+      </c>
+      <c r="H120" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>2640</t>
         </is>
       </c>
     </row>
@@ -4081,9 +4781,15 @@
       <c r="F121" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G121" t="inlineStr">
-        <is>
-          <t>2818</t>
+      <c r="G121" t="n">
+        <v>2818</v>
+      </c>
+      <c r="H121" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>2779</t>
         </is>
       </c>
     </row>
@@ -4112,9 +4818,15 @@
       <c r="F122" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G122" t="inlineStr">
-        <is>
-          <t>2817</t>
+      <c r="G122" t="n">
+        <v>2817</v>
+      </c>
+      <c r="H122" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I122" t="inlineStr">
+        <is>
+          <t>2855</t>
         </is>
       </c>
     </row>
@@ -4143,9 +4855,15 @@
       <c r="F123" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G123" t="inlineStr">
-        <is>
-          <t>3071</t>
+      <c r="G123" t="n">
+        <v>3071</v>
+      </c>
+      <c r="H123" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>3113</t>
         </is>
       </c>
     </row>
@@ -4174,9 +4892,15 @@
       <c r="F124" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G124" t="inlineStr">
-        <is>
-          <t>2843</t>
+      <c r="G124" t="n">
+        <v>2843</v>
+      </c>
+      <c r="H124" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>2881</t>
         </is>
       </c>
     </row>
@@ -4202,12 +4926,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F125" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G125" t="inlineStr">
-        <is>
-          <t>2158</t>
+      <c r="F125" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G125" t="n">
+        <v>2158</v>
+      </c>
+      <c r="H125" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I125" t="inlineStr">
+        <is>
+          <t>2146</t>
         </is>
       </c>
     </row>
@@ -4231,6 +4961,8 @@
       <c r="E126" t="inlineStr"/>
       <c r="F126" s="2" t="inlineStr"/>
       <c r="G126" t="inlineStr"/>
+      <c r="H126" s="2" t="inlineStr"/>
+      <c r="I126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" t="n">
@@ -4254,12 +4986,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F127" s="4" t="n">
+      <c r="F127" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="G127" t="inlineStr">
-        <is>
-          <t>2443</t>
+      <c r="G127" t="n">
+        <v>2443</v>
+      </c>
+      <c r="H127" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I127" t="inlineStr">
+        <is>
+          <t>2466</t>
         </is>
       </c>
     </row>
@@ -4288,9 +5026,15 @@
       <c r="F128" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G128" t="inlineStr">
-        <is>
-          <t>3446</t>
+      <c r="G128" t="n">
+        <v>3446</v>
+      </c>
+      <c r="H128" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="I128" t="inlineStr">
+        <is>
+          <t>3599</t>
         </is>
       </c>
     </row>
@@ -4314,6 +5058,8 @@
       <c r="E129" t="inlineStr"/>
       <c r="F129" s="2" t="inlineStr"/>
       <c r="G129" t="inlineStr"/>
+      <c r="H129" s="2" t="inlineStr"/>
+      <c r="I129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="n">
@@ -4337,12 +5083,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F130" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G130" t="inlineStr">
-        <is>
-          <t>2727</t>
+      <c r="F130" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G130" t="n">
+        <v>2727</v>
+      </c>
+      <c r="H130" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I130" t="inlineStr">
+        <is>
+          <t>2692</t>
         </is>
       </c>
     </row>
@@ -4368,12 +5120,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F131" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G131" t="inlineStr">
-        <is>
-          <t>2589</t>
+      <c r="F131" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G131" t="n">
+        <v>2589</v>
+      </c>
+      <c r="H131" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I131" t="inlineStr">
+        <is>
+          <t>2582</t>
         </is>
       </c>
     </row>
@@ -4402,9 +5160,15 @@
       <c r="F132" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G132" t="inlineStr">
-        <is>
-          <t>2896</t>
+      <c r="G132" t="n">
+        <v>2896</v>
+      </c>
+      <c r="H132" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I132" t="inlineStr">
+        <is>
+          <t>3099</t>
         </is>
       </c>
     </row>
@@ -4428,6 +5192,8 @@
       <c r="E133" t="inlineStr"/>
       <c r="F133" s="2" t="inlineStr"/>
       <c r="G133" t="inlineStr"/>
+      <c r="H133" s="2" t="inlineStr"/>
+      <c r="I133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="n">
@@ -4451,12 +5217,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F134" s="4" t="n">
+      <c r="F134" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="G134" t="inlineStr">
-        <is>
-          <t>2592</t>
+      <c r="G134" t="n">
+        <v>2592</v>
+      </c>
+      <c r="H134" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="I134" t="inlineStr">
+        <is>
+          <t>2584</t>
         </is>
       </c>
     </row>
@@ -4482,12 +5254,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F135" s="4" t="n">
+      <c r="F135" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="G135" t="inlineStr">
-        <is>
-          <t>2567</t>
+      <c r="G135" t="n">
+        <v>2567</v>
+      </c>
+      <c r="H135" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I135" t="inlineStr">
+        <is>
+          <t>2518</t>
         </is>
       </c>
     </row>
@@ -4513,12 +5291,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F136" s="4" t="n">
+      <c r="F136" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="G136" t="inlineStr">
-        <is>
-          <t>2520</t>
+      <c r="G136" t="n">
+        <v>2520</v>
+      </c>
+      <c r="H136" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I136" t="inlineStr">
+        <is>
+          <t>2534</t>
         </is>
       </c>
     </row>
@@ -4544,12 +5328,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F137" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G137" t="inlineStr">
-        <is>
-          <t>2050</t>
+      <c r="F137" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G137" t="n">
+        <v>2050</v>
+      </c>
+      <c r="H137" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I137" t="inlineStr">
+        <is>
+          <t>2080</t>
         </is>
       </c>
     </row>
@@ -4573,6 +5363,8 @@
       <c r="E138" t="inlineStr"/>
       <c r="F138" s="2" t="inlineStr"/>
       <c r="G138" t="inlineStr"/>
+      <c r="H138" s="2" t="inlineStr"/>
+      <c r="I138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -4594,6 +5386,8 @@
       <c r="E139" t="inlineStr"/>
       <c r="F139" s="2" t="inlineStr"/>
       <c r="G139" t="inlineStr"/>
+      <c r="H139" s="2" t="inlineStr"/>
+      <c r="I139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -4615,6 +5409,8 @@
       <c r="E140" t="inlineStr"/>
       <c r="F140" s="2" t="inlineStr"/>
       <c r="G140" t="inlineStr"/>
+      <c r="H140" s="2" t="inlineStr"/>
+      <c r="I140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="n">
@@ -4638,12 +5434,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F141" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G141" t="inlineStr">
-        <is>
-          <t>1979</t>
+      <c r="F141" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G141" t="n">
+        <v>1979</v>
+      </c>
+      <c r="H141" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I141" t="inlineStr">
+        <is>
+          <t>1991</t>
         </is>
       </c>
     </row>
@@ -4667,6 +5469,8 @@
       <c r="E142" t="inlineStr"/>
       <c r="F142" s="2" t="inlineStr"/>
       <c r="G142" t="inlineStr"/>
+      <c r="H142" s="2" t="inlineStr"/>
+      <c r="I142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="n">
@@ -4688,6 +5492,8 @@
       <c r="E143" t="inlineStr"/>
       <c r="F143" s="2" t="inlineStr"/>
       <c r="G143" t="inlineStr"/>
+      <c r="H143" s="2" t="inlineStr"/>
+      <c r="I143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -4709,6 +5515,8 @@
       <c r="E144" t="inlineStr"/>
       <c r="F144" s="2" t="inlineStr"/>
       <c r="G144" t="inlineStr"/>
+      <c r="H144" s="2" t="inlineStr"/>
+      <c r="I144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -4730,6 +5538,8 @@
       <c r="E145" t="inlineStr"/>
       <c r="F145" s="2" t="inlineStr"/>
       <c r="G145" t="inlineStr"/>
+      <c r="H145" s="2" t="inlineStr"/>
+      <c r="I145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -4751,6 +5561,8 @@
       <c r="E146" t="inlineStr"/>
       <c r="F146" s="2" t="inlineStr"/>
       <c r="G146" t="inlineStr"/>
+      <c r="H146" s="2" t="inlineStr"/>
+      <c r="I146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -4772,6 +5584,8 @@
       <c r="E147" t="inlineStr"/>
       <c r="F147" s="2" t="inlineStr"/>
       <c r="G147" t="inlineStr"/>
+      <c r="H147" s="2" t="inlineStr"/>
+      <c r="I147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -4793,6 +5607,8 @@
       <c r="E148" t="inlineStr"/>
       <c r="F148" s="2" t="inlineStr"/>
       <c r="G148" t="inlineStr"/>
+      <c r="H148" s="2" t="inlineStr"/>
+      <c r="I148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="n">
@@ -4814,6 +5630,8 @@
       <c r="E149" t="inlineStr"/>
       <c r="F149" s="2" t="inlineStr"/>
       <c r="G149" t="inlineStr"/>
+      <c r="H149" s="2" t="inlineStr"/>
+      <c r="I149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="n">
@@ -4835,6 +5653,8 @@
       <c r="E150" t="inlineStr"/>
       <c r="F150" s="2" t="inlineStr"/>
       <c r="G150" t="inlineStr"/>
+      <c r="H150" s="2" t="inlineStr"/>
+      <c r="I150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="n">
@@ -4856,6 +5676,8 @@
       <c r="E151" t="inlineStr"/>
       <c r="F151" s="2" t="inlineStr"/>
       <c r="G151" t="inlineStr"/>
+      <c r="H151" s="2" t="inlineStr"/>
+      <c r="I151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="n">
@@ -4877,6 +5699,8 @@
       <c r="E152" t="inlineStr"/>
       <c r="F152" s="2" t="inlineStr"/>
       <c r="G152" t="inlineStr"/>
+      <c r="H152" s="2" t="inlineStr"/>
+      <c r="I152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" t="n">
@@ -4898,6 +5722,8 @@
       <c r="E153" t="inlineStr"/>
       <c r="F153" s="2" t="inlineStr"/>
       <c r="G153" t="inlineStr"/>
+      <c r="H153" s="2" t="inlineStr"/>
+      <c r="I153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" t="n">
@@ -4921,12 +5747,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F154" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G154" t="inlineStr">
-        <is>
-          <t>1639</t>
+      <c r="F154" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G154" t="n">
+        <v>1639</v>
+      </c>
+      <c r="H154" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="I154" t="inlineStr">
+        <is>
+          <t>1830</t>
         </is>
       </c>
     </row>
@@ -4950,6 +5782,8 @@
       <c r="E155" t="inlineStr"/>
       <c r="F155" s="2" t="inlineStr"/>
       <c r="G155" t="inlineStr"/>
+      <c r="H155" s="2" t="inlineStr"/>
+      <c r="I155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="n">
@@ -4973,10 +5807,16 @@
           <t>Chinese</t>
         </is>
       </c>
-      <c r="F156" s="4" t="n">
+      <c r="F156" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="G156" t="inlineStr">
+      <c r="G156" t="n">
+        <v>3003</v>
+      </c>
+      <c r="H156" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I156" t="inlineStr">
         <is>
           <t>3003</t>
         </is>
@@ -5004,10 +5844,16 @@
           <t>Chinese</t>
         </is>
       </c>
-      <c r="F157" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G157" t="inlineStr">
+      <c r="F157" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G157" t="n">
+        <v>0</v>
+      </c>
+      <c r="H157" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I157" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5035,10 +5881,16 @@
           <t>Chinese</t>
         </is>
       </c>
-      <c r="F158" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G158" t="inlineStr">
+      <c r="F158" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G158" t="n">
+        <v>0</v>
+      </c>
+      <c r="H158" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5066,12 +5918,18 @@
           <t>Chinese</t>
         </is>
       </c>
-      <c r="F159" s="4" t="n">
+      <c r="F159" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="G159" t="inlineStr">
-        <is>
-          <t>3382</t>
+      <c r="G159" t="n">
+        <v>3382</v>
+      </c>
+      <c r="H159" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="I159" t="inlineStr">
+        <is>
+          <t>3542</t>
         </is>
       </c>
     </row>
@@ -5097,10 +5955,16 @@
           <t>Chinese</t>
         </is>
       </c>
-      <c r="F160" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G160" t="inlineStr">
+      <c r="F160" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G160" t="n">
+        <v>0</v>
+      </c>
+      <c r="H160" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I160" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5128,12 +5992,18 @@
           <t>Chinese</t>
         </is>
       </c>
-      <c r="F161" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G161" t="inlineStr">
-        <is>
-          <t>2630</t>
+      <c r="F161" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G161" t="n">
+        <v>2630</v>
+      </c>
+      <c r="H161" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I161" t="inlineStr">
+        <is>
+          <t>2645</t>
         </is>
       </c>
     </row>
@@ -5159,10 +6029,16 @@
           <t>Chinese</t>
         </is>
       </c>
-      <c r="F162" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G162" t="inlineStr">
+      <c r="F162" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G162" t="n">
+        <v>0</v>
+      </c>
+      <c r="H162" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I162" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5190,20 +6066,24 @@
           <t>Chinese</t>
         </is>
       </c>
-      <c r="F163" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G163" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="F163" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G163" t="n">
+        <v>0</v>
+      </c>
+      <c r="H163" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I163" t="inlineStr">
+        <is>
+          <t>2526</t>
         </is>
       </c>
     </row>
     <row r="164">
-      <c r="A164" t="inlineStr">
-        <is>
-          <t>9321819</t>
-        </is>
+      <c r="A164" t="n">
+        <v>9321819</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
@@ -5217,20 +6097,24 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F164" s="4" t="n">
+      <c r="F164" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="G164" t="inlineStr">
-        <is>
-          <t>2605</t>
+      <c r="G164" t="n">
+        <v>2605</v>
+      </c>
+      <c r="H164" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="I164" t="inlineStr">
+        <is>
+          <t>2738</t>
         </is>
       </c>
     </row>
     <row r="165">
-      <c r="A165" t="inlineStr">
-        <is>
-          <t>58615957</t>
-        </is>
+      <c r="A165" t="n">
+        <v>58615957</v>
       </c>
       <c r="B165" t="inlineStr">
         <is>
@@ -5247,17 +6131,21 @@
       <c r="F165" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G165" t="inlineStr">
-        <is>
-          <t>1635</t>
+      <c r="G165" t="n">
+        <v>1635</v>
+      </c>
+      <c r="H165" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I165" t="inlineStr">
+        <is>
+          <t>1951</t>
         </is>
       </c>
     </row>
     <row r="166">
-      <c r="A166" t="inlineStr">
-        <is>
-          <t>47928278</t>
-        </is>
+      <c r="A166" t="n">
+        <v>47928278</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>
@@ -5271,20 +6159,24 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F166" s="3" t="n">
+      <c r="F166" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="G166" t="inlineStr">
-        <is>
-          <t>4137</t>
+      <c r="G166" t="n">
+        <v>4137</v>
+      </c>
+      <c r="H166" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="I166" t="inlineStr">
+        <is>
+          <t>4475</t>
         </is>
       </c>
     </row>
     <row r="167">
-      <c r="A167" t="inlineStr">
-        <is>
-          <t>54134515</t>
-        </is>
+      <c r="A167" t="n">
+        <v>54134515</v>
       </c>
       <c r="B167" t="inlineStr">
         <is>
@@ -5298,20 +6190,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F167" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G167" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="F167" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G167" t="n">
+        <v>0</v>
+      </c>
+      <c r="H167" s="2" t="inlineStr"/>
+      <c r="I167" t="inlineStr"/>
     </row>
     <row r="168">
-      <c r="A168" t="inlineStr">
-        <is>
-          <t>54924790</t>
-        </is>
+      <c r="A168" t="n">
+        <v>54924790</v>
       </c>
       <c r="B168" t="inlineStr">
         <is>
@@ -5325,20 +6215,24 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F168" s="4" t="n">
+      <c r="F168" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="G168" t="inlineStr">
-        <is>
-          <t>2877</t>
+      <c r="G168" t="n">
+        <v>2877</v>
+      </c>
+      <c r="H168" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="I168" t="inlineStr">
+        <is>
+          <t>2990</t>
         </is>
       </c>
     </row>
     <row r="169">
-      <c r="A169" t="inlineStr">
-        <is>
-          <t>56265168</t>
-        </is>
+      <c r="A169" t="n">
+        <v>56265168</v>
       </c>
       <c r="B169" t="inlineStr">
         <is>
@@ -5355,17 +6249,21 @@
       <c r="F169" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="G169" t="inlineStr">
-        <is>
-          <t>2675</t>
+      <c r="G169" t="n">
+        <v>2675</v>
+      </c>
+      <c r="H169" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="I169" t="inlineStr">
+        <is>
+          <t>2752</t>
         </is>
       </c>
     </row>
     <row r="170">
-      <c r="A170" t="inlineStr">
-        <is>
-          <t>58615925</t>
-        </is>
+      <c r="A170" t="n">
+        <v>58615925</v>
       </c>
       <c r="B170" t="inlineStr">
         <is>
@@ -5382,9 +6280,73 @@
       <c r="F170" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G170" t="inlineStr">
-        <is>
-          <t>1861</t>
+      <c r="G170" t="n">
+        <v>1861</v>
+      </c>
+      <c r="H170" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I170" t="inlineStr">
+        <is>
+          <t>2131</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>27113069</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>㊥DumbSmoky</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr"/>
+      <c r="D171" t="inlineStr"/>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F171" s="2" t="inlineStr"/>
+      <c r="G171" t="inlineStr"/>
+      <c r="H171" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="I171" t="inlineStr">
+        <is>
+          <t>4138</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>47533851</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>Bibek</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr"/>
+      <c r="D172" t="inlineStr"/>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F172" s="2" t="inlineStr"/>
+      <c r="G172" t="inlineStr"/>
+      <c r="H172" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="I172" t="inlineStr">
+        <is>
+          <t>2053</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-01-21 11:32:09
</commit_message>
<xml_diff>
--- a/Season_Attack/82.xlsx
+++ b/Season_Attack/82.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I172"/>
+  <dimension ref="A1:K177"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,6 +436,16 @@
           <t>01-19_0</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>01-20_A</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>01-20_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -468,9 +478,15 @@
       <c r="H2" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>3336</t>
+      <c r="I2" t="n">
+        <v>3336</v>
+      </c>
+      <c r="J2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>3426</t>
         </is>
       </c>
     </row>
@@ -505,9 +521,15 @@
       <c r="H3" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>4143</t>
+      <c r="I3" t="n">
+        <v>4143</v>
+      </c>
+      <c r="J3" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>4359</t>
         </is>
       </c>
     </row>
@@ -542,9 +564,15 @@
       <c r="H4" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>3764</t>
+      <c r="I4" t="n">
+        <v>3764</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>4118</t>
         </is>
       </c>
     </row>
@@ -579,9 +607,15 @@
       <c r="H5" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>3795</t>
+      <c r="I5" t="n">
+        <v>3795</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>4146</t>
         </is>
       </c>
     </row>
@@ -604,7 +638,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F6" s="4" t="n">
@@ -616,9 +650,15 @@
       <c r="H6" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>4120</t>
+      <c r="I6" t="n">
+        <v>4120</v>
+      </c>
+      <c r="J6" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>4502</t>
         </is>
       </c>
     </row>
@@ -653,9 +693,15 @@
       <c r="H7" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>3923</t>
+      <c r="I7" t="n">
+        <v>3923</v>
+      </c>
+      <c r="J7" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>4096</t>
         </is>
       </c>
     </row>
@@ -690,9 +736,15 @@
       <c r="H8" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>3605</t>
+      <c r="I8" t="n">
+        <v>3605</v>
+      </c>
+      <c r="J8" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>3770</t>
         </is>
       </c>
     </row>
@@ -718,6 +770,8 @@
       <c r="G9" t="inlineStr"/>
       <c r="H9" s="2" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
+      <c r="J9" s="2" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -738,7 +792,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F10" s="4" t="n">
@@ -750,9 +804,15 @@
       <c r="H10" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>3932</t>
+      <c r="I10" t="n">
+        <v>3932</v>
+      </c>
+      <c r="J10" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>4243</t>
         </is>
       </c>
     </row>
@@ -787,9 +847,15 @@
       <c r="H11" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>3960</t>
+      <c r="I11" t="n">
+        <v>3960</v>
+      </c>
+      <c r="J11" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>4476</t>
         </is>
       </c>
     </row>
@@ -812,7 +878,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F12" s="2" t="n">
@@ -824,9 +890,15 @@
       <c r="H12" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>3740</t>
+      <c r="I12" t="n">
+        <v>3740</v>
+      </c>
+      <c r="J12" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>3930</t>
         </is>
       </c>
     </row>
@@ -861,9 +933,15 @@
       <c r="H13" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>2682</t>
+      <c r="I13" t="n">
+        <v>2682</v>
+      </c>
+      <c r="J13" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>2729</t>
         </is>
       </c>
     </row>
@@ -898,9 +976,15 @@
       <c r="H14" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>4586</t>
+      <c r="I14" t="n">
+        <v>4586</v>
+      </c>
+      <c r="J14" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>5024</t>
         </is>
       </c>
     </row>
@@ -935,9 +1019,15 @@
       <c r="H15" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>4023</t>
+      <c r="I15" t="n">
+        <v>4023</v>
+      </c>
+      <c r="J15" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>4287</t>
         </is>
       </c>
     </row>
@@ -960,7 +1050,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F16" s="4" t="n">
@@ -972,9 +1062,15 @@
       <c r="H16" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>4335</t>
+      <c r="I16" t="n">
+        <v>4335</v>
+      </c>
+      <c r="J16" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>4557</t>
         </is>
       </c>
     </row>
@@ -1009,9 +1105,15 @@
       <c r="H17" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>3837</t>
+      <c r="I17" t="n">
+        <v>3837</v>
+      </c>
+      <c r="J17" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>3963</t>
         </is>
       </c>
     </row>
@@ -1046,9 +1148,15 @@
       <c r="H18" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>3609</t>
+      <c r="I18" t="n">
+        <v>3609</v>
+      </c>
+      <c r="J18" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>3971</t>
         </is>
       </c>
     </row>
@@ -1071,7 +1179,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F19" s="4" t="n">
@@ -1083,9 +1191,15 @@
       <c r="H19" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>4525</t>
+      <c r="I19" t="n">
+        <v>4525</v>
+      </c>
+      <c r="J19" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>4777</t>
         </is>
       </c>
     </row>
@@ -1120,9 +1234,15 @@
       <c r="H20" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>3720</t>
+      <c r="I20" t="n">
+        <v>3720</v>
+      </c>
+      <c r="J20" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>3870</t>
         </is>
       </c>
     </row>
@@ -1157,9 +1277,15 @@
       <c r="H21" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>4068</t>
+      <c r="I21" t="n">
+        <v>4068</v>
+      </c>
+      <c r="J21" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>4280</t>
         </is>
       </c>
     </row>
@@ -1194,9 +1320,15 @@
       <c r="H22" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>2745</t>
+      <c r="I22" t="n">
+        <v>2745</v>
+      </c>
+      <c r="J22" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>3060</t>
         </is>
       </c>
     </row>
@@ -1219,7 +1351,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F23" s="4" t="n">
@@ -1231,9 +1363,15 @@
       <c r="H23" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>3916</t>
+      <c r="I23" t="n">
+        <v>3916</v>
+      </c>
+      <c r="J23" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>4274</t>
         </is>
       </c>
     </row>
@@ -1268,7 +1406,13 @@
       <c r="H24" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I24" t="inlineStr">
+      <c r="I24" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1305,9 +1449,15 @@
       <c r="H25" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>4027</t>
+      <c r="I25" t="n">
+        <v>4027</v>
+      </c>
+      <c r="J25" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>4317</t>
         </is>
       </c>
     </row>
@@ -1330,7 +1480,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F26" s="4" t="n">
@@ -1342,9 +1492,15 @@
       <c r="H26" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>4308</t>
+      <c r="I26" t="n">
+        <v>4308</v>
+      </c>
+      <c r="J26" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>4499</t>
         </is>
       </c>
     </row>
@@ -1379,9 +1535,15 @@
       <c r="H27" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>3503</t>
+      <c r="I27" t="n">
+        <v>3503</v>
+      </c>
+      <c r="J27" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>3732</t>
         </is>
       </c>
     </row>
@@ -1416,9 +1578,15 @@
       <c r="H28" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>4424</t>
+      <c r="I28" t="n">
+        <v>4424</v>
+      </c>
+      <c r="J28" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>4772</t>
         </is>
       </c>
     </row>
@@ -1453,9 +1621,15 @@
       <c r="H29" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>4068</t>
+      <c r="I29" t="n">
+        <v>4068</v>
+      </c>
+      <c r="J29" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>4258</t>
         </is>
       </c>
     </row>
@@ -1490,9 +1664,15 @@
       <c r="H30" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>4341</t>
+      <c r="I30" t="n">
+        <v>4341</v>
+      </c>
+      <c r="J30" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>4646</t>
         </is>
       </c>
     </row>
@@ -1527,9 +1707,15 @@
       <c r="H31" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>4464</t>
+      <c r="I31" t="n">
+        <v>4464</v>
+      </c>
+      <c r="J31" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>4589</t>
         </is>
       </c>
     </row>
@@ -1564,7 +1750,13 @@
       <c r="H32" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="I32" t="inlineStr">
+      <c r="I32" t="n">
+        <v>2813</v>
+      </c>
+      <c r="J32" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K32" t="inlineStr">
         <is>
           <t>2813</t>
         </is>
@@ -1601,9 +1793,15 @@
       <c r="H33" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>4227</t>
+      <c r="I33" t="n">
+        <v>4227</v>
+      </c>
+      <c r="J33" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>4487</t>
         </is>
       </c>
     </row>
@@ -1638,9 +1836,15 @@
       <c r="H34" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I34" t="inlineStr">
-        <is>
-          <t>3803</t>
+      <c r="I34" t="n">
+        <v>3803</v>
+      </c>
+      <c r="J34" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>4141</t>
         </is>
       </c>
     </row>
@@ -1675,9 +1879,15 @@
       <c r="H35" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>3753</t>
+      <c r="I35" t="n">
+        <v>3753</v>
+      </c>
+      <c r="J35" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>4020</t>
         </is>
       </c>
     </row>
@@ -1703,6 +1913,8 @@
       <c r="G36" t="inlineStr"/>
       <c r="H36" s="2" t="inlineStr"/>
       <c r="I36" t="inlineStr"/>
+      <c r="J36" s="2" t="inlineStr"/>
+      <c r="K36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -1735,9 +1947,15 @@
       <c r="H37" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>4054</t>
+      <c r="I37" t="n">
+        <v>4054</v>
+      </c>
+      <c r="J37" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>4304</t>
         </is>
       </c>
     </row>
@@ -1772,9 +1990,15 @@
       <c r="H38" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>3883</t>
+      <c r="I38" t="n">
+        <v>3883</v>
+      </c>
+      <c r="J38" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>4109</t>
         </is>
       </c>
     </row>
@@ -1797,7 +2021,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F39" s="4" t="n">
@@ -1809,9 +2033,15 @@
       <c r="H39" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>4642</t>
+      <c r="I39" t="n">
+        <v>4642</v>
+      </c>
+      <c r="J39" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>4826</t>
         </is>
       </c>
     </row>
@@ -1846,9 +2076,15 @@
       <c r="H40" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>3886</t>
+      <c r="I40" t="n">
+        <v>3886</v>
+      </c>
+      <c r="J40" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>4216</t>
         </is>
       </c>
     </row>
@@ -1883,9 +2119,15 @@
       <c r="H41" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="I41" t="inlineStr">
-        <is>
-          <t>4430</t>
+      <c r="I41" t="n">
+        <v>4430</v>
+      </c>
+      <c r="J41" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>4759</t>
         </is>
       </c>
     </row>
@@ -1920,9 +2162,15 @@
       <c r="H42" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>4198</t>
+      <c r="I42" t="n">
+        <v>4198</v>
+      </c>
+      <c r="J42" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>4433</t>
         </is>
       </c>
     </row>
@@ -1948,6 +2196,8 @@
       <c r="G43" t="inlineStr"/>
       <c r="H43" s="2" t="inlineStr"/>
       <c r="I43" t="inlineStr"/>
+      <c r="J43" s="2" t="inlineStr"/>
+      <c r="K43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -1980,9 +2230,15 @@
       <c r="H44" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>3724</t>
+      <c r="I44" t="n">
+        <v>3724</v>
+      </c>
+      <c r="J44" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>4001</t>
         </is>
       </c>
     </row>
@@ -2017,11 +2273,11 @@
       <c r="H45" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I45" t="inlineStr">
-        <is>
-          <t>3744</t>
-        </is>
-      </c>
+      <c r="I45" t="n">
+        <v>3744</v>
+      </c>
+      <c r="J45" s="2" t="inlineStr"/>
+      <c r="K45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -2054,9 +2310,15 @@
       <c r="H46" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I46" t="inlineStr">
-        <is>
-          <t>2662</t>
+      <c r="I46" t="n">
+        <v>2662</v>
+      </c>
+      <c r="J46" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>3069</t>
         </is>
       </c>
     </row>
@@ -2091,9 +2353,15 @@
       <c r="H47" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="I47" t="inlineStr">
-        <is>
-          <t>4274</t>
+      <c r="I47" t="n">
+        <v>4274</v>
+      </c>
+      <c r="J47" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>4537</t>
         </is>
       </c>
     </row>
@@ -2128,9 +2396,15 @@
       <c r="H48" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>4205</t>
+      <c r="I48" t="n">
+        <v>4205</v>
+      </c>
+      <c r="J48" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>4475</t>
         </is>
       </c>
     </row>
@@ -2165,7 +2439,13 @@
       <c r="H49" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I49" t="inlineStr">
+      <c r="I49" t="n">
+        <v>3394</v>
+      </c>
+      <c r="J49" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K49" t="inlineStr">
         <is>
           <t>3394</t>
         </is>
@@ -2193,6 +2473,8 @@
       <c r="G50" t="inlineStr"/>
       <c r="H50" s="2" t="inlineStr"/>
       <c r="I50" t="inlineStr"/>
+      <c r="J50" s="2" t="inlineStr"/>
+      <c r="K50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -2216,6 +2498,8 @@
       <c r="G51" t="inlineStr"/>
       <c r="H51" s="2" t="inlineStr"/>
       <c r="I51" t="inlineStr"/>
+      <c r="J51" s="2" t="inlineStr"/>
+      <c r="K51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -2248,9 +2532,15 @@
       <c r="H52" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>2537</t>
+      <c r="I52" t="n">
+        <v>2537</v>
+      </c>
+      <c r="J52" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>2535</t>
         </is>
       </c>
     </row>
@@ -2285,9 +2575,15 @@
       <c r="H53" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I53" t="inlineStr">
-        <is>
-          <t>2938</t>
+      <c r="I53" t="n">
+        <v>2938</v>
+      </c>
+      <c r="J53" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>3072</t>
         </is>
       </c>
     </row>
@@ -2322,9 +2618,15 @@
       <c r="H54" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="I54" t="inlineStr">
-        <is>
-          <t>2827</t>
+      <c r="I54" t="n">
+        <v>2827</v>
+      </c>
+      <c r="J54" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>2864</t>
         </is>
       </c>
     </row>
@@ -2359,9 +2661,15 @@
       <c r="H55" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="I55" t="inlineStr">
-        <is>
-          <t>4062</t>
+      <c r="I55" t="n">
+        <v>4062</v>
+      </c>
+      <c r="J55" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>4341</t>
         </is>
       </c>
     </row>
@@ -2396,9 +2704,15 @@
       <c r="H56" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I56" t="inlineStr">
-        <is>
-          <t>3378</t>
+      <c r="I56" t="n">
+        <v>3378</v>
+      </c>
+      <c r="J56" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>3585</t>
         </is>
       </c>
     </row>
@@ -2433,9 +2747,15 @@
       <c r="H57" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I57" t="inlineStr">
-        <is>
-          <t>3533</t>
+      <c r="I57" t="n">
+        <v>3533</v>
+      </c>
+      <c r="J57" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>3644</t>
         </is>
       </c>
     </row>
@@ -2470,9 +2790,15 @@
       <c r="H58" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I58" t="inlineStr">
-        <is>
-          <t>3721</t>
+      <c r="I58" t="n">
+        <v>3721</v>
+      </c>
+      <c r="J58" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>4005</t>
         </is>
       </c>
     </row>
@@ -2507,9 +2833,15 @@
       <c r="H59" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I59" t="inlineStr">
-        <is>
-          <t>3459</t>
+      <c r="I59" t="n">
+        <v>3459</v>
+      </c>
+      <c r="J59" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>3720</t>
         </is>
       </c>
     </row>
@@ -2544,9 +2876,15 @@
       <c r="H60" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I60" t="inlineStr">
-        <is>
-          <t>3828</t>
+      <c r="I60" t="n">
+        <v>3828</v>
+      </c>
+      <c r="J60" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>4075</t>
         </is>
       </c>
     </row>
@@ -2581,7 +2919,13 @@
       <c r="H61" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I61" t="inlineStr">
+      <c r="I61" t="n">
+        <v>3153</v>
+      </c>
+      <c r="J61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K61" t="inlineStr">
         <is>
           <t>3153</t>
         </is>
@@ -2618,9 +2962,15 @@
       <c r="H62" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="I62" t="inlineStr">
-        <is>
-          <t>3892</t>
+      <c r="I62" t="n">
+        <v>3892</v>
+      </c>
+      <c r="J62" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>4151</t>
         </is>
       </c>
     </row>
@@ -2655,7 +3005,13 @@
       <c r="H63" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I63" t="inlineStr">
+      <c r="I63" t="n">
+        <v>2898</v>
+      </c>
+      <c r="J63" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K63" t="inlineStr">
         <is>
           <t>2898</t>
         </is>
@@ -2692,9 +3048,15 @@
       <c r="H64" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I64" t="inlineStr">
-        <is>
-          <t>2909</t>
+      <c r="I64" t="n">
+        <v>2909</v>
+      </c>
+      <c r="J64" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>2956</t>
         </is>
       </c>
     </row>
@@ -2729,9 +3091,15 @@
       <c r="H65" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="I65" t="inlineStr">
-        <is>
-          <t>3728</t>
+      <c r="I65" t="n">
+        <v>3728</v>
+      </c>
+      <c r="J65" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>4058</t>
         </is>
       </c>
     </row>
@@ -2766,9 +3134,15 @@
       <c r="H66" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I66" t="inlineStr">
-        <is>
-          <t>2643</t>
+      <c r="I66" t="n">
+        <v>2643</v>
+      </c>
+      <c r="J66" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>2671</t>
         </is>
       </c>
     </row>
@@ -2803,9 +3177,15 @@
       <c r="H67" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="I67" t="inlineStr">
-        <is>
-          <t>3960</t>
+      <c r="I67" t="n">
+        <v>3960</v>
+      </c>
+      <c r="J67" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>4281</t>
         </is>
       </c>
     </row>
@@ -2840,9 +3220,15 @@
       <c r="H68" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I68" t="inlineStr">
-        <is>
-          <t>3519</t>
+      <c r="I68" t="n">
+        <v>3519</v>
+      </c>
+      <c r="J68" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>3626</t>
         </is>
       </c>
     </row>
@@ -2877,9 +3263,15 @@
       <c r="H69" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I69" t="inlineStr">
-        <is>
-          <t>3152</t>
+      <c r="I69" t="n">
+        <v>3152</v>
+      </c>
+      <c r="J69" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>3223</t>
         </is>
       </c>
     </row>
@@ -2914,9 +3306,15 @@
       <c r="H70" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="I70" t="inlineStr">
-        <is>
-          <t>3302</t>
+      <c r="I70" t="n">
+        <v>3302</v>
+      </c>
+      <c r="J70" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>3587</t>
         </is>
       </c>
     </row>
@@ -2951,9 +3349,15 @@
       <c r="H71" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="I71" t="inlineStr">
-        <is>
-          <t>3430</t>
+      <c r="I71" t="n">
+        <v>3430</v>
+      </c>
+      <c r="J71" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>3368</t>
         </is>
       </c>
     </row>
@@ -2988,9 +3392,15 @@
       <c r="H72" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I72" t="inlineStr">
-        <is>
-          <t>3999</t>
+      <c r="I72" t="n">
+        <v>3999</v>
+      </c>
+      <c r="J72" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>4158</t>
         </is>
       </c>
     </row>
@@ -3025,9 +3435,15 @@
       <c r="H73" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I73" t="inlineStr">
-        <is>
-          <t>3306</t>
+      <c r="I73" t="n">
+        <v>3306</v>
+      </c>
+      <c r="J73" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>3541</t>
         </is>
       </c>
     </row>
@@ -3062,9 +3478,15 @@
       <c r="H74" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I74" t="inlineStr">
-        <is>
-          <t>3177</t>
+      <c r="I74" t="n">
+        <v>3177</v>
+      </c>
+      <c r="J74" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>3322</t>
         </is>
       </c>
     </row>
@@ -3099,9 +3521,15 @@
       <c r="H75" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="I75" t="inlineStr">
-        <is>
-          <t>3180</t>
+      <c r="I75" t="n">
+        <v>3180</v>
+      </c>
+      <c r="J75" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>3281</t>
         </is>
       </c>
     </row>
@@ -3124,7 +3552,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F76" s="2" t="n">
@@ -3136,9 +3564,15 @@
       <c r="H76" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="I76" t="inlineStr">
-        <is>
-          <t>3762</t>
+      <c r="I76" t="n">
+        <v>3762</v>
+      </c>
+      <c r="J76" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>3784</t>
         </is>
       </c>
     </row>
@@ -3173,9 +3607,15 @@
       <c r="H77" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I77" t="inlineStr">
-        <is>
-          <t>3996</t>
+      <c r="I77" t="n">
+        <v>3996</v>
+      </c>
+      <c r="J77" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>4236</t>
         </is>
       </c>
     </row>
@@ -3210,7 +3650,13 @@
       <c r="H78" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I78" t="inlineStr">
+      <c r="I78" t="n">
+        <v>0</v>
+      </c>
+      <c r="J78" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3247,9 +3693,15 @@
       <c r="H79" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="I79" t="inlineStr">
-        <is>
-          <t>3875</t>
+      <c r="I79" t="n">
+        <v>3875</v>
+      </c>
+      <c r="J79" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>3967</t>
         </is>
       </c>
     </row>
@@ -3284,9 +3736,15 @@
       <c r="H80" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I80" t="inlineStr">
-        <is>
-          <t>3581</t>
+      <c r="I80" t="n">
+        <v>3581</v>
+      </c>
+      <c r="J80" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>3604</t>
         </is>
       </c>
     </row>
@@ -3321,9 +3779,15 @@
       <c r="H81" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="I81" t="inlineStr">
-        <is>
-          <t>3701</t>
+      <c r="I81" t="n">
+        <v>3701</v>
+      </c>
+      <c r="J81" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>3716</t>
         </is>
       </c>
     </row>
@@ -3358,9 +3822,15 @@
       <c r="H82" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I82" t="inlineStr">
-        <is>
-          <t>3716</t>
+      <c r="I82" t="n">
+        <v>3716</v>
+      </c>
+      <c r="J82" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>3902</t>
         </is>
       </c>
     </row>
@@ -3395,9 +3865,15 @@
       <c r="H83" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="I83" t="inlineStr">
-        <is>
-          <t>3596</t>
+      <c r="I83" t="n">
+        <v>3596</v>
+      </c>
+      <c r="J83" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>3719</t>
         </is>
       </c>
     </row>
@@ -3432,9 +3908,15 @@
       <c r="H84" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="I84" t="inlineStr">
-        <is>
-          <t>3540</t>
+      <c r="I84" t="n">
+        <v>3540</v>
+      </c>
+      <c r="J84" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>3672</t>
         </is>
       </c>
     </row>
@@ -3469,9 +3951,15 @@
       <c r="H85" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I85" t="inlineStr">
-        <is>
-          <t>3541</t>
+      <c r="I85" t="n">
+        <v>3541</v>
+      </c>
+      <c r="J85" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>3676</t>
         </is>
       </c>
     </row>
@@ -3506,9 +3994,15 @@
       <c r="H86" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I86" t="inlineStr">
-        <is>
-          <t>3146</t>
+      <c r="I86" t="n">
+        <v>3146</v>
+      </c>
+      <c r="J86" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>3184</t>
         </is>
       </c>
     </row>
@@ -3543,9 +4037,15 @@
       <c r="H87" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="I87" t="inlineStr">
-        <is>
-          <t>2990</t>
+      <c r="I87" t="n">
+        <v>2990</v>
+      </c>
+      <c r="J87" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>2981</t>
         </is>
       </c>
     </row>
@@ -3580,9 +4080,15 @@
       <c r="H88" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I88" t="inlineStr">
-        <is>
-          <t>3561</t>
+      <c r="I88" t="n">
+        <v>3561</v>
+      </c>
+      <c r="J88" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>3873</t>
         </is>
       </c>
     </row>
@@ -3617,9 +4123,15 @@
       <c r="H89" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I89" t="inlineStr">
-        <is>
-          <t>2770</t>
+      <c r="I89" t="n">
+        <v>2770</v>
+      </c>
+      <c r="J89" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>2782</t>
         </is>
       </c>
     </row>
@@ -3654,9 +4166,15 @@
       <c r="H90" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="I90" t="inlineStr">
-        <is>
-          <t>3050</t>
+      <c r="I90" t="n">
+        <v>3050</v>
+      </c>
+      <c r="J90" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>3141</t>
         </is>
       </c>
     </row>
@@ -3691,9 +4209,15 @@
       <c r="H91" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I91" t="inlineStr">
-        <is>
-          <t>2005</t>
+      <c r="I91" t="n">
+        <v>2005</v>
+      </c>
+      <c r="J91" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>2028</t>
         </is>
       </c>
     </row>
@@ -3728,9 +4252,15 @@
       <c r="H92" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I92" t="inlineStr">
-        <is>
-          <t>2707</t>
+      <c r="I92" t="n">
+        <v>2707</v>
+      </c>
+      <c r="J92" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>2710</t>
         </is>
       </c>
     </row>
@@ -3765,9 +4295,15 @@
       <c r="H93" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I93" t="inlineStr">
-        <is>
-          <t>2711</t>
+      <c r="I93" t="n">
+        <v>2711</v>
+      </c>
+      <c r="J93" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>2762</t>
         </is>
       </c>
     </row>
@@ -3802,9 +4338,15 @@
       <c r="H94" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I94" t="inlineStr">
-        <is>
-          <t>2286</t>
+      <c r="I94" t="n">
+        <v>2286</v>
+      </c>
+      <c r="J94" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>2273</t>
         </is>
       </c>
     </row>
@@ -3830,6 +4372,8 @@
       <c r="G95" t="inlineStr"/>
       <c r="H95" s="2" t="inlineStr"/>
       <c r="I95" t="inlineStr"/>
+      <c r="J95" s="2" t="inlineStr"/>
+      <c r="K95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -3862,9 +4406,15 @@
       <c r="H96" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I96" t="inlineStr">
-        <is>
-          <t>2408</t>
+      <c r="I96" t="n">
+        <v>2408</v>
+      </c>
+      <c r="J96" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>2402</t>
         </is>
       </c>
     </row>
@@ -3899,9 +4449,15 @@
       <c r="H97" s="5" t="n">
         <v>13</v>
       </c>
-      <c r="I97" t="inlineStr">
-        <is>
-          <t>2866</t>
+      <c r="I97" t="n">
+        <v>2866</v>
+      </c>
+      <c r="J97" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K97" t="inlineStr">
+        <is>
+          <t>3216</t>
         </is>
       </c>
     </row>
@@ -3936,9 +4492,15 @@
       <c r="H98" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="I98" t="inlineStr">
-        <is>
-          <t>2988</t>
+      <c r="I98" t="n">
+        <v>2988</v>
+      </c>
+      <c r="J98" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>3171</t>
         </is>
       </c>
     </row>
@@ -3973,9 +4535,15 @@
       <c r="H99" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I99" t="inlineStr">
-        <is>
-          <t>3601</t>
+      <c r="I99" t="n">
+        <v>3601</v>
+      </c>
+      <c r="J99" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K99" t="inlineStr">
+        <is>
+          <t>3700</t>
         </is>
       </c>
     </row>
@@ -4010,9 +4578,15 @@
       <c r="H100" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I100" t="inlineStr">
-        <is>
-          <t>3323</t>
+      <c r="I100" t="n">
+        <v>3323</v>
+      </c>
+      <c r="J100" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>3456</t>
         </is>
       </c>
     </row>
@@ -4047,9 +4621,15 @@
       <c r="H101" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="I101" t="inlineStr">
-        <is>
-          <t>2945</t>
+      <c r="I101" t="n">
+        <v>2945</v>
+      </c>
+      <c r="J101" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>3063</t>
         </is>
       </c>
     </row>
@@ -4084,9 +4664,15 @@
       <c r="H102" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I102" t="inlineStr">
-        <is>
-          <t>3614</t>
+      <c r="I102" t="n">
+        <v>3614</v>
+      </c>
+      <c r="J102" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>3792</t>
         </is>
       </c>
     </row>
@@ -4121,9 +4707,15 @@
       <c r="H103" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="I103" t="inlineStr">
-        <is>
-          <t>3296</t>
+      <c r="I103" t="n">
+        <v>3296</v>
+      </c>
+      <c r="J103" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>3267</t>
         </is>
       </c>
     </row>
@@ -4158,9 +4750,15 @@
       <c r="H104" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I104" t="inlineStr">
-        <is>
-          <t>2444</t>
+      <c r="I104" t="n">
+        <v>2444</v>
+      </c>
+      <c r="J104" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K104" t="inlineStr">
+        <is>
+          <t>2458</t>
         </is>
       </c>
     </row>
@@ -4195,9 +4793,15 @@
       <c r="H105" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="I105" t="inlineStr">
-        <is>
-          <t>3420</t>
+      <c r="I105" t="n">
+        <v>3420</v>
+      </c>
+      <c r="J105" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K105" t="inlineStr">
+        <is>
+          <t>3789</t>
         </is>
       </c>
     </row>
@@ -4232,9 +4836,15 @@
       <c r="H106" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="I106" t="inlineStr">
-        <is>
-          <t>3236</t>
+      <c r="I106" t="n">
+        <v>3236</v>
+      </c>
+      <c r="J106" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="K106" t="inlineStr">
+        <is>
+          <t>3344</t>
         </is>
       </c>
     </row>
@@ -4269,9 +4879,15 @@
       <c r="H107" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I107" t="inlineStr">
-        <is>
-          <t>3072</t>
+      <c r="I107" t="n">
+        <v>3072</v>
+      </c>
+      <c r="J107" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K107" t="inlineStr">
+        <is>
+          <t>3178</t>
         </is>
       </c>
     </row>
@@ -4306,9 +4922,15 @@
       <c r="H108" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="I108" t="inlineStr">
-        <is>
-          <t>2603</t>
+      <c r="I108" t="n">
+        <v>2603</v>
+      </c>
+      <c r="J108" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K108" t="inlineStr">
+        <is>
+          <t>2605</t>
         </is>
       </c>
     </row>
@@ -4343,9 +4965,15 @@
       <c r="H109" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I109" t="inlineStr">
-        <is>
-          <t>3100</t>
+      <c r="I109" t="n">
+        <v>3100</v>
+      </c>
+      <c r="J109" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>3070</t>
         </is>
       </c>
     </row>
@@ -4380,9 +5008,15 @@
       <c r="H110" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I110" t="inlineStr">
-        <is>
-          <t>3018</t>
+      <c r="I110" t="n">
+        <v>3018</v>
+      </c>
+      <c r="J110" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="K110" t="inlineStr">
+        <is>
+          <t>3048</t>
         </is>
       </c>
     </row>
@@ -4417,9 +5051,15 @@
       <c r="H111" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I111" t="inlineStr">
-        <is>
-          <t>3113</t>
+      <c r="I111" t="n">
+        <v>3113</v>
+      </c>
+      <c r="J111" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K111" t="inlineStr">
+        <is>
+          <t>3195</t>
         </is>
       </c>
     </row>
@@ -4454,9 +5094,15 @@
       <c r="H112" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="I112" t="inlineStr">
-        <is>
-          <t>3377</t>
+      <c r="I112" t="n">
+        <v>3377</v>
+      </c>
+      <c r="J112" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K112" t="inlineStr">
+        <is>
+          <t>3418</t>
         </is>
       </c>
     </row>
@@ -4491,9 +5137,15 @@
       <c r="H113" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="I113" t="inlineStr">
-        <is>
-          <t>2514</t>
+      <c r="I113" t="n">
+        <v>2514</v>
+      </c>
+      <c r="J113" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>2482</t>
         </is>
       </c>
     </row>
@@ -4528,9 +5180,15 @@
       <c r="H114" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="I114" t="inlineStr">
-        <is>
-          <t>2521</t>
+      <c r="I114" t="n">
+        <v>2521</v>
+      </c>
+      <c r="J114" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="K114" t="inlineStr">
+        <is>
+          <t>2554</t>
         </is>
       </c>
     </row>
@@ -4565,9 +5223,15 @@
       <c r="H115" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="I115" t="inlineStr">
-        <is>
-          <t>3048</t>
+      <c r="I115" t="n">
+        <v>3048</v>
+      </c>
+      <c r="J115" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>3010</t>
         </is>
       </c>
     </row>
@@ -4602,9 +5266,15 @@
       <c r="H116" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I116" t="inlineStr">
-        <is>
-          <t>2673</t>
+      <c r="I116" t="n">
+        <v>2673</v>
+      </c>
+      <c r="J116" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K116" t="inlineStr">
+        <is>
+          <t>2667</t>
         </is>
       </c>
     </row>
@@ -4639,9 +5309,15 @@
       <c r="H117" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I117" t="inlineStr">
-        <is>
-          <t>3022</t>
+      <c r="I117" t="n">
+        <v>3022</v>
+      </c>
+      <c r="J117" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>3184</t>
         </is>
       </c>
     </row>
@@ -4676,9 +5352,15 @@
       <c r="H118" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I118" t="inlineStr">
-        <is>
-          <t>2808</t>
+      <c r="I118" t="n">
+        <v>2808</v>
+      </c>
+      <c r="J118" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K118" t="inlineStr">
+        <is>
+          <t>2898</t>
         </is>
       </c>
     </row>
@@ -4713,9 +5395,15 @@
       <c r="H119" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I119" t="inlineStr">
-        <is>
-          <t>3197</t>
+      <c r="I119" t="n">
+        <v>3197</v>
+      </c>
+      <c r="J119" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="K119" t="inlineStr">
+        <is>
+          <t>3263</t>
         </is>
       </c>
     </row>
@@ -4750,9 +5438,15 @@
       <c r="H120" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="I120" t="inlineStr">
-        <is>
-          <t>2640</t>
+      <c r="I120" t="n">
+        <v>2640</v>
+      </c>
+      <c r="J120" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K120" t="inlineStr">
+        <is>
+          <t>2574</t>
         </is>
       </c>
     </row>
@@ -4787,9 +5481,15 @@
       <c r="H121" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="I121" t="inlineStr">
-        <is>
-          <t>2779</t>
+      <c r="I121" t="n">
+        <v>2779</v>
+      </c>
+      <c r="J121" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="K121" t="inlineStr">
+        <is>
+          <t>2932</t>
         </is>
       </c>
     </row>
@@ -4824,9 +5524,15 @@
       <c r="H122" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I122" t="inlineStr">
-        <is>
-          <t>2855</t>
+      <c r="I122" t="n">
+        <v>2855</v>
+      </c>
+      <c r="J122" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K122" t="inlineStr">
+        <is>
+          <t>2965</t>
         </is>
       </c>
     </row>
@@ -4861,9 +5567,15 @@
       <c r="H123" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I123" t="inlineStr">
-        <is>
-          <t>3113</t>
+      <c r="I123" t="n">
+        <v>3113</v>
+      </c>
+      <c r="J123" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K123" t="inlineStr">
+        <is>
+          <t>3242</t>
         </is>
       </c>
     </row>
@@ -4898,9 +5610,15 @@
       <c r="H124" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I124" t="inlineStr">
-        <is>
-          <t>2881</t>
+      <c r="I124" t="n">
+        <v>2881</v>
+      </c>
+      <c r="J124" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K124" t="inlineStr">
+        <is>
+          <t>2993</t>
         </is>
       </c>
     </row>
@@ -4935,9 +5653,15 @@
       <c r="H125" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I125" t="inlineStr">
-        <is>
-          <t>2146</t>
+      <c r="I125" t="n">
+        <v>2146</v>
+      </c>
+      <c r="J125" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K125" t="inlineStr">
+        <is>
+          <t>2138</t>
         </is>
       </c>
     </row>
@@ -4947,7 +5671,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>AdyYouTubeSs</t>
+          <t>权旨qua</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -4958,11 +5682,23 @@
       <c r="D126" t="n">
         <v>2741</v>
       </c>
-      <c r="E126" t="inlineStr"/>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
       <c r="F126" s="2" t="inlineStr"/>
       <c r="G126" t="inlineStr"/>
       <c r="H126" s="2" t="inlineStr"/>
       <c r="I126" t="inlineStr"/>
+      <c r="J126" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K126" t="inlineStr">
+        <is>
+          <t>2671</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
@@ -4995,9 +5731,15 @@
       <c r="H127" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I127" t="inlineStr">
-        <is>
-          <t>2466</t>
+      <c r="I127" t="n">
+        <v>2466</v>
+      </c>
+      <c r="J127" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K127" t="inlineStr">
+        <is>
+          <t>2424</t>
         </is>
       </c>
     </row>
@@ -5032,9 +5774,15 @@
       <c r="H128" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="I128" t="inlineStr">
-        <is>
-          <t>3599</t>
+      <c r="I128" t="n">
+        <v>3599</v>
+      </c>
+      <c r="J128" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K128" t="inlineStr">
+        <is>
+          <t>3858</t>
         </is>
       </c>
     </row>
@@ -5060,6 +5808,8 @@
       <c r="G129" t="inlineStr"/>
       <c r="H129" s="2" t="inlineStr"/>
       <c r="I129" t="inlineStr"/>
+      <c r="J129" s="2" t="inlineStr"/>
+      <c r="K129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="n">
@@ -5092,9 +5842,15 @@
       <c r="H130" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I130" t="inlineStr">
-        <is>
-          <t>2692</t>
+      <c r="I130" t="n">
+        <v>2692</v>
+      </c>
+      <c r="J130" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K130" t="inlineStr">
+        <is>
+          <t>2672</t>
         </is>
       </c>
     </row>
@@ -5129,9 +5885,15 @@
       <c r="H131" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I131" t="inlineStr">
-        <is>
-          <t>2582</t>
+      <c r="I131" t="n">
+        <v>2582</v>
+      </c>
+      <c r="J131" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="K131" t="inlineStr">
+        <is>
+          <t>2664</t>
         </is>
       </c>
     </row>
@@ -5166,9 +5928,15 @@
       <c r="H132" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I132" t="inlineStr">
-        <is>
-          <t>3099</t>
+      <c r="I132" t="n">
+        <v>3099</v>
+      </c>
+      <c r="J132" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K132" t="inlineStr">
+        <is>
+          <t>3259</t>
         </is>
       </c>
     </row>
@@ -5194,6 +5962,8 @@
       <c r="G133" t="inlineStr"/>
       <c r="H133" s="2" t="inlineStr"/>
       <c r="I133" t="inlineStr"/>
+      <c r="J133" s="2" t="inlineStr"/>
+      <c r="K133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="n">
@@ -5226,9 +5996,15 @@
       <c r="H134" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="I134" t="inlineStr">
-        <is>
-          <t>2584</t>
+      <c r="I134" t="n">
+        <v>2584</v>
+      </c>
+      <c r="J134" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="K134" t="inlineStr">
+        <is>
+          <t>2621</t>
         </is>
       </c>
     </row>
@@ -5263,9 +6039,15 @@
       <c r="H135" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="I135" t="inlineStr">
-        <is>
-          <t>2518</t>
+      <c r="I135" t="n">
+        <v>2518</v>
+      </c>
+      <c r="J135" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K135" t="inlineStr">
+        <is>
+          <t>2494</t>
         </is>
       </c>
     </row>
@@ -5300,9 +6082,15 @@
       <c r="H136" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="I136" t="inlineStr">
-        <is>
-          <t>2534</t>
+      <c r="I136" t="n">
+        <v>2534</v>
+      </c>
+      <c r="J136" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="K136" t="inlineStr">
+        <is>
+          <t>2540</t>
         </is>
       </c>
     </row>
@@ -5337,9 +6125,15 @@
       <c r="H137" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I137" t="inlineStr">
-        <is>
-          <t>2080</t>
+      <c r="I137" t="n">
+        <v>2080</v>
+      </c>
+      <c r="J137" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K137" t="inlineStr">
+        <is>
+          <t>2064</t>
         </is>
       </c>
     </row>
@@ -5365,6 +6159,8 @@
       <c r="G138" t="inlineStr"/>
       <c r="H138" s="2" t="inlineStr"/>
       <c r="I138" t="inlineStr"/>
+      <c r="J138" s="2" t="inlineStr"/>
+      <c r="K138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -5388,6 +6184,8 @@
       <c r="G139" t="inlineStr"/>
       <c r="H139" s="2" t="inlineStr"/>
       <c r="I139" t="inlineStr"/>
+      <c r="J139" s="2" t="inlineStr"/>
+      <c r="K139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -5411,6 +6209,8 @@
       <c r="G140" t="inlineStr"/>
       <c r="H140" s="2" t="inlineStr"/>
       <c r="I140" t="inlineStr"/>
+      <c r="J140" s="2" t="inlineStr"/>
+      <c r="K140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="n">
@@ -5443,9 +6243,15 @@
       <c r="H141" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I141" t="inlineStr">
-        <is>
-          <t>1991</t>
+      <c r="I141" t="n">
+        <v>1991</v>
+      </c>
+      <c r="J141" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K141" t="inlineStr">
+        <is>
+          <t>2022</t>
         </is>
       </c>
     </row>
@@ -5471,6 +6277,8 @@
       <c r="G142" t="inlineStr"/>
       <c r="H142" s="2" t="inlineStr"/>
       <c r="I142" t="inlineStr"/>
+      <c r="J142" s="2" t="inlineStr"/>
+      <c r="K142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="n">
@@ -5494,6 +6302,8 @@
       <c r="G143" t="inlineStr"/>
       <c r="H143" s="2" t="inlineStr"/>
       <c r="I143" t="inlineStr"/>
+      <c r="J143" s="2" t="inlineStr"/>
+      <c r="K143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -5517,6 +6327,8 @@
       <c r="G144" t="inlineStr"/>
       <c r="H144" s="2" t="inlineStr"/>
       <c r="I144" t="inlineStr"/>
+      <c r="J144" s="2" t="inlineStr"/>
+      <c r="K144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -5540,6 +6352,8 @@
       <c r="G145" t="inlineStr"/>
       <c r="H145" s="2" t="inlineStr"/>
       <c r="I145" t="inlineStr"/>
+      <c r="J145" s="2" t="inlineStr"/>
+      <c r="K145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -5563,6 +6377,8 @@
       <c r="G146" t="inlineStr"/>
       <c r="H146" s="2" t="inlineStr"/>
       <c r="I146" t="inlineStr"/>
+      <c r="J146" s="2" t="inlineStr"/>
+      <c r="K146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -5586,6 +6402,8 @@
       <c r="G147" t="inlineStr"/>
       <c r="H147" s="2" t="inlineStr"/>
       <c r="I147" t="inlineStr"/>
+      <c r="J147" s="2" t="inlineStr"/>
+      <c r="K147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -5609,6 +6427,8 @@
       <c r="G148" t="inlineStr"/>
       <c r="H148" s="2" t="inlineStr"/>
       <c r="I148" t="inlineStr"/>
+      <c r="J148" s="2" t="inlineStr"/>
+      <c r="K148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="n">
@@ -5632,6 +6452,8 @@
       <c r="G149" t="inlineStr"/>
       <c r="H149" s="2" t="inlineStr"/>
       <c r="I149" t="inlineStr"/>
+      <c r="J149" s="2" t="inlineStr"/>
+      <c r="K149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="n">
@@ -5655,6 +6477,8 @@
       <c r="G150" t="inlineStr"/>
       <c r="H150" s="2" t="inlineStr"/>
       <c r="I150" t="inlineStr"/>
+      <c r="J150" s="2" t="inlineStr"/>
+      <c r="K150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="n">
@@ -5678,6 +6502,8 @@
       <c r="G151" t="inlineStr"/>
       <c r="H151" s="2" t="inlineStr"/>
       <c r="I151" t="inlineStr"/>
+      <c r="J151" s="2" t="inlineStr"/>
+      <c r="K151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="n">
@@ -5701,6 +6527,8 @@
       <c r="G152" t="inlineStr"/>
       <c r="H152" s="2" t="inlineStr"/>
       <c r="I152" t="inlineStr"/>
+      <c r="J152" s="2" t="inlineStr"/>
+      <c r="K152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" t="n">
@@ -5724,6 +6552,8 @@
       <c r="G153" t="inlineStr"/>
       <c r="H153" s="2" t="inlineStr"/>
       <c r="I153" t="inlineStr"/>
+      <c r="J153" s="2" t="inlineStr"/>
+      <c r="K153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" t="n">
@@ -5756,9 +6586,15 @@
       <c r="H154" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="I154" t="inlineStr">
-        <is>
-          <t>1830</t>
+      <c r="I154" t="n">
+        <v>1830</v>
+      </c>
+      <c r="J154" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="K154" t="inlineStr">
+        <is>
+          <t>1790</t>
         </is>
       </c>
     </row>
@@ -5784,6 +6620,8 @@
       <c r="G155" t="inlineStr"/>
       <c r="H155" s="2" t="inlineStr"/>
       <c r="I155" t="inlineStr"/>
+      <c r="J155" s="2" t="inlineStr"/>
+      <c r="K155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="n">
@@ -5816,9 +6654,15 @@
       <c r="H156" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I156" t="inlineStr">
-        <is>
-          <t>3003</t>
+      <c r="I156" t="n">
+        <v>3003</v>
+      </c>
+      <c r="J156" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="K156" t="inlineStr">
+        <is>
+          <t>3700</t>
         </is>
       </c>
     </row>
@@ -5853,7 +6697,13 @@
       <c r="H157" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I157" t="inlineStr">
+      <c r="I157" t="n">
+        <v>0</v>
+      </c>
+      <c r="J157" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K157" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5890,9 +6740,15 @@
       <c r="H158" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I158" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I158" t="n">
+        <v>0</v>
+      </c>
+      <c r="J158" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K158" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -5927,9 +6783,15 @@
       <c r="H159" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="I159" t="inlineStr">
-        <is>
-          <t>3542</t>
+      <c r="I159" t="n">
+        <v>3542</v>
+      </c>
+      <c r="J159" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="K159" t="inlineStr">
+        <is>
+          <t>3844</t>
         </is>
       </c>
     </row>
@@ -5964,7 +6826,13 @@
       <c r="H160" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I160" t="inlineStr">
+      <c r="I160" t="n">
+        <v>0</v>
+      </c>
+      <c r="J160" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K160" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6001,9 +6869,15 @@
       <c r="H161" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I161" t="inlineStr">
-        <is>
-          <t>2645</t>
+      <c r="I161" t="n">
+        <v>2645</v>
+      </c>
+      <c r="J161" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="K161" t="inlineStr">
+        <is>
+          <t>2874</t>
         </is>
       </c>
     </row>
@@ -6038,7 +6912,13 @@
       <c r="H162" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I162" t="inlineStr">
+      <c r="I162" t="n">
+        <v>0</v>
+      </c>
+      <c r="J162" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K162" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6075,9 +6955,15 @@
       <c r="H163" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I163" t="inlineStr">
-        <is>
-          <t>2526</t>
+      <c r="I163" t="n">
+        <v>2526</v>
+      </c>
+      <c r="J163" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K163" t="inlineStr">
+        <is>
+          <t>2635</t>
         </is>
       </c>
     </row>
@@ -6106,9 +6992,15 @@
       <c r="H164" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="I164" t="inlineStr">
-        <is>
-          <t>2738</t>
+      <c r="I164" t="n">
+        <v>2738</v>
+      </c>
+      <c r="J164" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="K164" t="inlineStr">
+        <is>
+          <t>2732</t>
         </is>
       </c>
     </row>
@@ -6137,9 +7029,15 @@
       <c r="H165" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I165" t="inlineStr">
-        <is>
-          <t>1951</t>
+      <c r="I165" t="n">
+        <v>1951</v>
+      </c>
+      <c r="J165" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="K165" t="inlineStr">
+        <is>
+          <t>2090</t>
         </is>
       </c>
     </row>
@@ -6168,9 +7066,15 @@
       <c r="H166" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I166" t="inlineStr">
-        <is>
-          <t>4475</t>
+      <c r="I166" t="n">
+        <v>4475</v>
+      </c>
+      <c r="J166" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K166" t="inlineStr">
+        <is>
+          <t>4758</t>
         </is>
       </c>
     </row>
@@ -6198,6 +7102,8 @@
       </c>
       <c r="H167" s="2" t="inlineStr"/>
       <c r="I167" t="inlineStr"/>
+      <c r="J167" s="2" t="inlineStr"/>
+      <c r="K167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" t="n">
@@ -6224,9 +7130,15 @@
       <c r="H168" s="5" t="n">
         <v>13</v>
       </c>
-      <c r="I168" t="inlineStr">
-        <is>
-          <t>2990</t>
+      <c r="I168" t="n">
+        <v>2990</v>
+      </c>
+      <c r="J168" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K168" t="inlineStr">
+        <is>
+          <t>2950</t>
         </is>
       </c>
     </row>
@@ -6255,9 +7167,15 @@
       <c r="H169" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="I169" t="inlineStr">
-        <is>
-          <t>2752</t>
+      <c r="I169" t="n">
+        <v>2752</v>
+      </c>
+      <c r="J169" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="K169" t="inlineStr">
+        <is>
+          <t>2856</t>
         </is>
       </c>
     </row>
@@ -6286,17 +7204,21 @@
       <c r="H170" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I170" t="inlineStr">
-        <is>
-          <t>2131</t>
+      <c r="I170" t="n">
+        <v>2131</v>
+      </c>
+      <c r="J170" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K170" t="inlineStr">
+        <is>
+          <t>2368</t>
         </is>
       </c>
     </row>
     <row r="171">
-      <c r="A171" t="inlineStr">
-        <is>
-          <t>27113069</t>
-        </is>
+      <c r="A171" t="n">
+        <v>27113069</v>
       </c>
       <c r="B171" t="inlineStr">
         <is>
@@ -6315,17 +7237,21 @@
       <c r="H171" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="I171" t="inlineStr">
-        <is>
-          <t>4138</t>
+      <c r="I171" t="n">
+        <v>4138</v>
+      </c>
+      <c r="J171" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K171" t="inlineStr">
+        <is>
+          <t>4464</t>
         </is>
       </c>
     </row>
     <row r="172">
-      <c r="A172" t="inlineStr">
-        <is>
-          <t>47533851</t>
-        </is>
+      <c r="A172" t="n">
+        <v>47533851</v>
       </c>
       <c r="B172" t="inlineStr">
         <is>
@@ -6344,9 +7270,170 @@
       <c r="H172" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="I172" t="inlineStr">
-        <is>
-          <t>2053</t>
+      <c r="I172" t="n">
+        <v>2053</v>
+      </c>
+      <c r="J172" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="K172" t="inlineStr">
+        <is>
+          <t>2162</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>15436348</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>Lucas</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr"/>
+      <c r="D173" t="inlineStr"/>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F173" s="2" t="inlineStr"/>
+      <c r="G173" t="inlineStr"/>
+      <c r="H173" s="2" t="inlineStr"/>
+      <c r="I173" t="inlineStr"/>
+      <c r="J173" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K173" t="inlineStr">
+        <is>
+          <t>1813</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>53269862</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>New_Player111</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr"/>
+      <c r="D174" t="inlineStr"/>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F174" s="2" t="inlineStr"/>
+      <c r="G174" t="inlineStr"/>
+      <c r="H174" s="2" t="inlineStr"/>
+      <c r="I174" t="inlineStr"/>
+      <c r="J174" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K174" t="inlineStr">
+        <is>
+          <t>1666</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>55963040</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>Baliram</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr"/>
+      <c r="D175" t="inlineStr"/>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F175" s="2" t="inlineStr"/>
+      <c r="G175" t="inlineStr"/>
+      <c r="H175" s="2" t="inlineStr"/>
+      <c r="I175" t="inlineStr"/>
+      <c r="J175" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K175" t="inlineStr">
+        <is>
+          <t>2473</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>58132159</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>ExultantDelivery42</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr"/>
+      <c r="D176" t="inlineStr"/>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F176" s="2" t="inlineStr"/>
+      <c r="G176" t="inlineStr"/>
+      <c r="H176" s="2" t="inlineStr"/>
+      <c r="I176" t="inlineStr"/>
+      <c r="J176" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="K176" t="inlineStr">
+        <is>
+          <t>1528</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>48005945</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>NIKONEZNA</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr"/>
+      <c r="D177" t="inlineStr"/>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="F177" s="2" t="inlineStr"/>
+      <c r="G177" t="inlineStr"/>
+      <c r="H177" s="2" t="inlineStr"/>
+      <c r="I177" t="inlineStr"/>
+      <c r="J177" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="K177" t="inlineStr">
+        <is>
+          <t>2563</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-01-23 11:31:28
</commit_message>
<xml_diff>
--- a/Season_Attack/82.xlsx
+++ b/Season_Attack/82.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G178"/>
+  <dimension ref="A1:I181"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,6 +426,16 @@
           <t>01-21_0</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>01-22_A</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>01-22_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -452,9 +462,15 @@
       <c r="F2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>3481</t>
+      <c r="G2" t="n">
+        <v>3481</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>3531</t>
         </is>
       </c>
     </row>
@@ -483,9 +499,15 @@
       <c r="F3" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>4691</t>
+      <c r="G3" t="n">
+        <v>4691</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>35</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>4897</t>
         </is>
       </c>
     </row>
@@ -514,9 +536,15 @@
       <c r="F4" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>4441</t>
+      <c r="G4" t="n">
+        <v>4441</v>
+      </c>
+      <c r="H4" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>4746</t>
         </is>
       </c>
     </row>
@@ -545,9 +573,15 @@
       <c r="F5" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>4366</t>
+      <c r="G5" t="n">
+        <v>4366</v>
+      </c>
+      <c r="H5" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>4678</t>
         </is>
       </c>
     </row>
@@ -576,9 +610,15 @@
       <c r="F6" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>4698</t>
+      <c r="G6" t="n">
+        <v>4698</v>
+      </c>
+      <c r="H6" s="3" t="n">
+        <v>34</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>4962</t>
         </is>
       </c>
     </row>
@@ -607,9 +647,15 @@
       <c r="F7" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>4368</t>
+      <c r="G7" t="n">
+        <v>4368</v>
+      </c>
+      <c r="H7" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>4641</t>
         </is>
       </c>
     </row>
@@ -632,15 +678,21 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F8" s="3" t="n">
         <v>31</v>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>3918</t>
+      <c r="G8" t="n">
+        <v>3918</v>
+      </c>
+      <c r="H8" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>4137</t>
         </is>
       </c>
     </row>
@@ -664,6 +716,8 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" s="4" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
+      <c r="H9" s="4" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -690,9 +744,15 @@
       <c r="F10" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>4520</t>
+      <c r="G10" t="n">
+        <v>4520</v>
+      </c>
+      <c r="H10" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>4542</t>
         </is>
       </c>
     </row>
@@ -721,9 +781,15 @@
       <c r="F11" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>4674</t>
+      <c r="G11" t="n">
+        <v>4674</v>
+      </c>
+      <c r="H11" s="3" t="n">
+        <v>34</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>5218</t>
         </is>
       </c>
     </row>
@@ -752,9 +818,15 @@
       <c r="F12" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>4125</t>
+      <c r="G12" t="n">
+        <v>4125</v>
+      </c>
+      <c r="H12" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>4309</t>
         </is>
       </c>
     </row>
@@ -783,9 +855,15 @@
       <c r="F13" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>2879</t>
+      <c r="G13" t="n">
+        <v>2879</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>2903</t>
         </is>
       </c>
     </row>
@@ -814,9 +892,15 @@
       <c r="F14" s="3" t="n">
         <v>39</v>
       </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>5341</t>
+      <c r="G14" t="n">
+        <v>5341</v>
+      </c>
+      <c r="H14" s="3" t="n">
+        <v>38</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>5641</t>
         </is>
       </c>
     </row>
@@ -845,9 +929,15 @@
       <c r="F15" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>4559</t>
+      <c r="G15" t="n">
+        <v>4559</v>
+      </c>
+      <c r="H15" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>4783</t>
         </is>
       </c>
     </row>
@@ -876,9 +966,15 @@
       <c r="F16" s="3" t="n">
         <v>31</v>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>4776</t>
+      <c r="G16" t="n">
+        <v>4776</v>
+      </c>
+      <c r="H16" s="3" t="n">
+        <v>31</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>4843</t>
         </is>
       </c>
     </row>
@@ -907,9 +1003,15 @@
       <c r="F17" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>4203</t>
+      <c r="G17" t="n">
+        <v>4203</v>
+      </c>
+      <c r="H17" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>4378</t>
         </is>
       </c>
     </row>
@@ -938,9 +1040,15 @@
       <c r="F18" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>4262</t>
+      <c r="G18" t="n">
+        <v>4262</v>
+      </c>
+      <c r="H18" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>4619</t>
         </is>
       </c>
     </row>
@@ -969,9 +1077,15 @@
       <c r="F19" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>5215</t>
+      <c r="G19" t="n">
+        <v>5215</v>
+      </c>
+      <c r="H19" s="3" t="n">
+        <v>33</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>5441</t>
         </is>
       </c>
     </row>
@@ -1000,9 +1114,15 @@
       <c r="F20" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>4083</t>
+      <c r="G20" t="n">
+        <v>4083</v>
+      </c>
+      <c r="H20" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>4406</t>
         </is>
       </c>
     </row>
@@ -1031,9 +1151,15 @@
       <c r="F21" s="3" t="n">
         <v>39</v>
       </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>4561</t>
+      <c r="G21" t="n">
+        <v>4561</v>
+      </c>
+      <c r="H21" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>4884</t>
         </is>
       </c>
     </row>
@@ -1062,9 +1188,15 @@
       <c r="F22" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>2866</t>
+      <c r="G22" t="n">
+        <v>2866</v>
+      </c>
+      <c r="H22" s="3" t="n">
+        <v>33</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>3579</t>
         </is>
       </c>
     </row>
@@ -1093,9 +1225,15 @@
       <c r="F23" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>4641</t>
+      <c r="G23" t="n">
+        <v>4641</v>
+      </c>
+      <c r="H23" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>4965</t>
         </is>
       </c>
     </row>
@@ -1124,7 +1262,13 @@
       <c r="F24" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G24" t="inlineStr">
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1155,9 +1299,15 @@
       <c r="F25" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>4523</t>
+      <c r="G25" t="n">
+        <v>4523</v>
+      </c>
+      <c r="H25" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>4625</t>
         </is>
       </c>
     </row>
@@ -1186,9 +1336,15 @@
       <c r="F26" s="3" t="n">
         <v>35</v>
       </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>4788</t>
+      <c r="G26" t="n">
+        <v>4788</v>
+      </c>
+      <c r="H26" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>5184</t>
         </is>
       </c>
     </row>
@@ -1217,9 +1373,15 @@
       <c r="F27" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>3870</t>
+      <c r="G27" t="n">
+        <v>3870</v>
+      </c>
+      <c r="H27" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>3950</t>
         </is>
       </c>
     </row>
@@ -1248,9 +1410,15 @@
       <c r="F28" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>5108</t>
+      <c r="G28" t="n">
+        <v>5108</v>
+      </c>
+      <c r="H28" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>5456</t>
         </is>
       </c>
     </row>
@@ -1279,9 +1447,15 @@
       <c r="F29" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>4510</t>
+      <c r="G29" t="n">
+        <v>4510</v>
+      </c>
+      <c r="H29" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>4713</t>
         </is>
       </c>
     </row>
@@ -1310,9 +1484,15 @@
       <c r="F30" s="3" t="n">
         <v>31</v>
       </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>4706</t>
+      <c r="G30" t="n">
+        <v>4706</v>
+      </c>
+      <c r="H30" s="3" t="n">
+        <v>38</v>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>5160</t>
         </is>
       </c>
     </row>
@@ -1322,7 +1502,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>"Zephyr ᶻᵍˣ"</t>
+          <t>Auto-Battle</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1341,9 +1521,15 @@
       <c r="F31" s="3" t="n">
         <v>37</v>
       </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>4975</t>
+      <c r="G31" t="n">
+        <v>4975</v>
+      </c>
+      <c r="H31" s="3" t="n">
+        <v>37</v>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>5225</t>
         </is>
       </c>
     </row>
@@ -1372,7 +1558,13 @@
       <c r="F32" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="G32" t="inlineStr">
+      <c r="G32" t="n">
+        <v>2873</v>
+      </c>
+      <c r="H32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" t="inlineStr">
         <is>
           <t>2873</t>
         </is>
@@ -1403,9 +1595,15 @@
       <c r="F33" s="3" t="n">
         <v>38</v>
       </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>4746</t>
+      <c r="G33" t="n">
+        <v>4746</v>
+      </c>
+      <c r="H33" s="3" t="n">
+        <v>39</v>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>5073</t>
         </is>
       </c>
     </row>
@@ -1434,9 +1632,15 @@
       <c r="F34" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>4432</t>
+      <c r="G34" t="n">
+        <v>4432</v>
+      </c>
+      <c r="H34" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>4717</t>
         </is>
       </c>
     </row>
@@ -1465,9 +1669,15 @@
       <c r="F35" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>4233</t>
+      <c r="G35" t="n">
+        <v>4233</v>
+      </c>
+      <c r="H35" s="3" t="n">
+        <v>34</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>4343</t>
         </is>
       </c>
     </row>
@@ -1491,6 +1701,8 @@
       <c r="E36" t="inlineStr"/>
       <c r="F36" s="4" t="inlineStr"/>
       <c r="G36" t="inlineStr"/>
+      <c r="H36" s="4" t="inlineStr"/>
+      <c r="I36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -1517,9 +1729,15 @@
       <c r="F37" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>4548</t>
+      <c r="G37" t="n">
+        <v>4548</v>
+      </c>
+      <c r="H37" s="3" t="n">
+        <v>31</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>4771</t>
         </is>
       </c>
     </row>
@@ -1548,9 +1766,15 @@
       <c r="F38" s="3" t="n">
         <v>35</v>
       </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>4430</t>
+      <c r="G38" t="n">
+        <v>4430</v>
+      </c>
+      <c r="H38" s="3" t="n">
+        <v>35</v>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>4682</t>
         </is>
       </c>
     </row>
@@ -1579,9 +1803,15 @@
       <c r="F39" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>5092</t>
+      <c r="G39" t="n">
+        <v>5092</v>
+      </c>
+      <c r="H39" s="3" t="n">
+        <v>35</v>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>5299</t>
         </is>
       </c>
     </row>
@@ -1610,9 +1840,15 @@
       <c r="F40" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>4506</t>
+      <c r="G40" t="n">
+        <v>4506</v>
+      </c>
+      <c r="H40" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>4738</t>
         </is>
       </c>
     </row>
@@ -1641,9 +1877,15 @@
       <c r="F41" s="3" t="n">
         <v>35</v>
       </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>5076</t>
+      <c r="G41" t="n">
+        <v>5076</v>
+      </c>
+      <c r="H41" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>5338</t>
         </is>
       </c>
     </row>
@@ -1672,9 +1914,15 @@
       <c r="F42" s="3" t="n">
         <v>34</v>
       </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>4560</t>
+      <c r="G42" t="n">
+        <v>4560</v>
+      </c>
+      <c r="H42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>4552</t>
         </is>
       </c>
     </row>
@@ -1703,9 +1951,15 @@
       <c r="F43" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>2851</t>
+      <c r="G43" t="n">
+        <v>2851</v>
+      </c>
+      <c r="H43" s="3" t="n">
+        <v>39</v>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>2920</t>
         </is>
       </c>
     </row>
@@ -1734,9 +1988,15 @@
       <c r="F44" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>4169</t>
+      <c r="G44" t="n">
+        <v>4169</v>
+      </c>
+      <c r="H44" s="3" t="n">
+        <v>33</v>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>4351</t>
         </is>
       </c>
     </row>
@@ -1765,9 +2025,15 @@
       <c r="F45" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>4185</t>
+      <c r="G45" t="n">
+        <v>4185</v>
+      </c>
+      <c r="H45" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>4238</t>
         </is>
       </c>
     </row>
@@ -1796,9 +2062,15 @@
       <c r="F46" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>3085</t>
+      <c r="G46" t="n">
+        <v>3085</v>
+      </c>
+      <c r="H46" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>3112</t>
         </is>
       </c>
     </row>
@@ -1827,9 +2099,15 @@
       <c r="F47" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>4824</t>
+      <c r="G47" t="n">
+        <v>4824</v>
+      </c>
+      <c r="H47" s="3" t="n">
+        <v>36</v>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>5076</t>
         </is>
       </c>
     </row>
@@ -1858,9 +2136,15 @@
       <c r="F48" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>4486</t>
+      <c r="G48" t="n">
+        <v>4486</v>
+      </c>
+      <c r="H48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>4522</t>
         </is>
       </c>
     </row>
@@ -1889,7 +2173,13 @@
       <c r="F49" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G49" t="inlineStr">
+      <c r="G49" t="n">
+        <v>3416</v>
+      </c>
+      <c r="H49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I49" t="inlineStr">
         <is>
           <t>3416</t>
         </is>
@@ -1915,6 +2205,8 @@
       <c r="E50" t="inlineStr"/>
       <c r="F50" s="4" t="inlineStr"/>
       <c r="G50" t="inlineStr"/>
+      <c r="H50" s="4" t="inlineStr"/>
+      <c r="I50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -1936,6 +2228,8 @@
       <c r="E51" t="inlineStr"/>
       <c r="F51" s="4" t="inlineStr"/>
       <c r="G51" t="inlineStr"/>
+      <c r="H51" s="4" t="inlineStr"/>
+      <c r="I51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -1962,9 +2256,15 @@
       <c r="F52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>2533</t>
+      <c r="G52" t="n">
+        <v>2533</v>
+      </c>
+      <c r="H52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>2530</t>
         </is>
       </c>
     </row>
@@ -1993,9 +2293,15 @@
       <c r="F53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>3117</t>
+      <c r="G53" t="n">
+        <v>3117</v>
+      </c>
+      <c r="H53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>3141</t>
         </is>
       </c>
     </row>
@@ -2024,9 +2330,15 @@
       <c r="F54" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>2862</t>
+      <c r="G54" t="n">
+        <v>2862</v>
+      </c>
+      <c r="H54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>2891</t>
         </is>
       </c>
     </row>
@@ -2055,9 +2367,15 @@
       <c r="F55" s="5" t="n">
         <v>13</v>
       </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>4456</t>
+      <c r="G55" t="n">
+        <v>4456</v>
+      </c>
+      <c r="H55" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>4675</t>
         </is>
       </c>
     </row>
@@ -2086,9 +2404,15 @@
       <c r="F56" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>3675</t>
+      <c r="G56" t="n">
+        <v>3675</v>
+      </c>
+      <c r="H56" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>3846</t>
         </is>
       </c>
     </row>
@@ -2117,9 +2441,15 @@
       <c r="F57" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>3815</t>
+      <c r="G57" t="n">
+        <v>3815</v>
+      </c>
+      <c r="H57" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>3976</t>
         </is>
       </c>
     </row>
@@ -2148,9 +2478,15 @@
       <c r="F58" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>4176</t>
+      <c r="G58" t="n">
+        <v>4176</v>
+      </c>
+      <c r="H58" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>4408</t>
         </is>
       </c>
     </row>
@@ -2179,9 +2515,15 @@
       <c r="F59" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>3787</t>
+      <c r="G59" t="n">
+        <v>3787</v>
+      </c>
+      <c r="H59" s="3" t="n">
+        <v>33</v>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>3972</t>
         </is>
       </c>
     </row>
@@ -2210,9 +2552,15 @@
       <c r="F60" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>4164</t>
+      <c r="G60" t="n">
+        <v>4164</v>
+      </c>
+      <c r="H60" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>4428</t>
         </is>
       </c>
     </row>
@@ -2241,7 +2589,13 @@
       <c r="F61" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G61" t="inlineStr">
+      <c r="G61" t="n">
+        <v>3179</v>
+      </c>
+      <c r="H61" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I61" t="inlineStr">
         <is>
           <t>3179</t>
         </is>
@@ -2272,9 +2626,15 @@
       <c r="F62" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>4456</t>
+      <c r="G62" t="n">
+        <v>4456</v>
+      </c>
+      <c r="H62" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>4598</t>
         </is>
       </c>
     </row>
@@ -2303,9 +2663,15 @@
       <c r="F63" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>3047</t>
+      <c r="G63" t="n">
+        <v>3047</v>
+      </c>
+      <c r="H63" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>3381</t>
         </is>
       </c>
     </row>
@@ -2334,9 +2700,15 @@
       <c r="F64" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>2932</t>
+      <c r="G64" t="n">
+        <v>2932</v>
+      </c>
+      <c r="H64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>2907</t>
         </is>
       </c>
     </row>
@@ -2365,9 +2737,15 @@
       <c r="F65" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>4218</t>
+      <c r="G65" t="n">
+        <v>4218</v>
+      </c>
+      <c r="H65" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>4393</t>
         </is>
       </c>
     </row>
@@ -2396,9 +2774,15 @@
       <c r="F66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>2663</t>
+      <c r="G66" t="n">
+        <v>2663</v>
+      </c>
+      <c r="H66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>2693</t>
         </is>
       </c>
     </row>
@@ -2427,9 +2811,15 @@
       <c r="F67" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>4652</t>
+      <c r="G67" t="n">
+        <v>4652</v>
+      </c>
+      <c r="H67" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>4747</t>
         </is>
       </c>
     </row>
@@ -2458,9 +2848,15 @@
       <c r="F68" s="3" t="n">
         <v>32</v>
       </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>3799</t>
+      <c r="G68" t="n">
+        <v>3799</v>
+      </c>
+      <c r="H68" s="3" t="n">
+        <v>34</v>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>4053</t>
         </is>
       </c>
     </row>
@@ -2489,9 +2885,15 @@
       <c r="F69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>3244</t>
+      <c r="G69" t="n">
+        <v>3244</v>
+      </c>
+      <c r="H69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>3295</t>
         </is>
       </c>
     </row>
@@ -2520,9 +2922,15 @@
       <c r="F70" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>3883</t>
+      <c r="G70" t="n">
+        <v>3883</v>
+      </c>
+      <c r="H70" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>4016</t>
         </is>
       </c>
     </row>
@@ -2551,9 +2959,15 @@
       <c r="F71" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>3418</t>
+      <c r="G71" t="n">
+        <v>3418</v>
+      </c>
+      <c r="H71" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>3443</t>
         </is>
       </c>
     </row>
@@ -2582,9 +2996,15 @@
       <c r="F72" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>4488</t>
+      <c r="G72" t="n">
+        <v>4488</v>
+      </c>
+      <c r="H72" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>4647</t>
         </is>
       </c>
     </row>
@@ -2613,9 +3033,15 @@
       <c r="F73" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>3834</t>
+      <c r="G73" t="n">
+        <v>3834</v>
+      </c>
+      <c r="H73" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>3928</t>
         </is>
       </c>
     </row>
@@ -2644,9 +3070,15 @@
       <c r="F74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>3393</t>
+      <c r="G74" t="n">
+        <v>3393</v>
+      </c>
+      <c r="H74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>3459</t>
         </is>
       </c>
     </row>
@@ -2675,9 +3107,15 @@
       <c r="F75" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>3502</t>
+      <c r="G75" t="n">
+        <v>3502</v>
+      </c>
+      <c r="H75" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>3638</t>
         </is>
       </c>
     </row>
@@ -2706,9 +3144,15 @@
       <c r="F76" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="G76" t="inlineStr">
-        <is>
-          <t>4129</t>
+      <c r="G76" t="n">
+        <v>4129</v>
+      </c>
+      <c r="H76" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>4438</t>
         </is>
       </c>
     </row>
@@ -2737,9 +3181,15 @@
       <c r="F77" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>4459</t>
+      <c r="G77" t="n">
+        <v>4459</v>
+      </c>
+      <c r="H77" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>4598</t>
         </is>
       </c>
     </row>
@@ -2768,7 +3218,13 @@
       <c r="F78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G78" t="inlineStr">
+      <c r="G78" t="n">
+        <v>0</v>
+      </c>
+      <c r="H78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2799,9 +3255,15 @@
       <c r="F79" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>4278</t>
+      <c r="G79" t="n">
+        <v>4278</v>
+      </c>
+      <c r="H79" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>4542</t>
         </is>
       </c>
     </row>
@@ -2824,15 +3286,21 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F80" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="G80" t="inlineStr">
-        <is>
-          <t>3804</t>
+      <c r="G80" t="n">
+        <v>3804</v>
+      </c>
+      <c r="H80" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>4011</t>
         </is>
       </c>
     </row>
@@ -2861,9 +3329,15 @@
       <c r="F81" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>4107</t>
+      <c r="G81" t="n">
+        <v>4107</v>
+      </c>
+      <c r="H81" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>4233</t>
         </is>
       </c>
     </row>
@@ -2892,9 +3366,15 @@
       <c r="F82" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>4090</t>
+      <c r="G82" t="n">
+        <v>4090</v>
+      </c>
+      <c r="H82" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>4330</t>
         </is>
       </c>
     </row>
@@ -2923,9 +3403,15 @@
       <c r="F83" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>4003</t>
+      <c r="G83" t="n">
+        <v>4003</v>
+      </c>
+      <c r="H83" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>4167</t>
         </is>
       </c>
     </row>
@@ -2954,9 +3440,15 @@
       <c r="F84" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>3902</t>
+      <c r="G84" t="n">
+        <v>3902</v>
+      </c>
+      <c r="H84" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>4026</t>
         </is>
       </c>
     </row>
@@ -2985,9 +3477,15 @@
       <c r="F85" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>3846</t>
+      <c r="G85" t="n">
+        <v>3846</v>
+      </c>
+      <c r="H85" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>4006</t>
         </is>
       </c>
     </row>
@@ -3016,9 +3514,15 @@
       <c r="F86" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>3293</t>
+      <c r="G86" t="n">
+        <v>3293</v>
+      </c>
+      <c r="H86" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>3379</t>
         </is>
       </c>
     </row>
@@ -3047,7 +3551,13 @@
       <c r="F87" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="G87" t="inlineStr">
+      <c r="G87" t="n">
+        <v>3124</v>
+      </c>
+      <c r="H87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I87" t="inlineStr">
         <is>
           <t>3124</t>
         </is>
@@ -3078,9 +3588,15 @@
       <c r="F88" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="G88" t="inlineStr">
-        <is>
-          <t>4160</t>
+      <c r="G88" t="n">
+        <v>4160</v>
+      </c>
+      <c r="H88" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>4155</t>
         </is>
       </c>
     </row>
@@ -3109,9 +3625,15 @@
       <c r="F89" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t>2852</t>
+      <c r="G89" t="n">
+        <v>2852</v>
+      </c>
+      <c r="H89" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>2922</t>
         </is>
       </c>
     </row>
@@ -3140,9 +3662,15 @@
       <c r="F90" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>3179</t>
+      <c r="G90" t="n">
+        <v>3179</v>
+      </c>
+      <c r="H90" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>3223</t>
         </is>
       </c>
     </row>
@@ -3171,9 +3699,15 @@
       <c r="F91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>2023</t>
+      <c r="G91" t="n">
+        <v>2023</v>
+      </c>
+      <c r="H91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>2040</t>
         </is>
       </c>
     </row>
@@ -3202,9 +3736,15 @@
       <c r="F92" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>2660</t>
+      <c r="G92" t="n">
+        <v>2660</v>
+      </c>
+      <c r="H92" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>2694</t>
         </is>
       </c>
     </row>
@@ -3233,9 +3773,15 @@
       <c r="F93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>2797</t>
+      <c r="G93" t="n">
+        <v>2797</v>
+      </c>
+      <c r="H93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>2840</t>
         </is>
       </c>
     </row>
@@ -3264,9 +3810,15 @@
       <c r="F94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G94" t="inlineStr">
-        <is>
-          <t>2273</t>
+      <c r="G94" t="n">
+        <v>2273</v>
+      </c>
+      <c r="H94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>2276</t>
         </is>
       </c>
     </row>
@@ -3290,6 +3842,8 @@
       <c r="E95" t="inlineStr"/>
       <c r="F95" s="4" t="inlineStr"/>
       <c r="G95" t="inlineStr"/>
+      <c r="H95" s="4" t="inlineStr"/>
+      <c r="I95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -3316,9 +3870,15 @@
       <c r="F96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>2446</t>
+      <c r="G96" t="n">
+        <v>2446</v>
+      </c>
+      <c r="H96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>2442</t>
         </is>
       </c>
     </row>
@@ -3347,9 +3907,15 @@
       <c r="F97" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>3529</t>
+      <c r="G97" t="n">
+        <v>3529</v>
+      </c>
+      <c r="H97" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>3547</t>
         </is>
       </c>
     </row>
@@ -3378,9 +3944,15 @@
       <c r="F98" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>3156</t>
+      <c r="G98" t="n">
+        <v>3156</v>
+      </c>
+      <c r="H98" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>3186</t>
         </is>
       </c>
     </row>
@@ -3409,9 +3981,15 @@
       <c r="F99" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G99" t="inlineStr">
-        <is>
-          <t>3827</t>
+      <c r="G99" t="n">
+        <v>3827</v>
+      </c>
+      <c r="H99" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>3924</t>
         </is>
       </c>
     </row>
@@ -3440,9 +4018,15 @@
       <c r="F100" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G100" t="inlineStr">
-        <is>
-          <t>3547</t>
+      <c r="G100" t="n">
+        <v>3547</v>
+      </c>
+      <c r="H100" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>3702</t>
         </is>
       </c>
     </row>
@@ -3471,9 +4055,15 @@
       <c r="F101" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="G101" t="inlineStr">
-        <is>
-          <t>3147</t>
+      <c r="G101" t="n">
+        <v>3147</v>
+      </c>
+      <c r="H101" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>3445</t>
         </is>
       </c>
     </row>
@@ -3502,9 +4092,15 @@
       <c r="F102" s="3" t="n">
         <v>34</v>
       </c>
-      <c r="G102" t="inlineStr">
-        <is>
-          <t>3911</t>
+      <c r="G102" t="n">
+        <v>3911</v>
+      </c>
+      <c r="H102" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>4032</t>
         </is>
       </c>
     </row>
@@ -3533,9 +4129,15 @@
       <c r="F103" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="G103" t="inlineStr">
-        <is>
-          <t>3467</t>
+      <c r="G103" t="n">
+        <v>3467</v>
+      </c>
+      <c r="H103" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>3728</t>
         </is>
       </c>
     </row>
@@ -3564,9 +4166,15 @@
       <c r="F104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G104" t="inlineStr">
-        <is>
-          <t>2485</t>
+      <c r="G104" t="n">
+        <v>2485</v>
+      </c>
+      <c r="H104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>2468</t>
         </is>
       </c>
     </row>
@@ -3595,9 +4203,15 @@
       <c r="F105" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G105" t="inlineStr">
-        <is>
-          <t>4129</t>
+      <c r="G105" t="n">
+        <v>4129</v>
+      </c>
+      <c r="H105" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>4456</t>
         </is>
       </c>
     </row>
@@ -3626,9 +4240,15 @@
       <c r="F106" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="G106" t="inlineStr">
-        <is>
-          <t>3385</t>
+      <c r="G106" t="n">
+        <v>3385</v>
+      </c>
+      <c r="H106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>3539</t>
         </is>
       </c>
     </row>
@@ -3657,9 +4277,15 @@
       <c r="F107" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G107" t="inlineStr">
-        <is>
-          <t>3314</t>
+      <c r="G107" t="n">
+        <v>3314</v>
+      </c>
+      <c r="H107" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>3399</t>
         </is>
       </c>
     </row>
@@ -3688,9 +4314,15 @@
       <c r="F108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G108" t="inlineStr">
-        <is>
-          <t>2616</t>
+      <c r="G108" t="n">
+        <v>2616</v>
+      </c>
+      <c r="H108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>2630</t>
         </is>
       </c>
     </row>
@@ -3719,9 +4351,15 @@
       <c r="F109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G109" t="inlineStr">
-        <is>
-          <t>3077</t>
+      <c r="G109" t="n">
+        <v>3077</v>
+      </c>
+      <c r="H109" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>3390</t>
         </is>
       </c>
     </row>
@@ -3750,9 +4388,15 @@
       <c r="F110" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G110" t="inlineStr">
-        <is>
-          <t>3081</t>
+      <c r="G110" t="n">
+        <v>3081</v>
+      </c>
+      <c r="H110" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>3228</t>
         </is>
       </c>
     </row>
@@ -3781,9 +4425,15 @@
       <c r="F111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G111" t="inlineStr">
-        <is>
-          <t>3292</t>
+      <c r="G111" t="n">
+        <v>3292</v>
+      </c>
+      <c r="H111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>3352</t>
         </is>
       </c>
     </row>
@@ -3812,9 +4462,15 @@
       <c r="F112" s="4" t="n">
         <v>26</v>
       </c>
-      <c r="G112" t="inlineStr">
-        <is>
-          <t>3658</t>
+      <c r="G112" t="n">
+        <v>3658</v>
+      </c>
+      <c r="H112" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>3926</t>
         </is>
       </c>
     </row>
@@ -3843,9 +4499,15 @@
       <c r="F113" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="G113" t="inlineStr">
-        <is>
-          <t>2477</t>
+      <c r="G113" t="n">
+        <v>2477</v>
+      </c>
+      <c r="H113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>2463</t>
         </is>
       </c>
     </row>
@@ -3874,9 +4536,15 @@
       <c r="F114" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="G114" t="inlineStr">
-        <is>
-          <t>2598</t>
+      <c r="G114" t="n">
+        <v>2598</v>
+      </c>
+      <c r="H114" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>2645</t>
         </is>
       </c>
     </row>
@@ -3905,9 +4573,15 @@
       <c r="F115" s="5" t="n">
         <v>13</v>
       </c>
-      <c r="G115" t="inlineStr">
-        <is>
-          <t>3094</t>
+      <c r="G115" t="n">
+        <v>3094</v>
+      </c>
+      <c r="H115" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>3319</t>
         </is>
       </c>
     </row>
@@ -3936,9 +4610,15 @@
       <c r="F116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G116" t="inlineStr">
-        <is>
-          <t>2682</t>
+      <c r="G116" t="n">
+        <v>2682</v>
+      </c>
+      <c r="H116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>2737</t>
         </is>
       </c>
     </row>
@@ -3967,9 +4647,15 @@
       <c r="F117" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G117" t="inlineStr">
-        <is>
-          <t>3323</t>
+      <c r="G117" t="n">
+        <v>3323</v>
+      </c>
+      <c r="H117" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>3361</t>
         </is>
       </c>
     </row>
@@ -3998,9 +4684,15 @@
       <c r="F118" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G118" t="inlineStr">
-        <is>
-          <t>3016</t>
+      <c r="G118" t="n">
+        <v>3016</v>
+      </c>
+      <c r="H118" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>3113</t>
         </is>
       </c>
     </row>
@@ -4029,9 +4721,15 @@
       <c r="F119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G119" t="inlineStr">
-        <is>
-          <t>3260</t>
+      <c r="G119" t="n">
+        <v>3260</v>
+      </c>
+      <c r="H119" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>3369</t>
         </is>
       </c>
     </row>
@@ -4060,9 +4758,15 @@
       <c r="F120" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="G120" t="inlineStr">
-        <is>
-          <t>2640</t>
+      <c r="G120" t="n">
+        <v>2640</v>
+      </c>
+      <c r="H120" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>2703</t>
         </is>
       </c>
     </row>
@@ -4091,9 +4795,15 @@
       <c r="F121" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G121" t="inlineStr">
-        <is>
-          <t>3032</t>
+      <c r="G121" t="n">
+        <v>3032</v>
+      </c>
+      <c r="H121" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>3046</t>
         </is>
       </c>
     </row>
@@ -4122,9 +4832,15 @@
       <c r="F122" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="G122" t="inlineStr">
-        <is>
-          <t>3046</t>
+      <c r="G122" t="n">
+        <v>3046</v>
+      </c>
+      <c r="H122" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I122" t="inlineStr">
+        <is>
+          <t>3085</t>
         </is>
       </c>
     </row>
@@ -4153,9 +4869,15 @@
       <c r="F123" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G123" t="inlineStr">
-        <is>
-          <t>3331</t>
+      <c r="G123" t="n">
+        <v>3331</v>
+      </c>
+      <c r="H123" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>3446</t>
         </is>
       </c>
     </row>
@@ -4184,9 +4906,15 @@
       <c r="F124" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G124" t="inlineStr">
-        <is>
-          <t>3032</t>
+      <c r="G124" t="n">
+        <v>3032</v>
+      </c>
+      <c r="H124" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>2951</t>
         </is>
       </c>
     </row>
@@ -4215,7 +4943,13 @@
       <c r="F125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G125" t="inlineStr">
+      <c r="G125" t="n">
+        <v>2119</v>
+      </c>
+      <c r="H125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I125" t="inlineStr">
         <is>
           <t>2119</t>
         </is>
@@ -4246,9 +4980,15 @@
       <c r="F126" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="G126" t="inlineStr">
-        <is>
-          <t>2701</t>
+      <c r="G126" t="n">
+        <v>2701</v>
+      </c>
+      <c r="H126" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I126" t="inlineStr">
+        <is>
+          <t>2652</t>
         </is>
       </c>
     </row>
@@ -4277,9 +5017,15 @@
       <c r="F127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G127" t="inlineStr">
-        <is>
-          <t>2452</t>
+      <c r="G127" t="n">
+        <v>2452</v>
+      </c>
+      <c r="H127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I127" t="inlineStr">
+        <is>
+          <t>2416</t>
         </is>
       </c>
     </row>
@@ -4308,9 +5054,15 @@
       <c r="F128" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G128" t="inlineStr">
-        <is>
-          <t>4075</t>
+      <c r="G128" t="n">
+        <v>4075</v>
+      </c>
+      <c r="H128" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I128" t="inlineStr">
+        <is>
+          <t>4325</t>
         </is>
       </c>
     </row>
@@ -4334,6 +5086,8 @@
       <c r="E129" t="inlineStr"/>
       <c r="F129" s="4" t="inlineStr"/>
       <c r="G129" t="inlineStr"/>
+      <c r="H129" s="4" t="inlineStr"/>
+      <c r="I129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="n">
@@ -4360,9 +5114,15 @@
       <c r="F130" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G130" t="inlineStr">
-        <is>
-          <t>2674</t>
+      <c r="G130" t="n">
+        <v>2674</v>
+      </c>
+      <c r="H130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I130" t="inlineStr">
+        <is>
+          <t>2658</t>
         </is>
       </c>
     </row>
@@ -4391,9 +5151,15 @@
       <c r="F131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G131" t="inlineStr">
-        <is>
-          <t>2721</t>
+      <c r="G131" t="n">
+        <v>2721</v>
+      </c>
+      <c r="H131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I131" t="inlineStr">
+        <is>
+          <t>2747</t>
         </is>
       </c>
     </row>
@@ -4422,9 +5188,15 @@
       <c r="F132" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G132" t="inlineStr">
-        <is>
-          <t>3337</t>
+      <c r="G132" t="n">
+        <v>3337</v>
+      </c>
+      <c r="H132" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I132" t="inlineStr">
+        <is>
+          <t>3461</t>
         </is>
       </c>
     </row>
@@ -4448,6 +5220,8 @@
       <c r="E133" t="inlineStr"/>
       <c r="F133" s="4" t="inlineStr"/>
       <c r="G133" t="inlineStr"/>
+      <c r="H133" s="4" t="inlineStr"/>
+      <c r="I133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="n">
@@ -4474,9 +5248,15 @@
       <c r="F134" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="G134" t="inlineStr">
-        <is>
-          <t>2665</t>
+      <c r="G134" t="n">
+        <v>2665</v>
+      </c>
+      <c r="H134" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="I134" t="inlineStr">
+        <is>
+          <t>2690</t>
         </is>
       </c>
     </row>
@@ -4505,9 +5285,15 @@
       <c r="F135" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G135" t="inlineStr">
-        <is>
-          <t>2479</t>
+      <c r="G135" t="n">
+        <v>2479</v>
+      </c>
+      <c r="H135" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I135" t="inlineStr">
+        <is>
+          <t>2468</t>
         </is>
       </c>
     </row>
@@ -4536,9 +5322,15 @@
       <c r="F136" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="G136" t="inlineStr">
-        <is>
-          <t>2687</t>
+      <c r="G136" t="n">
+        <v>2687</v>
+      </c>
+      <c r="H136" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="I136" t="inlineStr">
+        <is>
+          <t>2761</t>
         </is>
       </c>
     </row>
@@ -4567,9 +5359,15 @@
       <c r="F137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G137" t="inlineStr">
-        <is>
-          <t>2063</t>
+      <c r="G137" t="n">
+        <v>2063</v>
+      </c>
+      <c r="H137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I137" t="inlineStr">
+        <is>
+          <t>2103</t>
         </is>
       </c>
     </row>
@@ -4593,6 +5391,8 @@
       <c r="E138" t="inlineStr"/>
       <c r="F138" s="4" t="inlineStr"/>
       <c r="G138" t="inlineStr"/>
+      <c r="H138" s="4" t="inlineStr"/>
+      <c r="I138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -4614,6 +5414,8 @@
       <c r="E139" t="inlineStr"/>
       <c r="F139" s="4" t="inlineStr"/>
       <c r="G139" t="inlineStr"/>
+      <c r="H139" s="4" t="inlineStr"/>
+      <c r="I139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -4635,6 +5437,8 @@
       <c r="E140" t="inlineStr"/>
       <c r="F140" s="4" t="inlineStr"/>
       <c r="G140" t="inlineStr"/>
+      <c r="H140" s="4" t="inlineStr"/>
+      <c r="I140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="n">
@@ -4661,9 +5465,15 @@
       <c r="F141" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G141" t="inlineStr">
-        <is>
-          <t>2009</t>
+      <c r="G141" t="n">
+        <v>2009</v>
+      </c>
+      <c r="H141" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I141" t="inlineStr">
+        <is>
+          <t>1999</t>
         </is>
       </c>
     </row>
@@ -4687,6 +5497,8 @@
       <c r="E142" t="inlineStr"/>
       <c r="F142" s="4" t="inlineStr"/>
       <c r="G142" t="inlineStr"/>
+      <c r="H142" s="4" t="inlineStr"/>
+      <c r="I142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="n">
@@ -4708,6 +5520,8 @@
       <c r="E143" t="inlineStr"/>
       <c r="F143" s="4" t="inlineStr"/>
       <c r="G143" t="inlineStr"/>
+      <c r="H143" s="4" t="inlineStr"/>
+      <c r="I143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -4729,6 +5543,8 @@
       <c r="E144" t="inlineStr"/>
       <c r="F144" s="4" t="inlineStr"/>
       <c r="G144" t="inlineStr"/>
+      <c r="H144" s="4" t="inlineStr"/>
+      <c r="I144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -4750,6 +5566,8 @@
       <c r="E145" t="inlineStr"/>
       <c r="F145" s="4" t="inlineStr"/>
       <c r="G145" t="inlineStr"/>
+      <c r="H145" s="4" t="inlineStr"/>
+      <c r="I145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -4771,6 +5589,8 @@
       <c r="E146" t="inlineStr"/>
       <c r="F146" s="4" t="inlineStr"/>
       <c r="G146" t="inlineStr"/>
+      <c r="H146" s="4" t="inlineStr"/>
+      <c r="I146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -4792,6 +5612,8 @@
       <c r="E147" t="inlineStr"/>
       <c r="F147" s="4" t="inlineStr"/>
       <c r="G147" t="inlineStr"/>
+      <c r="H147" s="4" t="inlineStr"/>
+      <c r="I147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -4813,6 +5635,8 @@
       <c r="E148" t="inlineStr"/>
       <c r="F148" s="4" t="inlineStr"/>
       <c r="G148" t="inlineStr"/>
+      <c r="H148" s="4" t="inlineStr"/>
+      <c r="I148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="n">
@@ -4834,6 +5658,8 @@
       <c r="E149" t="inlineStr"/>
       <c r="F149" s="4" t="inlineStr"/>
       <c r="G149" t="inlineStr"/>
+      <c r="H149" s="4" t="inlineStr"/>
+      <c r="I149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="n">
@@ -4855,6 +5681,8 @@
       <c r="E150" t="inlineStr"/>
       <c r="F150" s="4" t="inlineStr"/>
       <c r="G150" t="inlineStr"/>
+      <c r="H150" s="4" t="inlineStr"/>
+      <c r="I150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="n">
@@ -4876,6 +5704,8 @@
       <c r="E151" t="inlineStr"/>
       <c r="F151" s="4" t="inlineStr"/>
       <c r="G151" t="inlineStr"/>
+      <c r="H151" s="4" t="inlineStr"/>
+      <c r="I151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="n">
@@ -4897,6 +5727,8 @@
       <c r="E152" t="inlineStr"/>
       <c r="F152" s="4" t="inlineStr"/>
       <c r="G152" t="inlineStr"/>
+      <c r="H152" s="4" t="inlineStr"/>
+      <c r="I152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" t="n">
@@ -4918,6 +5750,8 @@
       <c r="E153" t="inlineStr"/>
       <c r="F153" s="4" t="inlineStr"/>
       <c r="G153" t="inlineStr"/>
+      <c r="H153" s="4" t="inlineStr"/>
+      <c r="I153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" t="n">
@@ -4944,9 +5778,15 @@
       <c r="F154" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="G154" t="inlineStr">
-        <is>
-          <t>1956</t>
+      <c r="G154" t="n">
+        <v>1956</v>
+      </c>
+      <c r="H154" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="I154" t="inlineStr">
+        <is>
+          <t>2152</t>
         </is>
       </c>
     </row>
@@ -4970,6 +5810,8 @@
       <c r="E155" t="inlineStr"/>
       <c r="F155" s="4" t="inlineStr"/>
       <c r="G155" t="inlineStr"/>
+      <c r="H155" s="4" t="inlineStr"/>
+      <c r="I155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="n">
@@ -4996,9 +5838,15 @@
       <c r="F156" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G156" t="inlineStr">
-        <is>
-          <t>3700</t>
+      <c r="G156" t="n">
+        <v>3700</v>
+      </c>
+      <c r="H156" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="I156" t="inlineStr">
+        <is>
+          <t>4022</t>
         </is>
       </c>
     </row>
@@ -5027,7 +5875,13 @@
       <c r="F157" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G157" t="inlineStr">
+      <c r="G157" t="n">
+        <v>0</v>
+      </c>
+      <c r="H157" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I157" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5058,7 +5912,13 @@
       <c r="F158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G158" t="inlineStr">
+      <c r="G158" t="n">
+        <v>2500</v>
+      </c>
+      <c r="H158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I158" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -5089,9 +5949,15 @@
       <c r="F159" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="G159" t="inlineStr">
-        <is>
-          <t>4144</t>
+      <c r="G159" t="n">
+        <v>4144</v>
+      </c>
+      <c r="H159" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I159" t="inlineStr">
+        <is>
+          <t>4411</t>
         </is>
       </c>
     </row>
@@ -5120,7 +5986,13 @@
       <c r="F160" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G160" t="inlineStr">
+      <c r="G160" t="n">
+        <v>0</v>
+      </c>
+      <c r="H160" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I160" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5151,9 +6023,15 @@
       <c r="F161" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G161" t="inlineStr">
-        <is>
-          <t>2919</t>
+      <c r="G161" t="n">
+        <v>2919</v>
+      </c>
+      <c r="H161" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I161" t="inlineStr">
+        <is>
+          <t>3066</t>
         </is>
       </c>
     </row>
@@ -5182,7 +6060,13 @@
       <c r="F162" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G162" t="inlineStr">
+      <c r="G162" t="n">
+        <v>0</v>
+      </c>
+      <c r="H162" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I162" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5213,17 +6097,21 @@
       <c r="F163" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G163" t="inlineStr">
-        <is>
-          <t>2742</t>
+      <c r="G163" t="n">
+        <v>2742</v>
+      </c>
+      <c r="H163" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I163" t="inlineStr">
+        <is>
+          <t>2802</t>
         </is>
       </c>
     </row>
     <row r="164">
-      <c r="A164" t="inlineStr">
-        <is>
-          <t>56829330</t>
-        </is>
+      <c r="A164" t="n">
+        <v>56829330</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
@@ -5240,17 +6128,21 @@
       <c r="F164" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="G164" t="inlineStr">
-        <is>
-          <t>2906</t>
+      <c r="G164" t="n">
+        <v>2906</v>
+      </c>
+      <c r="H164" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="I164" t="inlineStr">
+        <is>
+          <t>2931</t>
         </is>
       </c>
     </row>
     <row r="165">
-      <c r="A165" t="inlineStr">
-        <is>
-          <t>9321819</t>
-        </is>
+      <c r="A165" t="n">
+        <v>9321819</v>
       </c>
       <c r="B165" t="inlineStr">
         <is>
@@ -5267,17 +6159,21 @@
       <c r="F165" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G165" t="inlineStr">
-        <is>
-          <t>2807</t>
+      <c r="G165" t="n">
+        <v>2807</v>
+      </c>
+      <c r="H165" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="I165" t="inlineStr">
+        <is>
+          <t>2847</t>
         </is>
       </c>
     </row>
     <row r="166">
-      <c r="A166" t="inlineStr">
-        <is>
-          <t>15436348</t>
-        </is>
+      <c r="A166" t="n">
+        <v>15436348</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>
@@ -5294,17 +6190,21 @@
       <c r="F166" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G166" t="inlineStr">
-        <is>
-          <t>1805</t>
+      <c r="G166" t="n">
+        <v>1805</v>
+      </c>
+      <c r="H166" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I166" t="inlineStr">
+        <is>
+          <t>1798</t>
         </is>
       </c>
     </row>
     <row r="167">
-      <c r="A167" t="inlineStr">
-        <is>
-          <t>58615957</t>
-        </is>
+      <c r="A167" t="n">
+        <v>58615957</v>
       </c>
       <c r="B167" t="inlineStr">
         <is>
@@ -5321,17 +6221,21 @@
       <c r="F167" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G167" t="inlineStr">
-        <is>
-          <t>2446</t>
+      <c r="G167" t="n">
+        <v>2446</v>
+      </c>
+      <c r="H167" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I167" t="inlineStr">
+        <is>
+          <t>2530</t>
         </is>
       </c>
     </row>
     <row r="168">
-      <c r="A168" t="inlineStr">
-        <is>
-          <t>27113069</t>
-        </is>
+      <c r="A168" t="n">
+        <v>27113069</v>
       </c>
       <c r="B168" t="inlineStr">
         <is>
@@ -5348,17 +6252,21 @@
       <c r="F168" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="G168" t="inlineStr">
-        <is>
-          <t>4584</t>
+      <c r="G168" t="n">
+        <v>4584</v>
+      </c>
+      <c r="H168" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="I168" t="inlineStr">
+        <is>
+          <t>4631</t>
         </is>
       </c>
     </row>
     <row r="169">
-      <c r="A169" t="inlineStr">
-        <is>
-          <t>47533851</t>
-        </is>
+      <c r="A169" t="n">
+        <v>47533851</v>
       </c>
       <c r="B169" t="inlineStr">
         <is>
@@ -5375,17 +6283,21 @@
       <c r="F169" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G169" t="inlineStr">
-        <is>
-          <t>2198</t>
+      <c r="G169" t="n">
+        <v>2198</v>
+      </c>
+      <c r="H169" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I169" t="inlineStr">
+        <is>
+          <t>2315</t>
         </is>
       </c>
     </row>
     <row r="170">
-      <c r="A170" t="inlineStr">
-        <is>
-          <t>47928278</t>
-        </is>
+      <c r="A170" t="n">
+        <v>47928278</v>
       </c>
       <c r="B170" t="inlineStr">
         <is>
@@ -5402,17 +6314,21 @@
       <c r="F170" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="G170" t="inlineStr">
-        <is>
-          <t>5055</t>
+      <c r="G170" t="n">
+        <v>5055</v>
+      </c>
+      <c r="H170" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="I170" t="inlineStr">
+        <is>
+          <t>5307</t>
         </is>
       </c>
     </row>
     <row r="171">
-      <c r="A171" t="inlineStr">
-        <is>
-          <t>50742014</t>
-        </is>
+      <c r="A171" t="n">
+        <v>50742014</v>
       </c>
       <c r="B171" t="inlineStr">
         <is>
@@ -5429,17 +6345,21 @@
       <c r="F171" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G171" t="inlineStr">
-        <is>
-          <t>999</t>
+      <c r="G171" t="n">
+        <v>999</v>
+      </c>
+      <c r="H171" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I171" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="172">
-      <c r="A172" t="inlineStr">
-        <is>
-          <t>53269862</t>
-        </is>
+      <c r="A172" t="n">
+        <v>53269862</v>
       </c>
       <c r="B172" t="inlineStr">
         <is>
@@ -5456,17 +6376,21 @@
       <c r="F172" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="G172" t="inlineStr">
-        <is>
-          <t>1680</t>
+      <c r="G172" t="n">
+        <v>1680</v>
+      </c>
+      <c r="H172" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I172" t="inlineStr">
+        <is>
+          <t>2043</t>
         </is>
       </c>
     </row>
     <row r="173">
-      <c r="A173" t="inlineStr">
-        <is>
-          <t>54924790</t>
-        </is>
+      <c r="A173" t="n">
+        <v>54924790</v>
       </c>
       <c r="B173" t="inlineStr">
         <is>
@@ -5483,17 +6407,21 @@
       <c r="F173" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G173" t="inlineStr">
-        <is>
-          <t>2924</t>
+      <c r="G173" t="n">
+        <v>2924</v>
+      </c>
+      <c r="H173" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I173" t="inlineStr">
+        <is>
+          <t>2906</t>
         </is>
       </c>
     </row>
     <row r="174">
-      <c r="A174" t="inlineStr">
-        <is>
-          <t>55963040</t>
-        </is>
+      <c r="A174" t="n">
+        <v>55963040</v>
       </c>
       <c r="B174" t="inlineStr">
         <is>
@@ -5510,17 +6438,21 @@
       <c r="F174" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G174" t="inlineStr">
-        <is>
-          <t>2450</t>
+      <c r="G174" t="n">
+        <v>2450</v>
+      </c>
+      <c r="H174" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I174" t="inlineStr">
+        <is>
+          <t>2430</t>
         </is>
       </c>
     </row>
     <row r="175">
-      <c r="A175" t="inlineStr">
-        <is>
-          <t>58132159</t>
-        </is>
+      <c r="A175" t="n">
+        <v>58132159</v>
       </c>
       <c r="B175" t="inlineStr">
         <is>
@@ -5537,17 +6469,21 @@
       <c r="F175" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G175" t="inlineStr">
-        <is>
-          <t>1514</t>
+      <c r="G175" t="n">
+        <v>1514</v>
+      </c>
+      <c r="H175" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I175" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="176">
-      <c r="A176" t="inlineStr">
-        <is>
-          <t>58562596</t>
-        </is>
+      <c r="A176" t="n">
+        <v>58562596</v>
       </c>
       <c r="B176" t="inlineStr">
         <is>
@@ -5564,17 +6500,21 @@
       <c r="F176" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G176" t="inlineStr">
+      <c r="G176" t="n">
+        <v>0</v>
+      </c>
+      <c r="H176" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I176" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
     </row>
     <row r="177">
-      <c r="A177" t="inlineStr">
-        <is>
-          <t>58615925</t>
-        </is>
+      <c r="A177" t="n">
+        <v>58615925</v>
       </c>
       <c r="B177" t="inlineStr">
         <is>
@@ -5591,17 +6531,21 @@
       <c r="F177" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G177" t="inlineStr">
-        <is>
-          <t>2583</t>
+      <c r="G177" t="n">
+        <v>2583</v>
+      </c>
+      <c r="H177" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I177" t="inlineStr">
+        <is>
+          <t>2608</t>
         </is>
       </c>
     </row>
     <row r="178">
-      <c r="A178" t="inlineStr">
-        <is>
-          <t>48005945</t>
-        </is>
+      <c r="A178" t="n">
+        <v>48005945</v>
       </c>
       <c r="B178" t="inlineStr">
         <is>
@@ -5618,9 +6562,102 @@
       <c r="F178" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G178" t="inlineStr">
-        <is>
-          <t>2541</t>
+      <c r="G178" t="n">
+        <v>2541</v>
+      </c>
+      <c r="H178" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="I178" t="inlineStr">
+        <is>
+          <t>2716</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>12333251</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>"㊌ Mingxuan"</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr"/>
+      <c r="D179" t="inlineStr"/>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F179" s="4" t="inlineStr"/>
+      <c r="G179" t="inlineStr"/>
+      <c r="H179" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I179" t="inlineStr">
+        <is>
+          <t>2997</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>26497650</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>mithun</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr"/>
+      <c r="D180" t="inlineStr"/>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F180" s="4" t="inlineStr"/>
+      <c r="G180" t="inlineStr"/>
+      <c r="H180" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="I180" t="inlineStr">
+        <is>
+          <t>2697</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>56691087</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>LongestSovereign8</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr"/>
+      <c r="D181" t="inlineStr"/>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F181" s="4" t="inlineStr"/>
+      <c r="G181" t="inlineStr"/>
+      <c r="H181" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="I181" t="inlineStr">
+        <is>
+          <t>1887</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-01-26 11:32:31
</commit_message>
<xml_diff>
--- a/Season_Attack/82.xlsx
+++ b/Season_Attack/82.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I181"/>
+  <dimension ref="A1:G186"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -418,22 +418,12 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>01-21_A</t>
+          <t>01-25_A</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>01-21_0</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>01-22_A</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>01-22_0</t>
+          <t>01-25_0</t>
         </is>
       </c>
     </row>
@@ -462,15 +452,9 @@
       <c r="F2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G2" t="n">
-        <v>3481</v>
-      </c>
-      <c r="H2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>3531</t>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>3838</t>
         </is>
       </c>
     </row>
@@ -497,17 +481,11 @@
         </is>
       </c>
       <c r="F3" s="3" t="n">
-        <v>33</v>
-      </c>
-      <c r="G3" t="n">
-        <v>4691</v>
-      </c>
-      <c r="H3" s="3" t="n">
-        <v>35</v>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>4897</t>
+        <v>36</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>5730</t>
         </is>
       </c>
     </row>
@@ -536,15 +514,9 @@
       <c r="F4" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G4" t="n">
-        <v>4441</v>
-      </c>
-      <c r="H4" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>4746</t>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>5617</t>
         </is>
       </c>
     </row>
@@ -571,17 +543,11 @@
         </is>
       </c>
       <c r="F5" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="G5" t="n">
-        <v>4366</v>
-      </c>
-      <c r="H5" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>4678</t>
+        <v>24</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>5574</t>
         </is>
       </c>
     </row>
@@ -607,18 +573,12 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F6" s="4" t="n">
-        <v>27</v>
-      </c>
-      <c r="G6" t="n">
-        <v>4698</v>
-      </c>
-      <c r="H6" s="3" t="n">
-        <v>34</v>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>4962</t>
+      <c r="F6" s="3" t="n">
+        <v>33</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>5628</t>
         </is>
       </c>
     </row>
@@ -647,15 +607,9 @@
       <c r="F7" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G7" t="n">
-        <v>4368</v>
-      </c>
-      <c r="H7" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>4641</t>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>5157</t>
         </is>
       </c>
     </row>
@@ -684,15 +638,9 @@
       <c r="F8" s="3" t="n">
         <v>31</v>
       </c>
-      <c r="G8" t="n">
-        <v>3918</v>
-      </c>
-      <c r="H8" s="4" t="n">
-        <v>30</v>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>4137</t>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>5444</t>
         </is>
       </c>
     </row>
@@ -716,8 +664,6 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" s="4" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
-      <c r="H9" s="4" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -744,15 +690,9 @@
       <c r="F10" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="G10" t="n">
-        <v>4520</v>
-      </c>
-      <c r="H10" s="3" t="n">
-        <v>40</v>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>4542</t>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>5099</t>
         </is>
       </c>
     </row>
@@ -778,18 +718,12 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F11" s="4" t="n">
-        <v>30</v>
-      </c>
-      <c r="G11" t="n">
-        <v>4674</v>
-      </c>
-      <c r="H11" s="3" t="n">
-        <v>34</v>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>5218</t>
+      <c r="F11" s="3" t="n">
+        <v>38</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>6285</t>
         </is>
       </c>
     </row>
@@ -816,17 +750,11 @@
         </is>
       </c>
       <c r="F12" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="G12" t="n">
-        <v>4125</v>
-      </c>
-      <c r="H12" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>4309</t>
+        <v>23</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>5404</t>
         </is>
       </c>
     </row>
@@ -853,17 +781,11 @@
         </is>
       </c>
       <c r="F13" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="G13" t="n">
-        <v>2879</v>
-      </c>
-      <c r="H13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>2903</t>
+        <v>3</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>3047</t>
         </is>
       </c>
     </row>
@@ -890,17 +812,11 @@
         </is>
       </c>
       <c r="F14" s="3" t="n">
-        <v>39</v>
-      </c>
-      <c r="G14" t="n">
-        <v>5341</v>
-      </c>
-      <c r="H14" s="3" t="n">
-        <v>38</v>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>5641</t>
+        <v>37</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>6563</t>
         </is>
       </c>
     </row>
@@ -927,17 +843,11 @@
         </is>
       </c>
       <c r="F15" s="4" t="n">
-        <v>25</v>
-      </c>
-      <c r="G15" t="n">
-        <v>4559</v>
-      </c>
-      <c r="H15" s="4" t="n">
-        <v>23</v>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>4783</t>
+        <v>20</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>5442</t>
         </is>
       </c>
     </row>
@@ -964,17 +874,11 @@
         </is>
       </c>
       <c r="F16" s="3" t="n">
-        <v>31</v>
-      </c>
-      <c r="G16" t="n">
-        <v>4776</v>
-      </c>
-      <c r="H16" s="3" t="n">
-        <v>31</v>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>4843</t>
+        <v>36</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>6000</t>
         </is>
       </c>
     </row>
@@ -1001,17 +905,11 @@
         </is>
       </c>
       <c r="F17" s="4" t="n">
-        <v>22</v>
-      </c>
-      <c r="G17" t="n">
-        <v>4203</v>
-      </c>
-      <c r="H17" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>4378</t>
+        <v>29</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>5060</t>
         </is>
       </c>
     </row>
@@ -1040,15 +938,9 @@
       <c r="F18" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G18" t="n">
-        <v>4262</v>
-      </c>
-      <c r="H18" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>4619</t>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>5588</t>
         </is>
       </c>
     </row>
@@ -1077,15 +969,9 @@
       <c r="F19" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="G19" t="n">
-        <v>5215</v>
-      </c>
-      <c r="H19" s="3" t="n">
-        <v>33</v>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>5441</t>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>6394</t>
         </is>
       </c>
     </row>
@@ -1112,17 +998,11 @@
         </is>
       </c>
       <c r="F20" s="4" t="n">
-        <v>21</v>
-      </c>
-      <c r="G20" t="n">
-        <v>4083</v>
-      </c>
-      <c r="H20" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>4406</t>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>5322</t>
         </is>
       </c>
     </row>
@@ -1149,17 +1029,11 @@
         </is>
       </c>
       <c r="F21" s="3" t="n">
-        <v>39</v>
-      </c>
-      <c r="G21" t="n">
-        <v>4561</v>
-      </c>
-      <c r="H21" s="3" t="n">
-        <v>40</v>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>4884</t>
+        <v>38</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>5502</t>
         </is>
       </c>
     </row>
@@ -1185,18 +1059,12 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F22" s="4" t="n">
-        <v>29</v>
-      </c>
-      <c r="G22" t="n">
-        <v>2866</v>
-      </c>
-      <c r="H22" s="3" t="n">
-        <v>33</v>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>3579</t>
+      <c r="F22" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>4531</t>
         </is>
       </c>
     </row>
@@ -1225,15 +1093,9 @@
       <c r="F23" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="G23" t="n">
-        <v>4641</v>
-      </c>
-      <c r="H23" s="3" t="n">
-        <v>32</v>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>4965</t>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>5727</t>
         </is>
       </c>
     </row>
@@ -1262,13 +1124,7 @@
       <c r="F24" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G24" t="n">
-        <v>0</v>
-      </c>
-      <c r="H24" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I24" t="inlineStr">
+      <c r="G24" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1299,15 +1155,9 @@
       <c r="F25" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="G25" t="n">
-        <v>4523</v>
-      </c>
-      <c r="H25" s="3" t="n">
-        <v>40</v>
-      </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>4625</t>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>5355</t>
         </is>
       </c>
     </row>
@@ -1334,17 +1184,11 @@
         </is>
       </c>
       <c r="F26" s="3" t="n">
-        <v>35</v>
-      </c>
-      <c r="G26" t="n">
-        <v>4788</v>
-      </c>
-      <c r="H26" s="3" t="n">
-        <v>32</v>
-      </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>5184</t>
+        <v>38</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>5908</t>
         </is>
       </c>
     </row>
@@ -1373,15 +1217,9 @@
       <c r="F27" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="G27" t="n">
-        <v>3870</v>
-      </c>
-      <c r="H27" s="4" t="n">
-        <v>27</v>
-      </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>3950</t>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>5163</t>
         </is>
       </c>
     </row>
@@ -1410,15 +1248,9 @@
       <c r="F28" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="G28" t="n">
-        <v>5108</v>
-      </c>
-      <c r="H28" s="3" t="n">
-        <v>40</v>
-      </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>5456</t>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>6225</t>
         </is>
       </c>
     </row>
@@ -1445,17 +1277,11 @@
         </is>
       </c>
       <c r="F29" s="4" t="n">
-        <v>29</v>
-      </c>
-      <c r="G29" t="n">
-        <v>4510</v>
-      </c>
-      <c r="H29" s="4" t="n">
         <v>28</v>
       </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>4713</t>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>5329</t>
         </is>
       </c>
     </row>
@@ -1482,17 +1308,11 @@
         </is>
       </c>
       <c r="F30" s="3" t="n">
-        <v>31</v>
-      </c>
-      <c r="G30" t="n">
-        <v>4706</v>
-      </c>
-      <c r="H30" s="3" t="n">
-        <v>38</v>
-      </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>5160</t>
+        <v>39</v>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>6198</t>
         </is>
       </c>
     </row>
@@ -1518,18 +1338,12 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F31" s="3" t="n">
-        <v>37</v>
-      </c>
-      <c r="G31" t="n">
-        <v>4975</v>
-      </c>
-      <c r="H31" s="3" t="n">
-        <v>37</v>
-      </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>5225</t>
+      <c r="F31" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>6004</t>
         </is>
       </c>
     </row>
@@ -1555,18 +1369,12 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F32" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="G32" t="n">
-        <v>2873</v>
-      </c>
-      <c r="H32" s="2" t="n">
+      <c r="F32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>2873</t>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>2919</t>
         </is>
       </c>
     </row>
@@ -1593,17 +1401,11 @@
         </is>
       </c>
       <c r="F33" s="3" t="n">
-        <v>38</v>
-      </c>
-      <c r="G33" t="n">
-        <v>4746</v>
-      </c>
-      <c r="H33" s="3" t="n">
-        <v>39</v>
-      </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>5073</t>
+        <v>37</v>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>6015</t>
         </is>
       </c>
     </row>
@@ -1629,18 +1431,12 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F34" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="G34" t="n">
-        <v>4432</v>
-      </c>
-      <c r="H34" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="I34" t="inlineStr">
-        <is>
-          <t>4717</t>
+      <c r="F34" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>5349</t>
         </is>
       </c>
     </row>
@@ -1669,15 +1465,9 @@
       <c r="F35" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="G35" t="n">
-        <v>4233</v>
-      </c>
-      <c r="H35" s="3" t="n">
-        <v>34</v>
-      </c>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>4343</t>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>5030</t>
         </is>
       </c>
     </row>
@@ -1701,8 +1491,6 @@
       <c r="E36" t="inlineStr"/>
       <c r="F36" s="4" t="inlineStr"/>
       <c r="G36" t="inlineStr"/>
-      <c r="H36" s="4" t="inlineStr"/>
-      <c r="I36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -1726,18 +1514,12 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F37" s="3" t="n">
-        <v>33</v>
-      </c>
-      <c r="G37" t="n">
-        <v>4548</v>
-      </c>
-      <c r="H37" s="3" t="n">
-        <v>31</v>
-      </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>4771</t>
+      <c r="F37" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>5405</t>
         </is>
       </c>
     </row>
@@ -1766,15 +1548,9 @@
       <c r="F38" s="3" t="n">
         <v>35</v>
       </c>
-      <c r="G38" t="n">
-        <v>4430</v>
-      </c>
-      <c r="H38" s="3" t="n">
-        <v>35</v>
-      </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>4682</t>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>5299</t>
         </is>
       </c>
     </row>
@@ -1801,17 +1577,11 @@
         </is>
       </c>
       <c r="F39" s="3" t="n">
-        <v>33</v>
-      </c>
-      <c r="G39" t="n">
-        <v>5092</v>
-      </c>
-      <c r="H39" s="3" t="n">
-        <v>35</v>
-      </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>5299</t>
+        <v>36</v>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>6136</t>
         </is>
       </c>
     </row>
@@ -1838,17 +1608,11 @@
         </is>
       </c>
       <c r="F40" s="4" t="n">
-        <v>21</v>
-      </c>
-      <c r="G40" t="n">
-        <v>4506</v>
-      </c>
-      <c r="H40" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>4738</t>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>5429</t>
         </is>
       </c>
     </row>
@@ -1875,17 +1639,11 @@
         </is>
       </c>
       <c r="F41" s="3" t="n">
-        <v>35</v>
-      </c>
-      <c r="G41" t="n">
-        <v>5076</v>
-      </c>
-      <c r="H41" s="3" t="n">
-        <v>32</v>
-      </c>
-      <c r="I41" t="inlineStr">
-        <is>
-          <t>5338</t>
+        <v>40</v>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>6215</t>
         </is>
       </c>
     </row>
@@ -1912,17 +1670,11 @@
         </is>
       </c>
       <c r="F42" s="3" t="n">
-        <v>34</v>
-      </c>
-      <c r="G42" t="n">
-        <v>4560</v>
-      </c>
-      <c r="H42" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>4552</t>
+        <v>39</v>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>5526</t>
         </is>
       </c>
     </row>
@@ -1948,18 +1700,12 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F43" s="4" t="n">
-        <v>30</v>
-      </c>
-      <c r="G43" t="n">
-        <v>2851</v>
-      </c>
-      <c r="H43" s="3" t="n">
-        <v>39</v>
-      </c>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>2920</t>
+      <c r="F43" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>3202</t>
         </is>
       </c>
     </row>
@@ -1988,15 +1734,9 @@
       <c r="F44" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="G44" t="n">
-        <v>4169</v>
-      </c>
-      <c r="H44" s="3" t="n">
-        <v>33</v>
-      </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>4351</t>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>5191</t>
         </is>
       </c>
     </row>
@@ -2017,25 +1757,9 @@
       <c r="D45" t="n">
         <v>6207</v>
       </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>三馆</t>
-        </is>
-      </c>
-      <c r="F45" s="4" t="n">
-        <v>30</v>
-      </c>
-      <c r="G45" t="n">
-        <v>4185</v>
-      </c>
-      <c r="H45" s="4" t="n">
-        <v>30</v>
-      </c>
-      <c r="I45" t="inlineStr">
-        <is>
-          <t>4238</t>
-        </is>
-      </c>
+      <c r="E45" t="inlineStr"/>
+      <c r="F45" s="4" t="inlineStr"/>
+      <c r="G45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -2062,13 +1786,7 @@
       <c r="F46" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G46" t="n">
-        <v>3085</v>
-      </c>
-      <c r="H46" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I46" t="inlineStr">
+      <c r="G46" t="inlineStr">
         <is>
           <t>3112</t>
         </is>
@@ -2097,17 +1815,11 @@
         </is>
       </c>
       <c r="F47" s="3" t="n">
-        <v>36</v>
-      </c>
-      <c r="G47" t="n">
-        <v>4824</v>
-      </c>
-      <c r="H47" s="3" t="n">
-        <v>36</v>
-      </c>
-      <c r="I47" t="inlineStr">
-        <is>
-          <t>5076</t>
+        <v>34</v>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>5817</t>
         </is>
       </c>
     </row>
@@ -2136,15 +1848,9 @@
       <c r="F48" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G48" t="n">
-        <v>4486</v>
-      </c>
-      <c r="H48" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>4522</t>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>4582</t>
         </is>
       </c>
     </row>
@@ -2173,15 +1879,9 @@
       <c r="F49" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G49" t="n">
-        <v>3416</v>
-      </c>
-      <c r="H49" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I49" t="inlineStr">
-        <is>
-          <t>3416</t>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>3445</t>
         </is>
       </c>
     </row>
@@ -2205,8 +1905,6 @@
       <c r="E50" t="inlineStr"/>
       <c r="F50" s="4" t="inlineStr"/>
       <c r="G50" t="inlineStr"/>
-      <c r="H50" s="4" t="inlineStr"/>
-      <c r="I50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -2228,8 +1926,6 @@
       <c r="E51" t="inlineStr"/>
       <c r="F51" s="4" t="inlineStr"/>
       <c r="G51" t="inlineStr"/>
-      <c r="H51" s="4" t="inlineStr"/>
-      <c r="I51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -2256,15 +1952,9 @@
       <c r="F52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G52" t="n">
-        <v>2533</v>
-      </c>
-      <c r="H52" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>2530</t>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>2574</t>
         </is>
       </c>
     </row>
@@ -2293,15 +1983,9 @@
       <c r="F53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G53" t="n">
-        <v>3117</v>
-      </c>
-      <c r="H53" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I53" t="inlineStr">
-        <is>
-          <t>3141</t>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>3353</t>
         </is>
       </c>
     </row>
@@ -2330,15 +2014,9 @@
       <c r="F54" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G54" t="n">
-        <v>2862</v>
-      </c>
-      <c r="H54" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I54" t="inlineStr">
-        <is>
-          <t>2891</t>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>2990</t>
         </is>
       </c>
     </row>
@@ -2364,18 +2042,12 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F55" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="G55" t="n">
-        <v>4456</v>
-      </c>
-      <c r="H55" s="4" t="n">
-        <v>27</v>
-      </c>
-      <c r="I55" t="inlineStr">
-        <is>
-          <t>4675</t>
+      <c r="F55" s="4" t="n">
+        <v>26</v>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>5304</t>
         </is>
       </c>
     </row>
@@ -2404,15 +2076,9 @@
       <c r="F56" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="G56" t="n">
-        <v>3675</v>
-      </c>
-      <c r="H56" s="3" t="n">
-        <v>40</v>
-      </c>
-      <c r="I56" t="inlineStr">
-        <is>
-          <t>3846</t>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>4147</t>
         </is>
       </c>
     </row>
@@ -2439,17 +2105,11 @@
         </is>
       </c>
       <c r="F57" s="4" t="n">
-        <v>21</v>
-      </c>
-      <c r="G57" t="n">
-        <v>3815</v>
-      </c>
-      <c r="H57" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="I57" t="inlineStr">
-        <is>
-          <t>3976</t>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>4383</t>
         </is>
       </c>
     </row>
@@ -2478,15 +2138,9 @@
       <c r="F58" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G58" t="n">
-        <v>4176</v>
-      </c>
-      <c r="H58" s="4" t="n">
-        <v>21</v>
-      </c>
-      <c r="I58" t="inlineStr">
-        <is>
-          <t>4408</t>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>5199</t>
         </is>
       </c>
     </row>
@@ -2513,17 +2167,11 @@
         </is>
       </c>
       <c r="F59" s="3" t="n">
-        <v>33</v>
-      </c>
-      <c r="G59" t="n">
-        <v>3787</v>
-      </c>
-      <c r="H59" s="3" t="n">
-        <v>33</v>
-      </c>
-      <c r="I59" t="inlineStr">
-        <is>
-          <t>3972</t>
+        <v>35</v>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>4472</t>
         </is>
       </c>
     </row>
@@ -2549,18 +2197,12 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F60" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="G60" t="n">
-        <v>4164</v>
-      </c>
-      <c r="H60" s="4" t="n">
+      <c r="F60" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="I60" t="inlineStr">
-        <is>
-          <t>4428</t>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>5031</t>
         </is>
       </c>
     </row>
@@ -2589,13 +2231,7 @@
       <c r="F61" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G61" t="n">
-        <v>3179</v>
-      </c>
-      <c r="H61" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I61" t="inlineStr">
+      <c r="G61" t="inlineStr">
         <is>
           <t>3179</t>
         </is>
@@ -2624,17 +2260,11 @@
         </is>
       </c>
       <c r="F62" s="4" t="n">
-        <v>21</v>
-      </c>
-      <c r="G62" t="n">
-        <v>4456</v>
-      </c>
-      <c r="H62" s="4" t="n">
-        <v>24</v>
-      </c>
-      <c r="I62" t="inlineStr">
-        <is>
-          <t>4598</t>
+        <v>23</v>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>5233</t>
         </is>
       </c>
     </row>
@@ -2660,18 +2290,12 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F63" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="G63" t="n">
-        <v>3047</v>
-      </c>
-      <c r="H63" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="I63" t="inlineStr">
-        <is>
-          <t>3381</t>
+      <c r="F63" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>3749</t>
         </is>
       </c>
     </row>
@@ -2697,18 +2321,12 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F64" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G64" t="n">
-        <v>2932</v>
-      </c>
-      <c r="H64" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I64" t="inlineStr">
-        <is>
-          <t>2907</t>
+      <c r="F64" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>3357</t>
         </is>
       </c>
     </row>
@@ -2737,15 +2355,9 @@
       <c r="F65" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="G65" t="n">
-        <v>4218</v>
-      </c>
-      <c r="H65" s="4" t="n">
-        <v>23</v>
-      </c>
-      <c r="I65" t="inlineStr">
-        <is>
-          <t>4393</t>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>4940</t>
         </is>
       </c>
     </row>
@@ -2774,15 +2386,9 @@
       <c r="F66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G66" t="n">
-        <v>2663</v>
-      </c>
-      <c r="H66" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I66" t="inlineStr">
-        <is>
-          <t>2693</t>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>2753</t>
         </is>
       </c>
     </row>
@@ -2809,17 +2415,11 @@
         </is>
       </c>
       <c r="F67" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="G67" t="n">
-        <v>4652</v>
-      </c>
-      <c r="H67" s="4" t="n">
-        <v>29</v>
-      </c>
-      <c r="I67" t="inlineStr">
-        <is>
-          <t>4747</t>
+        <v>28</v>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>5618</t>
         </is>
       </c>
     </row>
@@ -2846,17 +2446,11 @@
         </is>
       </c>
       <c r="F68" s="3" t="n">
-        <v>32</v>
-      </c>
-      <c r="G68" t="n">
-        <v>3799</v>
-      </c>
-      <c r="H68" s="3" t="n">
-        <v>34</v>
-      </c>
-      <c r="I68" t="inlineStr">
-        <is>
-          <t>4053</t>
+        <v>36</v>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>4464</t>
         </is>
       </c>
     </row>
@@ -2882,18 +2476,12 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F69" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G69" t="n">
-        <v>3244</v>
-      </c>
-      <c r="H69" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I69" t="inlineStr">
-        <is>
-          <t>3295</t>
+      <c r="F69" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>3988</t>
         </is>
       </c>
     </row>
@@ -2922,15 +2510,9 @@
       <c r="F70" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="G70" t="n">
-        <v>3883</v>
-      </c>
-      <c r="H70" s="4" t="n">
-        <v>23</v>
-      </c>
-      <c r="I70" t="inlineStr">
-        <is>
-          <t>4016</t>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>4477</t>
         </is>
       </c>
     </row>
@@ -2956,18 +2538,12 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F71" s="5" t="n">
-        <v>14</v>
-      </c>
-      <c r="G71" t="n">
-        <v>3418</v>
-      </c>
-      <c r="H71" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="I71" t="inlineStr">
-        <is>
-          <t>3443</t>
+      <c r="F71" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>3898</t>
         </is>
       </c>
     </row>
@@ -2996,15 +2572,9 @@
       <c r="F72" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="G72" t="n">
-        <v>4488</v>
-      </c>
-      <c r="H72" s="3" t="n">
-        <v>40</v>
-      </c>
-      <c r="I72" t="inlineStr">
-        <is>
-          <t>4647</t>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>5513</t>
         </is>
       </c>
     </row>
@@ -3033,15 +2603,9 @@
       <c r="F73" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G73" t="n">
-        <v>3834</v>
-      </c>
-      <c r="H73" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="I73" t="inlineStr">
-        <is>
-          <t>3928</t>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>4274</t>
         </is>
       </c>
     </row>
@@ -3067,18 +2631,12 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F74" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G74" t="n">
-        <v>3393</v>
-      </c>
-      <c r="H74" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I74" t="inlineStr">
-        <is>
-          <t>3459</t>
+      <c r="F74" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>3822</t>
         </is>
       </c>
     </row>
@@ -3107,15 +2665,9 @@
       <c r="F75" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="G75" t="n">
-        <v>3502</v>
-      </c>
-      <c r="H75" s="4" t="n">
-        <v>25</v>
-      </c>
-      <c r="I75" t="inlineStr">
-        <is>
-          <t>3638</t>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>3983</t>
         </is>
       </c>
     </row>
@@ -3142,17 +2694,11 @@
         </is>
       </c>
       <c r="F76" s="4" t="n">
-        <v>23</v>
-      </c>
-      <c r="G76" t="n">
-        <v>4129</v>
-      </c>
-      <c r="H76" s="4" t="n">
-        <v>25</v>
-      </c>
-      <c r="I76" t="inlineStr">
-        <is>
-          <t>4438</t>
+        <v>21</v>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>4888</t>
         </is>
       </c>
     </row>
@@ -3181,15 +2727,9 @@
       <c r="F77" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G77" t="n">
-        <v>4459</v>
-      </c>
-      <c r="H77" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="I77" t="inlineStr">
-        <is>
-          <t>4598</t>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>5136</t>
         </is>
       </c>
     </row>
@@ -3218,13 +2758,7 @@
       <c r="F78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G78" t="n">
-        <v>0</v>
-      </c>
-      <c r="H78" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I78" t="inlineStr">
+      <c r="G78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3255,15 +2789,9 @@
       <c r="F79" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G79" t="n">
-        <v>4278</v>
-      </c>
-      <c r="H79" s="4" t="n">
-        <v>30</v>
-      </c>
-      <c r="I79" t="inlineStr">
-        <is>
-          <t>4542</t>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>5106</t>
         </is>
       </c>
     </row>
@@ -3284,25 +2812,9 @@
       <c r="D80" t="n">
         <v>4545</v>
       </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>二馆</t>
-        </is>
-      </c>
-      <c r="F80" s="4" t="n">
-        <v>23</v>
-      </c>
-      <c r="G80" t="n">
-        <v>3804</v>
-      </c>
-      <c r="H80" s="4" t="n">
-        <v>29</v>
-      </c>
-      <c r="I80" t="inlineStr">
-        <is>
-          <t>4011</t>
-        </is>
-      </c>
+      <c r="E80" t="inlineStr"/>
+      <c r="F80" s="4" t="inlineStr"/>
+      <c r="G80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -3329,15 +2841,9 @@
       <c r="F81" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G81" t="n">
-        <v>4107</v>
-      </c>
-      <c r="H81" s="4" t="n">
-        <v>30</v>
-      </c>
-      <c r="I81" t="inlineStr">
-        <is>
-          <t>4233</t>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>4733</t>
         </is>
       </c>
     </row>
@@ -3363,18 +2869,12 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F82" s="4" t="n">
-        <v>30</v>
-      </c>
-      <c r="G82" t="n">
-        <v>4090</v>
-      </c>
-      <c r="H82" s="4" t="n">
-        <v>30</v>
-      </c>
-      <c r="I82" t="inlineStr">
-        <is>
-          <t>4330</t>
+      <c r="F82" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>4822</t>
         </is>
       </c>
     </row>
@@ -3403,15 +2903,9 @@
       <c r="F83" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="G83" t="n">
-        <v>4003</v>
-      </c>
-      <c r="H83" s="3" t="n">
-        <v>40</v>
-      </c>
-      <c r="I83" t="inlineStr">
-        <is>
-          <t>4167</t>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>4701</t>
         </is>
       </c>
     </row>
@@ -3440,15 +2934,9 @@
       <c r="F84" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="G84" t="n">
-        <v>3902</v>
-      </c>
-      <c r="H84" s="4" t="n">
-        <v>23</v>
-      </c>
-      <c r="I84" t="inlineStr">
-        <is>
-          <t>4026</t>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>4523</t>
         </is>
       </c>
     </row>
@@ -3474,18 +2962,12 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F85" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="G85" t="n">
-        <v>3846</v>
-      </c>
-      <c r="H85" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="I85" t="inlineStr">
-        <is>
-          <t>4006</t>
+      <c r="F85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>4224</t>
         </is>
       </c>
     </row>
@@ -3512,17 +2994,11 @@
         </is>
       </c>
       <c r="F86" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="G86" t="n">
-        <v>3293</v>
-      </c>
-      <c r="H86" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="I86" t="inlineStr">
-        <is>
-          <t>3379</t>
+        <v>10</v>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>3701</t>
         </is>
       </c>
     </row>
@@ -3548,18 +3024,12 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F87" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="G87" t="n">
-        <v>3124</v>
-      </c>
-      <c r="H87" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I87" t="inlineStr">
-        <is>
-          <t>3124</t>
+      <c r="F87" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>3596</t>
         </is>
       </c>
     </row>
@@ -3585,18 +3055,12 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F88" s="3" t="n">
-        <v>33</v>
-      </c>
-      <c r="G88" t="n">
-        <v>4160</v>
-      </c>
-      <c r="H88" s="3" t="n">
-        <v>32</v>
-      </c>
-      <c r="I88" t="inlineStr">
-        <is>
-          <t>4155</t>
+      <c r="F88" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>4412</t>
         </is>
       </c>
     </row>
@@ -3625,15 +3089,9 @@
       <c r="F89" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G89" t="n">
-        <v>2852</v>
-      </c>
-      <c r="H89" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="I89" t="inlineStr">
-        <is>
-          <t>2922</t>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>3052</t>
         </is>
       </c>
     </row>
@@ -3662,15 +3120,9 @@
       <c r="F90" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="G90" t="n">
-        <v>3179</v>
-      </c>
-      <c r="H90" s="4" t="n">
-        <v>23</v>
-      </c>
-      <c r="I90" t="inlineStr">
-        <is>
-          <t>3223</t>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>3506</t>
         </is>
       </c>
     </row>
@@ -3699,15 +3151,9 @@
       <c r="F91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G91" t="n">
-        <v>2023</v>
-      </c>
-      <c r="H91" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I91" t="inlineStr">
-        <is>
-          <t>2040</t>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>2084</t>
         </is>
       </c>
     </row>
@@ -3736,15 +3182,9 @@
       <c r="F92" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G92" t="n">
-        <v>2660</v>
-      </c>
-      <c r="H92" s="4" t="n">
-        <v>30</v>
-      </c>
-      <c r="I92" t="inlineStr">
-        <is>
-          <t>2694</t>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>2815</t>
         </is>
       </c>
     </row>
@@ -3773,15 +3213,9 @@
       <c r="F93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G93" t="n">
-        <v>2797</v>
-      </c>
-      <c r="H93" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I93" t="inlineStr">
-        <is>
-          <t>2840</t>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>2998</t>
         </is>
       </c>
     </row>
@@ -3810,15 +3244,9 @@
       <c r="F94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G94" t="n">
-        <v>2273</v>
-      </c>
-      <c r="H94" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I94" t="inlineStr">
-        <is>
-          <t>2276</t>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>2280</t>
         </is>
       </c>
     </row>
@@ -3828,7 +3256,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Rename</t>
+          <t>Disparaître</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -3842,8 +3270,6 @@
       <c r="E95" t="inlineStr"/>
       <c r="F95" s="4" t="inlineStr"/>
       <c r="G95" t="inlineStr"/>
-      <c r="H95" s="4" t="inlineStr"/>
-      <c r="I95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -3870,15 +3296,9 @@
       <c r="F96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G96" t="n">
-        <v>2446</v>
-      </c>
-      <c r="H96" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I96" t="inlineStr">
-        <is>
-          <t>2442</t>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>2415</t>
         </is>
       </c>
     </row>
@@ -3904,18 +3324,12 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F97" s="4" t="n">
-        <v>21</v>
-      </c>
-      <c r="G97" t="n">
-        <v>3529</v>
-      </c>
-      <c r="H97" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="I97" t="inlineStr">
-        <is>
-          <t>3547</t>
+      <c r="F97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>3580</t>
         </is>
       </c>
     </row>
@@ -3941,18 +3355,12 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F98" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="G98" t="n">
-        <v>3156</v>
-      </c>
-      <c r="H98" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="I98" t="inlineStr">
-        <is>
-          <t>3186</t>
+      <c r="F98" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>3743</t>
         </is>
       </c>
     </row>
@@ -3981,15 +3389,9 @@
       <c r="F99" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G99" t="n">
-        <v>3827</v>
-      </c>
-      <c r="H99" s="4" t="n">
-        <v>30</v>
-      </c>
-      <c r="I99" t="inlineStr">
-        <is>
-          <t>3924</t>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>4375</t>
         </is>
       </c>
     </row>
@@ -4018,15 +3420,9 @@
       <c r="F100" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G100" t="n">
-        <v>3547</v>
-      </c>
-      <c r="H100" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="I100" t="inlineStr">
-        <is>
-          <t>3702</t>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>3873</t>
         </is>
       </c>
     </row>
@@ -4052,18 +3448,12 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F101" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="G101" t="n">
-        <v>3147</v>
-      </c>
-      <c r="H101" s="4" t="n">
+      <c r="F101" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="I101" t="inlineStr">
-        <is>
-          <t>3445</t>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>4082</t>
         </is>
       </c>
     </row>
@@ -4092,15 +3482,9 @@
       <c r="F102" s="3" t="n">
         <v>34</v>
       </c>
-      <c r="G102" t="n">
-        <v>3911</v>
-      </c>
-      <c r="H102" s="3" t="n">
-        <v>32</v>
-      </c>
-      <c r="I102" t="inlineStr">
-        <is>
-          <t>4032</t>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>4389</t>
         </is>
       </c>
     </row>
@@ -4127,17 +3511,11 @@
         </is>
       </c>
       <c r="F103" s="4" t="n">
-        <v>23</v>
-      </c>
-      <c r="G103" t="n">
-        <v>3467</v>
-      </c>
-      <c r="H103" s="4" t="n">
-        <v>25</v>
-      </c>
-      <c r="I103" t="inlineStr">
-        <is>
-          <t>3728</t>
+        <v>22</v>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>4077</t>
         </is>
       </c>
     </row>
@@ -4166,15 +3544,9 @@
       <c r="F104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G104" t="n">
-        <v>2485</v>
-      </c>
-      <c r="H104" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I104" t="inlineStr">
-        <is>
-          <t>2468</t>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>2457</t>
         </is>
       </c>
     </row>
@@ -4201,17 +3573,11 @@
         </is>
       </c>
       <c r="F105" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="G105" t="n">
-        <v>4129</v>
-      </c>
-      <c r="H105" s="4" t="n">
-        <v>21</v>
-      </c>
-      <c r="I105" t="inlineStr">
-        <is>
-          <t>4456</t>
+        <v>22</v>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>5241</t>
         </is>
       </c>
     </row>
@@ -4238,17 +3604,11 @@
         </is>
       </c>
       <c r="F106" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="G106" t="n">
-        <v>3385</v>
-      </c>
-      <c r="H106" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I106" t="inlineStr">
-        <is>
-          <t>3539</t>
+        <v>12</v>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>3946</t>
         </is>
       </c>
     </row>
@@ -4277,15 +3637,9 @@
       <c r="F107" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G107" t="n">
-        <v>3314</v>
-      </c>
-      <c r="H107" s="4" t="n">
-        <v>30</v>
-      </c>
-      <c r="I107" t="inlineStr">
-        <is>
-          <t>3399</t>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>3594</t>
         </is>
       </c>
     </row>
@@ -4314,15 +3668,9 @@
       <c r="F108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G108" t="n">
-        <v>2616</v>
-      </c>
-      <c r="H108" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I108" t="inlineStr">
-        <is>
-          <t>2630</t>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>2752</t>
         </is>
       </c>
     </row>
@@ -4351,15 +3699,9 @@
       <c r="F109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G109" t="n">
-        <v>3077</v>
-      </c>
-      <c r="H109" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="I109" t="inlineStr">
-        <is>
-          <t>3390</t>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>3483</t>
         </is>
       </c>
     </row>
@@ -4385,18 +3727,12 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F110" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G110" t="n">
-        <v>3081</v>
-      </c>
-      <c r="H110" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="I110" t="inlineStr">
-        <is>
-          <t>3228</t>
+      <c r="F110" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>3574</t>
         </is>
       </c>
     </row>
@@ -4425,15 +3761,9 @@
       <c r="F111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G111" t="n">
-        <v>3292</v>
-      </c>
-      <c r="H111" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I111" t="inlineStr">
-        <is>
-          <t>3352</t>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>3698</t>
         </is>
       </c>
     </row>
@@ -4460,17 +3790,11 @@
         </is>
       </c>
       <c r="F112" s="4" t="n">
-        <v>26</v>
-      </c>
-      <c r="G112" t="n">
-        <v>3658</v>
-      </c>
-      <c r="H112" s="4" t="n">
-        <v>30</v>
-      </c>
-      <c r="I112" t="inlineStr">
-        <is>
-          <t>3926</t>
+        <v>29</v>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>4160</t>
         </is>
       </c>
     </row>
@@ -4497,17 +3821,11 @@
         </is>
       </c>
       <c r="F113" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G113" t="n">
-        <v>2477</v>
-      </c>
-      <c r="H113" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I113" t="inlineStr">
-        <is>
-          <t>2463</t>
+        <v>18</v>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>2663</t>
         </is>
       </c>
     </row>
@@ -4536,15 +3854,9 @@
       <c r="F114" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="G114" t="n">
-        <v>2598</v>
-      </c>
-      <c r="H114" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="I114" t="inlineStr">
-        <is>
-          <t>2645</t>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>2832</t>
         </is>
       </c>
     </row>
@@ -4570,18 +3882,12 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F115" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="G115" t="n">
-        <v>3094</v>
-      </c>
-      <c r="H115" s="4" t="n">
+      <c r="F115" s="4" t="n">
         <v>28</v>
       </c>
-      <c r="I115" t="inlineStr">
-        <is>
-          <t>3319</t>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>3710</t>
         </is>
       </c>
     </row>
@@ -4610,15 +3916,9 @@
       <c r="F116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G116" t="n">
-        <v>2682</v>
-      </c>
-      <c r="H116" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I116" t="inlineStr">
-        <is>
-          <t>2737</t>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>2946</t>
         </is>
       </c>
     </row>
@@ -4647,15 +3947,9 @@
       <c r="F117" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G117" t="n">
-        <v>3323</v>
-      </c>
-      <c r="H117" s="4" t="n">
-        <v>30</v>
-      </c>
-      <c r="I117" t="inlineStr">
-        <is>
-          <t>3361</t>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>3733</t>
         </is>
       </c>
     </row>
@@ -4684,15 +3978,9 @@
       <c r="F118" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G118" t="n">
-        <v>3016</v>
-      </c>
-      <c r="H118" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="I118" t="inlineStr">
-        <is>
-          <t>3113</t>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>3348</t>
         </is>
       </c>
     </row>
@@ -4718,18 +4006,12 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F119" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G119" t="n">
-        <v>3260</v>
-      </c>
-      <c r="H119" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="I119" t="inlineStr">
-        <is>
-          <t>3369</t>
+      <c r="F119" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>3647</t>
         </is>
       </c>
     </row>
@@ -4756,17 +4038,11 @@
         </is>
       </c>
       <c r="F120" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="G120" t="n">
-        <v>2640</v>
-      </c>
-      <c r="H120" s="4" t="n">
-        <v>30</v>
-      </c>
-      <c r="I120" t="inlineStr">
-        <is>
-          <t>2703</t>
+        <v>18</v>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>3000</t>
         </is>
       </c>
     </row>
@@ -4795,15 +4071,9 @@
       <c r="F121" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G121" t="n">
-        <v>3032</v>
-      </c>
-      <c r="H121" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="I121" t="inlineStr">
-        <is>
-          <t>3046</t>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>3304</t>
         </is>
       </c>
     </row>
@@ -4829,18 +4099,12 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F122" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="G122" t="n">
-        <v>3046</v>
-      </c>
-      <c r="H122" s="4" t="n">
+      <c r="F122" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="I122" t="inlineStr">
-        <is>
-          <t>3085</t>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>3309</t>
         </is>
       </c>
     </row>
@@ -4869,15 +4133,9 @@
       <c r="F123" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G123" t="n">
-        <v>3331</v>
-      </c>
-      <c r="H123" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="I123" t="inlineStr">
-        <is>
-          <t>3446</t>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>3676</t>
         </is>
       </c>
     </row>
@@ -4903,18 +4161,12 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F124" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="G124" t="n">
-        <v>3032</v>
-      </c>
-      <c r="H124" s="2" t="n">
+      <c r="F124" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I124" t="inlineStr">
-        <is>
-          <t>2951</t>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>3128</t>
         </is>
       </c>
     </row>
@@ -4943,15 +4195,9 @@
       <c r="F125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G125" t="n">
-        <v>2119</v>
-      </c>
-      <c r="H125" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I125" t="inlineStr">
-        <is>
-          <t>2119</t>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>2087</t>
         </is>
       </c>
     </row>
@@ -4977,18 +4223,12 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F126" s="5" t="n">
-        <v>14</v>
-      </c>
-      <c r="G126" t="n">
-        <v>2701</v>
-      </c>
-      <c r="H126" s="4" t="n">
+      <c r="F126" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="I126" t="inlineStr">
-        <is>
-          <t>2652</t>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>2830</t>
         </is>
       </c>
     </row>
@@ -5017,15 +4257,9 @@
       <c r="F127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G127" t="n">
-        <v>2452</v>
-      </c>
-      <c r="H127" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I127" t="inlineStr">
-        <is>
-          <t>2416</t>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>2397</t>
         </is>
       </c>
     </row>
@@ -5054,15 +4288,9 @@
       <c r="F128" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G128" t="n">
-        <v>4075</v>
-      </c>
-      <c r="H128" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="I128" t="inlineStr">
-        <is>
-          <t>4325</t>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>5025</t>
         </is>
       </c>
     </row>
@@ -5086,8 +4314,6 @@
       <c r="E129" t="inlineStr"/>
       <c r="F129" s="4" t="inlineStr"/>
       <c r="G129" t="inlineStr"/>
-      <c r="H129" s="4" t="inlineStr"/>
-      <c r="I129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="n">
@@ -5114,15 +4340,9 @@
       <c r="F130" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G130" t="n">
-        <v>2674</v>
-      </c>
-      <c r="H130" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I130" t="inlineStr">
-        <is>
-          <t>2658</t>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>2668</t>
         </is>
       </c>
     </row>
@@ -5151,15 +4371,9 @@
       <c r="F131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G131" t="n">
-        <v>2721</v>
-      </c>
-      <c r="H131" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I131" t="inlineStr">
-        <is>
-          <t>2747</t>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>2798</t>
         </is>
       </c>
     </row>
@@ -5188,15 +4402,9 @@
       <c r="F132" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G132" t="n">
-        <v>3337</v>
-      </c>
-      <c r="H132" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="I132" t="inlineStr">
-        <is>
-          <t>3461</t>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>3763</t>
         </is>
       </c>
     </row>
@@ -5220,8 +4428,6 @@
       <c r="E133" t="inlineStr"/>
       <c r="F133" s="4" t="inlineStr"/>
       <c r="G133" t="inlineStr"/>
-      <c r="H133" s="4" t="inlineStr"/>
-      <c r="I133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="n">
@@ -5248,15 +4454,9 @@
       <c r="F134" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="G134" t="n">
-        <v>2665</v>
-      </c>
-      <c r="H134" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="I134" t="inlineStr">
-        <is>
-          <t>2690</t>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>2794</t>
         </is>
       </c>
     </row>
@@ -5285,15 +4485,9 @@
       <c r="F135" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G135" t="n">
-        <v>2479</v>
-      </c>
-      <c r="H135" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I135" t="inlineStr">
-        <is>
-          <t>2468</t>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>2492</t>
         </is>
       </c>
     </row>
@@ -5320,17 +4514,11 @@
         </is>
       </c>
       <c r="F136" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="G136" t="n">
-        <v>2687</v>
-      </c>
-      <c r="H136" s="5" t="n">
-        <v>11</v>
-      </c>
-      <c r="I136" t="inlineStr">
-        <is>
-          <t>2761</t>
+        <v>5</v>
+      </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>2932</t>
         </is>
       </c>
     </row>
@@ -5359,15 +4547,9 @@
       <c r="F137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G137" t="n">
-        <v>2063</v>
-      </c>
-      <c r="H137" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I137" t="inlineStr">
-        <is>
-          <t>2103</t>
+      <c r="G137" t="inlineStr">
+        <is>
+          <t>2134</t>
         </is>
       </c>
     </row>
@@ -5391,8 +4573,6 @@
       <c r="E138" t="inlineStr"/>
       <c r="F138" s="4" t="inlineStr"/>
       <c r="G138" t="inlineStr"/>
-      <c r="H138" s="4" t="inlineStr"/>
-      <c r="I138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -5414,8 +4594,6 @@
       <c r="E139" t="inlineStr"/>
       <c r="F139" s="4" t="inlineStr"/>
       <c r="G139" t="inlineStr"/>
-      <c r="H139" s="4" t="inlineStr"/>
-      <c r="I139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -5437,8 +4615,6 @@
       <c r="E140" t="inlineStr"/>
       <c r="F140" s="4" t="inlineStr"/>
       <c r="G140" t="inlineStr"/>
-      <c r="H140" s="4" t="inlineStr"/>
-      <c r="I140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="n">
@@ -5465,15 +4641,9 @@
       <c r="F141" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G141" t="n">
-        <v>2009</v>
-      </c>
-      <c r="H141" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I141" t="inlineStr">
-        <is>
-          <t>1999</t>
+      <c r="G141" t="inlineStr">
+        <is>
+          <t>2003</t>
         </is>
       </c>
     </row>
@@ -5497,8 +4667,6 @@
       <c r="E142" t="inlineStr"/>
       <c r="F142" s="4" t="inlineStr"/>
       <c r="G142" t="inlineStr"/>
-      <c r="H142" s="4" t="inlineStr"/>
-      <c r="I142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="n">
@@ -5520,8 +4688,6 @@
       <c r="E143" t="inlineStr"/>
       <c r="F143" s="4" t="inlineStr"/>
       <c r="G143" t="inlineStr"/>
-      <c r="H143" s="4" t="inlineStr"/>
-      <c r="I143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -5543,8 +4709,6 @@
       <c r="E144" t="inlineStr"/>
       <c r="F144" s="4" t="inlineStr"/>
       <c r="G144" t="inlineStr"/>
-      <c r="H144" s="4" t="inlineStr"/>
-      <c r="I144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -5566,8 +4730,6 @@
       <c r="E145" t="inlineStr"/>
       <c r="F145" s="4" t="inlineStr"/>
       <c r="G145" t="inlineStr"/>
-      <c r="H145" s="4" t="inlineStr"/>
-      <c r="I145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -5589,8 +4751,6 @@
       <c r="E146" t="inlineStr"/>
       <c r="F146" s="4" t="inlineStr"/>
       <c r="G146" t="inlineStr"/>
-      <c r="H146" s="4" t="inlineStr"/>
-      <c r="I146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -5612,8 +4772,6 @@
       <c r="E147" t="inlineStr"/>
       <c r="F147" s="4" t="inlineStr"/>
       <c r="G147" t="inlineStr"/>
-      <c r="H147" s="4" t="inlineStr"/>
-      <c r="I147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -5635,8 +4793,6 @@
       <c r="E148" t="inlineStr"/>
       <c r="F148" s="4" t="inlineStr"/>
       <c r="G148" t="inlineStr"/>
-      <c r="H148" s="4" t="inlineStr"/>
-      <c r="I148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="n">
@@ -5658,8 +4814,6 @@
       <c r="E149" t="inlineStr"/>
       <c r="F149" s="4" t="inlineStr"/>
       <c r="G149" t="inlineStr"/>
-      <c r="H149" s="4" t="inlineStr"/>
-      <c r="I149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="n">
@@ -5681,8 +4835,6 @@
       <c r="E150" t="inlineStr"/>
       <c r="F150" s="4" t="inlineStr"/>
       <c r="G150" t="inlineStr"/>
-      <c r="H150" s="4" t="inlineStr"/>
-      <c r="I150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="n">
@@ -5704,8 +4856,6 @@
       <c r="E151" t="inlineStr"/>
       <c r="F151" s="4" t="inlineStr"/>
       <c r="G151" t="inlineStr"/>
-      <c r="H151" s="4" t="inlineStr"/>
-      <c r="I151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="n">
@@ -5727,8 +4877,6 @@
       <c r="E152" t="inlineStr"/>
       <c r="F152" s="4" t="inlineStr"/>
       <c r="G152" t="inlineStr"/>
-      <c r="H152" s="4" t="inlineStr"/>
-      <c r="I152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" t="n">
@@ -5750,8 +4898,6 @@
       <c r="E153" t="inlineStr"/>
       <c r="F153" s="4" t="inlineStr"/>
       <c r="G153" t="inlineStr"/>
-      <c r="H153" s="4" t="inlineStr"/>
-      <c r="I153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" t="n">
@@ -5778,15 +4924,9 @@
       <c r="F154" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="G154" t="n">
-        <v>1956</v>
-      </c>
-      <c r="H154" s="4" t="n">
-        <v>24</v>
-      </c>
-      <c r="I154" t="inlineStr">
-        <is>
-          <t>2152</t>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>2381</t>
         </is>
       </c>
     </row>
@@ -5810,8 +4950,6 @@
       <c r="E155" t="inlineStr"/>
       <c r="F155" s="4" t="inlineStr"/>
       <c r="G155" t="inlineStr"/>
-      <c r="H155" s="4" t="inlineStr"/>
-      <c r="I155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="n">
@@ -5835,18 +4973,12 @@
           <t>Chinese</t>
         </is>
       </c>
-      <c r="F156" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G156" t="n">
-        <v>3700</v>
-      </c>
-      <c r="H156" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="I156" t="inlineStr">
-        <is>
-          <t>4022</t>
+      <c r="F156" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>5283</t>
         </is>
       </c>
     </row>
@@ -5875,13 +5007,7 @@
       <c r="F157" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G157" t="n">
-        <v>0</v>
-      </c>
-      <c r="H157" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I157" t="inlineStr">
+      <c r="G157" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5912,15 +5038,9 @@
       <c r="F158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G158" t="n">
-        <v>2500</v>
-      </c>
-      <c r="H158" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I158" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>2523</t>
         </is>
       </c>
     </row>
@@ -5946,18 +5066,12 @@
           <t>Chinese</t>
         </is>
       </c>
-      <c r="F159" s="5" t="n">
-        <v>19</v>
-      </c>
-      <c r="G159" t="n">
-        <v>4144</v>
-      </c>
-      <c r="H159" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="I159" t="inlineStr">
-        <is>
-          <t>4411</t>
+      <c r="F159" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="G159" t="inlineStr">
+        <is>
+          <t>5498</t>
         </is>
       </c>
     </row>
@@ -5986,13 +5100,7 @@
       <c r="F160" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G160" t="n">
-        <v>0</v>
-      </c>
-      <c r="H160" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I160" t="inlineStr">
+      <c r="G160" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6023,15 +5131,9 @@
       <c r="F161" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G161" t="n">
-        <v>2919</v>
-      </c>
-      <c r="H161" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I161" t="inlineStr">
-        <is>
-          <t>3066</t>
+      <c r="G161" t="inlineStr">
+        <is>
+          <t>3211</t>
         </is>
       </c>
     </row>
@@ -6060,13 +5162,7 @@
       <c r="F162" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G162" t="n">
-        <v>0</v>
-      </c>
-      <c r="H162" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I162" t="inlineStr">
+      <c r="G162" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6097,21 +5193,17 @@
       <c r="F163" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G163" t="n">
-        <v>2742</v>
-      </c>
-      <c r="H163" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I163" t="inlineStr">
-        <is>
-          <t>2802</t>
+      <c r="G163" t="inlineStr">
+        <is>
+          <t>3097</t>
         </is>
       </c>
     </row>
     <row r="164">
-      <c r="A164" t="n">
-        <v>56829330</v>
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>56829330</t>
+        </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
@@ -6128,21 +5220,17 @@
       <c r="F164" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="G164" t="n">
-        <v>2906</v>
-      </c>
-      <c r="H164" s="4" t="n">
-        <v>27</v>
-      </c>
-      <c r="I164" t="inlineStr">
-        <is>
-          <t>2931</t>
+      <c r="G164" t="inlineStr">
+        <is>
+          <t>3125</t>
         </is>
       </c>
     </row>
     <row r="165">
-      <c r="A165" t="n">
-        <v>9321819</v>
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>9321819</t>
+        </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
@@ -6156,24 +5244,20 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F165" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="G165" t="n">
-        <v>2807</v>
-      </c>
-      <c r="H165" s="4" t="n">
-        <v>23</v>
-      </c>
-      <c r="I165" t="inlineStr">
-        <is>
-          <t>2847</t>
+      <c r="F165" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="G165" t="inlineStr">
+        <is>
+          <t>2966</t>
         </is>
       </c>
     </row>
     <row r="166">
-      <c r="A166" t="n">
-        <v>15436348</v>
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>15436348</t>
+        </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
@@ -6190,25 +5274,21 @@
       <c r="F166" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G166" t="n">
-        <v>1805</v>
-      </c>
-      <c r="H166" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I166" t="inlineStr">
-        <is>
-          <t>1798</t>
+      <c r="G166" t="inlineStr">
+        <is>
+          <t>1779</t>
         </is>
       </c>
     </row>
     <row r="167">
-      <c r="A167" t="n">
-        <v>58615957</v>
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>20372140</t>
+        </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Anesu597386</t>
+          <t>Player-20372140</t>
         </is>
       </c>
       <c r="C167" t="inlineStr"/>
@@ -6218,121 +5298,105 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F167" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="G167" t="n">
-        <v>2446</v>
-      </c>
-      <c r="H167" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="I167" t="inlineStr">
-        <is>
-          <t>2530</t>
+      <c r="F167" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="G167" t="inlineStr">
+        <is>
+          <t>2518</t>
         </is>
       </c>
     </row>
     <row r="168">
-      <c r="A168" t="n">
-        <v>27113069</v>
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>47928278</t>
+        </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>㊥DumbSmoky</t>
+          <t>㊥JOSE</t>
         </is>
       </c>
       <c r="C168" t="inlineStr"/>
       <c r="D168" t="inlineStr"/>
       <c r="E168" t="inlineStr">
         <is>
-          <t>三馆</t>
-        </is>
-      </c>
-      <c r="F168" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="G168" t="n">
-        <v>4584</v>
-      </c>
-      <c r="H168" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="I168" t="inlineStr">
-        <is>
-          <t>4631</t>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F168" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G168" t="inlineStr">
+        <is>
+          <t>6129</t>
         </is>
       </c>
     </row>
     <row r="169">
-      <c r="A169" t="n">
-        <v>47533851</v>
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>57442184</t>
+        </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Bibek</t>
+          <t>Adarsh</t>
         </is>
       </c>
       <c r="C169" t="inlineStr"/>
       <c r="D169" t="inlineStr"/>
       <c r="E169" t="inlineStr">
         <is>
-          <t>三馆</t>
-        </is>
-      </c>
-      <c r="F169" s="4" t="n">
-        <v>30</v>
-      </c>
-      <c r="G169" t="n">
-        <v>2198</v>
-      </c>
-      <c r="H169" s="4" t="n">
-        <v>30</v>
-      </c>
-      <c r="I169" t="inlineStr">
-        <is>
-          <t>2315</t>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F169" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="G169" t="inlineStr">
+        <is>
+          <t>2288</t>
         </is>
       </c>
     </row>
     <row r="170">
-      <c r="A170" t="n">
-        <v>47928278</v>
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>58615957</t>
+        </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>㊥JOSE</t>
+          <t>Anesu597386</t>
         </is>
       </c>
       <c r="C170" t="inlineStr"/>
       <c r="D170" t="inlineStr"/>
       <c r="E170" t="inlineStr">
         <is>
-          <t>三馆</t>
-        </is>
-      </c>
-      <c r="F170" s="3" t="n">
-        <v>40</v>
-      </c>
-      <c r="G170" t="n">
-        <v>5055</v>
-      </c>
-      <c r="H170" s="3" t="n">
-        <v>40</v>
-      </c>
-      <c r="I170" t="inlineStr">
-        <is>
-          <t>5307</t>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F170" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="G170" t="inlineStr">
+        <is>
+          <t>2608</t>
         </is>
       </c>
     </row>
     <row r="171">
-      <c r="A171" t="n">
-        <v>50742014</v>
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>12333251</t>
+        </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>"Aditya Naik"</t>
+          <t>"㊌ Mingxuan"</t>
         </is>
       </c>
       <c r="C171" t="inlineStr"/>
@@ -6345,25 +5409,21 @@
       <c r="F171" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G171" t="n">
-        <v>999</v>
-      </c>
-      <c r="H171" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I171" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G171" t="inlineStr">
+        <is>
+          <t>3067</t>
         </is>
       </c>
     </row>
     <row r="172">
-      <c r="A172" t="n">
-        <v>53269862</v>
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>27113069</t>
+        </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>New_Player111</t>
+          <t>㊥DumbSmoky</t>
         </is>
       </c>
       <c r="C172" t="inlineStr"/>
@@ -6373,28 +5433,24 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F172" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="G172" t="n">
-        <v>1680</v>
-      </c>
-      <c r="H172" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="I172" t="inlineStr">
-        <is>
-          <t>2043</t>
+      <c r="F172" s="3" t="n">
+        <v>37</v>
+      </c>
+      <c r="G172" t="inlineStr">
+        <is>
+          <t>5701</t>
         </is>
       </c>
     </row>
     <row r="173">
-      <c r="A173" t="n">
-        <v>54924790</v>
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>47533851</t>
+        </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Sujit4u</t>
+          <t>Bibek</t>
         </is>
       </c>
       <c r="C173" t="inlineStr"/>
@@ -6404,28 +5460,24 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F173" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G173" t="n">
-        <v>2924</v>
-      </c>
-      <c r="H173" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I173" t="inlineStr">
-        <is>
-          <t>2906</t>
+      <c r="F173" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="G173" t="inlineStr">
+        <is>
+          <t>2286</t>
         </is>
       </c>
     </row>
     <row r="174">
-      <c r="A174" t="n">
-        <v>55963040</v>
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>50742014</t>
+        </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Baliram</t>
+          <t>"Aditya Naik"</t>
         </is>
       </c>
       <c r="C174" t="inlineStr"/>
@@ -6438,25 +5490,21 @@
       <c r="F174" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G174" t="n">
-        <v>2450</v>
-      </c>
-      <c r="H174" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I174" t="inlineStr">
-        <is>
-          <t>2430</t>
+      <c r="G174" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="175">
-      <c r="A175" t="n">
-        <v>58132159</v>
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>53269862</t>
+        </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>ExultantDelivery42</t>
+          <t>New_Player111</t>
         </is>
       </c>
       <c r="C175" t="inlineStr"/>
@@ -6469,25 +5517,21 @@
       <c r="F175" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G175" t="n">
-        <v>1514</v>
-      </c>
-      <c r="H175" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I175" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G175" t="inlineStr">
+        <is>
+          <t>2062</t>
         </is>
       </c>
     </row>
     <row r="176">
-      <c r="A176" t="n">
-        <v>58562596</v>
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>54924790</t>
+        </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Player-58562596</t>
+          <t>Sujit4u</t>
         </is>
       </c>
       <c r="C176" t="inlineStr"/>
@@ -6500,25 +5544,21 @@
       <c r="F176" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G176" t="n">
-        <v>0</v>
-      </c>
-      <c r="H176" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I176" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G176" t="inlineStr">
+        <is>
+          <t>3019</t>
         </is>
       </c>
     </row>
     <row r="177">
-      <c r="A177" t="n">
-        <v>58615925</v>
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>55963040</t>
+        </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>齐天的大圣</t>
+          <t>Baliram</t>
         </is>
       </c>
       <c r="C177" t="inlineStr"/>
@@ -6528,61 +5568,51 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F177" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="G177" t="n">
-        <v>2583</v>
-      </c>
-      <c r="H177" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="I177" t="inlineStr">
-        <is>
-          <t>2608</t>
+      <c r="F177" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G177" t="inlineStr">
+        <is>
+          <t>2399</t>
         </is>
       </c>
     </row>
     <row r="178">
-      <c r="A178" t="n">
-        <v>48005945</v>
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>56691087</t>
+        </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>NIKONEZNA</t>
+          <t>LongestSovereign8</t>
         </is>
       </c>
       <c r="C178" t="inlineStr"/>
       <c r="D178" t="inlineStr"/>
       <c r="E178" t="inlineStr">
         <is>
-          <t>Chinese</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="F178" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G178" t="n">
-        <v>2541</v>
-      </c>
-      <c r="H178" s="5" t="n">
-        <v>11</v>
-      </c>
-      <c r="I178" t="inlineStr">
-        <is>
-          <t>2716</t>
+      <c r="G178" t="inlineStr">
+        <is>
+          <t>1882</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>12333251</t>
+          <t>57339836</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>"㊌ Mingxuan"</t>
+          <t>Player-57339836</t>
         </is>
       </c>
       <c r="C179" t="inlineStr"/>
@@ -6592,26 +5622,24 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F179" s="4" t="inlineStr"/>
-      <c r="G179" t="inlineStr"/>
-      <c r="H179" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="I179" t="inlineStr">
-        <is>
-          <t>2997</t>
+      <c r="F179" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G179" t="inlineStr">
+        <is>
+          <t>1149</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>26497650</t>
+          <t>57605565</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>mithun</t>
+          <t>"Leonel Messi"</t>
         </is>
       </c>
       <c r="C180" t="inlineStr"/>
@@ -6621,26 +5649,24 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F180" s="4" t="inlineStr"/>
-      <c r="G180" t="inlineStr"/>
-      <c r="H180" s="4" t="n">
-        <v>27</v>
-      </c>
-      <c r="I180" t="inlineStr">
-        <is>
-          <t>2697</t>
+      <c r="F180" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="G180" t="inlineStr">
+        <is>
+          <t>1560</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>56691087</t>
+          <t>58132159</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>LongestSovereign8</t>
+          <t>ExultantDelivery42</t>
         </is>
       </c>
       <c r="C181" t="inlineStr"/>
@@ -6650,14 +5676,147 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F181" s="4" t="inlineStr"/>
-      <c r="G181" t="inlineStr"/>
-      <c r="H181" s="4" t="n">
-        <v>21</v>
-      </c>
-      <c r="I181" t="inlineStr">
-        <is>
-          <t>1887</t>
+      <c r="F181" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G181" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>58562596</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>Player-58562596</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr"/>
+      <c r="D182" t="inlineStr"/>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F182" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G182" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>58615925</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>齐天的大圣</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr"/>
+      <c r="D183" t="inlineStr"/>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F183" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="G183" t="inlineStr">
+        <is>
+          <t>2877</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>58635041</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>Player-58635041</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr"/>
+      <c r="D184" t="inlineStr"/>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F184" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="G184" t="inlineStr">
+        <is>
+          <t>1608</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>58644547</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>RotaryPreparation39</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr"/>
+      <c r="D185" t="inlineStr"/>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F185" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="G185" t="inlineStr">
+        <is>
+          <t>1632</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>48005945</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>NIKONEZNA</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr"/>
+      <c r="D186" t="inlineStr"/>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="F186" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G186" t="inlineStr">
+        <is>
+          <t>2668</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-01-28 11:30:31
</commit_message>
<xml_diff>
--- a/Season_Attack/82.xlsx
+++ b/Season_Attack/82.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G186"/>
+  <dimension ref="A1:I189"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,6 +426,16 @@
           <t>01-25_0</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>01-27_A</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>01-27_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -452,9 +462,15 @@
       <c r="F2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>3838</t>
+      <c r="G2" t="n">
+        <v>3838</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>4157</t>
         </is>
       </c>
     </row>
@@ -483,9 +499,15 @@
       <c r="F3" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>5730</t>
+      <c r="G3" t="n">
+        <v>5730</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>36</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>6236</t>
         </is>
       </c>
     </row>
@@ -508,15 +530,21 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F4" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>5617</t>
+      <c r="G4" t="n">
+        <v>5617</v>
+      </c>
+      <c r="H4" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>6298</t>
         </is>
       </c>
     </row>
@@ -539,15 +567,21 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F5" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>5574</t>
+      <c r="G5" t="n">
+        <v>5574</v>
+      </c>
+      <c r="H5" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>6114</t>
         </is>
       </c>
     </row>
@@ -570,15 +604,21 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F6" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>5628</t>
+      <c r="G6" t="n">
+        <v>5628</v>
+      </c>
+      <c r="H6" s="3" t="n">
+        <v>37</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>6287</t>
         </is>
       </c>
     </row>
@@ -601,15 +641,21 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F7" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>5157</t>
+      <c r="G7" t="n">
+        <v>5157</v>
+      </c>
+      <c r="H7" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>5641</t>
         </is>
       </c>
     </row>
@@ -632,15 +678,21 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F8" s="3" t="n">
         <v>31</v>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>5444</t>
+      <c r="G8" t="n">
+        <v>5444</v>
+      </c>
+      <c r="H8" s="3" t="n">
+        <v>33</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>5979</t>
         </is>
       </c>
     </row>
@@ -664,6 +716,8 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" s="4" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
+      <c r="H9" s="4" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -684,15 +738,21 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F10" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>5099</t>
+      <c r="G10" t="n">
+        <v>5099</v>
+      </c>
+      <c r="H10" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>5486</t>
         </is>
       </c>
     </row>
@@ -715,15 +775,21 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F11" s="3" t="n">
         <v>38</v>
       </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>6285</t>
+      <c r="G11" t="n">
+        <v>6285</v>
+      </c>
+      <c r="H11" s="3" t="n">
+        <v>37</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>6932</t>
         </is>
       </c>
     </row>
@@ -746,15 +812,21 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F12" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>5404</t>
+      <c r="G12" t="n">
+        <v>5404</v>
+      </c>
+      <c r="H12" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>6058</t>
         </is>
       </c>
     </row>
@@ -783,7 +855,13 @@
       <c r="F13" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="G13" t="n">
+        <v>3047</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="inlineStr">
         <is>
           <t>3047</t>
         </is>
@@ -808,15 +886,21 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F14" s="3" t="n">
         <v>37</v>
       </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>6563</t>
+      <c r="G14" t="n">
+        <v>6563</v>
+      </c>
+      <c r="H14" s="3" t="n">
+        <v>38</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>7047</t>
         </is>
       </c>
     </row>
@@ -839,15 +923,21 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F15" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>5442</t>
+      <c r="G15" t="n">
+        <v>5442</v>
+      </c>
+      <c r="H15" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>5862</t>
         </is>
       </c>
     </row>
@@ -870,15 +960,21 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F16" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>6000</t>
+      <c r="G16" t="n">
+        <v>6000</v>
+      </c>
+      <c r="H16" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>6324</t>
         </is>
       </c>
     </row>
@@ -907,9 +1003,15 @@
       <c r="F17" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>5060</t>
+      <c r="G17" t="n">
+        <v>5060</v>
+      </c>
+      <c r="H17" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>5352</t>
         </is>
       </c>
     </row>
@@ -932,15 +1034,21 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Chinese</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F18" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>5588</t>
+      <c r="G18" t="n">
+        <v>5588</v>
+      </c>
+      <c r="H18" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>5991</t>
         </is>
       </c>
     </row>
@@ -963,15 +1071,21 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F19" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>6394</t>
+      <c r="G19" t="n">
+        <v>6394</v>
+      </c>
+      <c r="H19" s="3" t="n">
+        <v>33</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>7021</t>
         </is>
       </c>
     </row>
@@ -1000,9 +1114,15 @@
       <c r="F20" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>5322</t>
+      <c r="G20" t="n">
+        <v>5322</v>
+      </c>
+      <c r="H20" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>5814</t>
         </is>
       </c>
     </row>
@@ -1025,15 +1145,21 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F21" s="3" t="n">
         <v>38</v>
       </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>5502</t>
+      <c r="G21" t="n">
+        <v>5502</v>
+      </c>
+      <c r="H21" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>5995</t>
         </is>
       </c>
     </row>
@@ -1062,9 +1188,15 @@
       <c r="F22" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>4531</t>
+      <c r="G22" t="n">
+        <v>4531</v>
+      </c>
+      <c r="H22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>5285</t>
         </is>
       </c>
     </row>
@@ -1087,15 +1219,21 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F23" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>5727</t>
+      <c r="G23" t="n">
+        <v>5727</v>
+      </c>
+      <c r="H23" s="3" t="n">
+        <v>33</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>6367</t>
         </is>
       </c>
     </row>
@@ -1124,7 +1262,13 @@
       <c r="F24" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G24" t="inlineStr">
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1149,15 +1293,21 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F25" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>5355</t>
+      <c r="G25" t="n">
+        <v>5355</v>
+      </c>
+      <c r="H25" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>5682</t>
         </is>
       </c>
     </row>
@@ -1180,15 +1330,21 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F26" s="3" t="n">
         <v>38</v>
       </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>5908</t>
+      <c r="G26" t="n">
+        <v>5908</v>
+      </c>
+      <c r="H26" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>6668</t>
         </is>
       </c>
     </row>
@@ -1211,15 +1367,21 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F27" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>5163</t>
+      <c r="G27" t="n">
+        <v>5163</v>
+      </c>
+      <c r="H27" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>6052</t>
         </is>
       </c>
     </row>
@@ -1242,15 +1404,21 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F28" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>6225</t>
+      <c r="G28" t="n">
+        <v>6225</v>
+      </c>
+      <c r="H28" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>6986</t>
         </is>
       </c>
     </row>
@@ -1273,15 +1441,21 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F29" s="4" t="n">
         <v>28</v>
       </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>5329</t>
+      <c r="G29" t="n">
+        <v>5329</v>
+      </c>
+      <c r="H29" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>6019</t>
         </is>
       </c>
     </row>
@@ -1310,9 +1484,15 @@
       <c r="F30" s="3" t="n">
         <v>39</v>
       </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>6198</t>
+      <c r="G30" t="n">
+        <v>6198</v>
+      </c>
+      <c r="H30" s="3" t="n">
+        <v>34</v>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>6526</t>
         </is>
       </c>
     </row>
@@ -1341,9 +1521,15 @@
       <c r="F31" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>6004</t>
+      <c r="G31" t="n">
+        <v>6004</v>
+      </c>
+      <c r="H31" s="3" t="n">
+        <v>35</v>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>6613</t>
         </is>
       </c>
     </row>
@@ -1366,15 +1552,21 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>2919</t>
+      <c r="G32" t="n">
+        <v>2919</v>
+      </c>
+      <c r="H32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>2935</t>
         </is>
       </c>
     </row>
@@ -1397,15 +1589,21 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F33" s="3" t="n">
         <v>37</v>
       </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>6015</t>
+      <c r="G33" t="n">
+        <v>6015</v>
+      </c>
+      <c r="H33" s="3" t="n">
+        <v>39</v>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>6457</t>
         </is>
       </c>
     </row>
@@ -1428,15 +1626,21 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F34" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>5349</t>
+      <c r="G34" t="n">
+        <v>5349</v>
+      </c>
+      <c r="H34" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>5769</t>
         </is>
       </c>
     </row>
@@ -1459,15 +1663,21 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F35" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>5030</t>
+      <c r="G35" t="n">
+        <v>5030</v>
+      </c>
+      <c r="H35" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>5280</t>
         </is>
       </c>
     </row>
@@ -1491,6 +1701,8 @@
       <c r="E36" t="inlineStr"/>
       <c r="F36" s="4" t="inlineStr"/>
       <c r="G36" t="inlineStr"/>
+      <c r="H36" s="4" t="inlineStr"/>
+      <c r="I36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -1511,15 +1723,21 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F37" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>5405</t>
+      <c r="G37" t="n">
+        <v>5405</v>
+      </c>
+      <c r="H37" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>6058</t>
         </is>
       </c>
     </row>
@@ -1542,15 +1760,21 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F38" s="3" t="n">
         <v>35</v>
       </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>5299</t>
+      <c r="G38" t="n">
+        <v>5299</v>
+      </c>
+      <c r="H38" s="3" t="n">
+        <v>35</v>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>5555</t>
         </is>
       </c>
     </row>
@@ -1573,15 +1797,21 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F39" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>6136</t>
+      <c r="G39" t="n">
+        <v>6136</v>
+      </c>
+      <c r="H39" s="3" t="n">
+        <v>36</v>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>6974</t>
         </is>
       </c>
     </row>
@@ -1604,15 +1834,21 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F40" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>5429</t>
+      <c r="G40" t="n">
+        <v>5429</v>
+      </c>
+      <c r="H40" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>5817</t>
         </is>
       </c>
     </row>
@@ -1635,15 +1871,21 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F41" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>6215</t>
+      <c r="G41" t="n">
+        <v>6215</v>
+      </c>
+      <c r="H41" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>6898</t>
         </is>
       </c>
     </row>
@@ -1666,15 +1908,21 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F42" s="3" t="n">
         <v>39</v>
       </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>5526</t>
+      <c r="G42" t="n">
+        <v>5526</v>
+      </c>
+      <c r="H42" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>6009</t>
         </is>
       </c>
     </row>
@@ -1703,11 +1951,11 @@
       <c r="F43" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>3202</t>
-        </is>
-      </c>
+      <c r="G43" t="n">
+        <v>3202</v>
+      </c>
+      <c r="H43" s="4" t="inlineStr"/>
+      <c r="I43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -1728,15 +1976,21 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F44" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>5191</t>
+      <c r="G44" t="n">
+        <v>5191</v>
+      </c>
+      <c r="H44" s="3" t="n">
+        <v>33</v>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>5765</t>
         </is>
       </c>
     </row>
@@ -1757,9 +2011,21 @@
       <c r="D45" t="n">
         <v>6207</v>
       </c>
-      <c r="E45" t="inlineStr"/>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
       <c r="F45" s="4" t="inlineStr"/>
       <c r="G45" t="inlineStr"/>
+      <c r="H45" s="3" t="n">
+        <v>33</v>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>6075</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -1786,7 +2052,13 @@
       <c r="F46" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G46" t="inlineStr">
+      <c r="G46" t="n">
+        <v>3112</v>
+      </c>
+      <c r="H46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I46" t="inlineStr">
         <is>
           <t>3112</t>
         </is>
@@ -1811,15 +2083,21 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F47" s="3" t="n">
         <v>34</v>
       </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>5817</t>
+      <c r="G47" t="n">
+        <v>5817</v>
+      </c>
+      <c r="H47" s="3" t="n">
+        <v>34</v>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>6244</t>
         </is>
       </c>
     </row>
@@ -1848,9 +2126,15 @@
       <c r="F48" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>4582</t>
+      <c r="G48" t="n">
+        <v>4582</v>
+      </c>
+      <c r="H48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>4581</t>
         </is>
       </c>
     </row>
@@ -1879,7 +2163,13 @@
       <c r="F49" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G49" t="inlineStr">
+      <c r="G49" t="n">
+        <v>3445</v>
+      </c>
+      <c r="H49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I49" t="inlineStr">
         <is>
           <t>3445</t>
         </is>
@@ -1905,6 +2195,8 @@
       <c r="E50" t="inlineStr"/>
       <c r="F50" s="4" t="inlineStr"/>
       <c r="G50" t="inlineStr"/>
+      <c r="H50" s="4" t="inlineStr"/>
+      <c r="I50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -1926,6 +2218,8 @@
       <c r="E51" t="inlineStr"/>
       <c r="F51" s="4" t="inlineStr"/>
       <c r="G51" t="inlineStr"/>
+      <c r="H51" s="4" t="inlineStr"/>
+      <c r="I51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -1952,9 +2246,15 @@
       <c r="F52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>2574</t>
+      <c r="G52" t="n">
+        <v>2574</v>
+      </c>
+      <c r="H52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>2608</t>
         </is>
       </c>
     </row>
@@ -1983,9 +2283,15 @@
       <c r="F53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>3353</t>
+      <c r="G53" t="n">
+        <v>3353</v>
+      </c>
+      <c r="H53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>3488</t>
         </is>
       </c>
     </row>
@@ -2014,9 +2320,15 @@
       <c r="F54" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>2990</t>
+      <c r="G54" t="n">
+        <v>2990</v>
+      </c>
+      <c r="H54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>3036</t>
         </is>
       </c>
     </row>
@@ -2045,9 +2357,15 @@
       <c r="F55" s="4" t="n">
         <v>26</v>
       </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>5304</t>
+      <c r="G55" t="n">
+        <v>5304</v>
+      </c>
+      <c r="H55" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>5779</t>
         </is>
       </c>
     </row>
@@ -2076,9 +2394,15 @@
       <c r="F56" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>4147</t>
+      <c r="G56" t="n">
+        <v>4147</v>
+      </c>
+      <c r="H56" s="3" t="n">
+        <v>36</v>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>4408</t>
         </is>
       </c>
     </row>
@@ -2107,9 +2431,15 @@
       <c r="F57" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>4383</t>
+      <c r="G57" t="n">
+        <v>4383</v>
+      </c>
+      <c r="H57" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>4637</t>
         </is>
       </c>
     </row>
@@ -2138,9 +2468,15 @@
       <c r="F58" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>5199</t>
+      <c r="G58" t="n">
+        <v>5199</v>
+      </c>
+      <c r="H58" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>5636</t>
         </is>
       </c>
     </row>
@@ -2169,9 +2505,15 @@
       <c r="F59" s="3" t="n">
         <v>35</v>
       </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>4472</t>
+      <c r="G59" t="n">
+        <v>4472</v>
+      </c>
+      <c r="H59" s="3" t="n">
+        <v>33</v>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>4704</t>
         </is>
       </c>
     </row>
@@ -2200,9 +2542,15 @@
       <c r="F60" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>5031</t>
+      <c r="G60" t="n">
+        <v>5031</v>
+      </c>
+      <c r="H60" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>5208</t>
         </is>
       </c>
     </row>
@@ -2231,9 +2579,15 @@
       <c r="F61" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>3179</t>
+      <c r="G61" t="n">
+        <v>3179</v>
+      </c>
+      <c r="H61" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>3195</t>
         </is>
       </c>
     </row>
@@ -2262,9 +2616,15 @@
       <c r="F62" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>5233</t>
+      <c r="G62" t="n">
+        <v>5233</v>
+      </c>
+      <c r="H62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>5429</t>
         </is>
       </c>
     </row>
@@ -2293,9 +2653,15 @@
       <c r="F63" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>3749</t>
+      <c r="G63" t="n">
+        <v>3749</v>
+      </c>
+      <c r="H63" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>3765</t>
         </is>
       </c>
     </row>
@@ -2324,9 +2690,15 @@
       <c r="F64" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>3357</t>
+      <c r="G64" t="n">
+        <v>3357</v>
+      </c>
+      <c r="H64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>3324</t>
         </is>
       </c>
     </row>
@@ -2355,9 +2727,15 @@
       <c r="F65" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>4940</t>
+      <c r="G65" t="n">
+        <v>4940</v>
+      </c>
+      <c r="H65" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>5259</t>
         </is>
       </c>
     </row>
@@ -2386,9 +2764,15 @@
       <c r="F66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>2753</t>
+      <c r="G66" t="n">
+        <v>2753</v>
+      </c>
+      <c r="H66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>2869</t>
         </is>
       </c>
     </row>
@@ -2417,9 +2801,15 @@
       <c r="F67" s="4" t="n">
         <v>28</v>
       </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>5618</t>
+      <c r="G67" t="n">
+        <v>5618</v>
+      </c>
+      <c r="H67" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>6163</t>
         </is>
       </c>
     </row>
@@ -2448,9 +2838,15 @@
       <c r="F68" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>4464</t>
+      <c r="G68" t="n">
+        <v>4464</v>
+      </c>
+      <c r="H68" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>4646</t>
         </is>
       </c>
     </row>
@@ -2479,9 +2875,15 @@
       <c r="F69" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>3988</t>
+      <c r="G69" t="n">
+        <v>3988</v>
+      </c>
+      <c r="H69" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>4469</t>
         </is>
       </c>
     </row>
@@ -2510,9 +2912,15 @@
       <c r="F70" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>4477</t>
+      <c r="G70" t="n">
+        <v>4477</v>
+      </c>
+      <c r="H70" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>4675</t>
         </is>
       </c>
     </row>
@@ -2541,9 +2949,15 @@
       <c r="F71" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>3898</t>
+      <c r="G71" t="n">
+        <v>3898</v>
+      </c>
+      <c r="H71" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>4266</t>
         </is>
       </c>
     </row>
@@ -2566,15 +2980,21 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F72" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>5513</t>
+      <c r="G72" t="n">
+        <v>5513</v>
+      </c>
+      <c r="H72" s="3" t="n">
+        <v>39</v>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>5916</t>
         </is>
       </c>
     </row>
@@ -2603,9 +3023,15 @@
       <c r="F73" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>4274</t>
+      <c r="G73" t="n">
+        <v>4274</v>
+      </c>
+      <c r="H73" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>4550</t>
         </is>
       </c>
     </row>
@@ -2634,9 +3060,15 @@
       <c r="F74" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>3822</t>
+      <c r="G74" t="n">
+        <v>3822</v>
+      </c>
+      <c r="H74" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>4364</t>
         </is>
       </c>
     </row>
@@ -2665,9 +3097,15 @@
       <c r="F75" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>3983</t>
+      <c r="G75" t="n">
+        <v>3983</v>
+      </c>
+      <c r="H75" s="4" t="n">
+        <v>26</v>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>4112</t>
         </is>
       </c>
     </row>
@@ -2690,15 +3128,21 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F76" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="G76" t="inlineStr">
-        <is>
-          <t>4888</t>
+      <c r="G76" t="n">
+        <v>4888</v>
+      </c>
+      <c r="H76" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>5183</t>
         </is>
       </c>
     </row>
@@ -2727,9 +3171,15 @@
       <c r="F77" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>5136</t>
+      <c r="G77" t="n">
+        <v>5136</v>
+      </c>
+      <c r="H77" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>5529</t>
         </is>
       </c>
     </row>
@@ -2758,7 +3208,13 @@
       <c r="F78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G78" t="inlineStr">
+      <c r="G78" t="n">
+        <v>0</v>
+      </c>
+      <c r="H78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2789,9 +3245,15 @@
       <c r="F79" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>5106</t>
+      <c r="G79" t="n">
+        <v>5106</v>
+      </c>
+      <c r="H79" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>5440</t>
         </is>
       </c>
     </row>
@@ -2812,9 +3274,21 @@
       <c r="D80" t="n">
         <v>4545</v>
       </c>
-      <c r="E80" t="inlineStr"/>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
       <c r="F80" s="4" t="inlineStr"/>
       <c r="G80" t="inlineStr"/>
+      <c r="H80" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>4918</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -2841,9 +3315,15 @@
       <c r="F81" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>4733</t>
+      <c r="G81" t="n">
+        <v>4733</v>
+      </c>
+      <c r="H81" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>4896</t>
         </is>
       </c>
     </row>
@@ -2872,9 +3352,15 @@
       <c r="F82" s="3" t="n">
         <v>32</v>
       </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>4822</t>
+      <c r="G82" t="n">
+        <v>4822</v>
+      </c>
+      <c r="H82" s="3" t="n">
+        <v>31</v>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>5130</t>
         </is>
       </c>
     </row>
@@ -2903,9 +3389,15 @@
       <c r="F83" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>4701</t>
+      <c r="G83" t="n">
+        <v>4701</v>
+      </c>
+      <c r="H83" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>4868</t>
         </is>
       </c>
     </row>
@@ -2934,9 +3426,15 @@
       <c r="F84" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>4523</t>
+      <c r="G84" t="n">
+        <v>4523</v>
+      </c>
+      <c r="H84" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>4773</t>
         </is>
       </c>
     </row>
@@ -2965,9 +3463,15 @@
       <c r="F85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>4224</t>
+      <c r="G85" t="n">
+        <v>4224</v>
+      </c>
+      <c r="H85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>4407</t>
         </is>
       </c>
     </row>
@@ -2996,9 +3500,15 @@
       <c r="F86" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>3701</t>
+      <c r="G86" t="n">
+        <v>3701</v>
+      </c>
+      <c r="H86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>3819</t>
         </is>
       </c>
     </row>
@@ -3027,9 +3537,15 @@
       <c r="F87" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G87" t="inlineStr">
-        <is>
-          <t>3596</t>
+      <c r="G87" t="n">
+        <v>3596</v>
+      </c>
+      <c r="H87" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>3812</t>
         </is>
       </c>
     </row>
@@ -3058,9 +3574,15 @@
       <c r="F88" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="G88" t="inlineStr">
-        <is>
-          <t>4412</t>
+      <c r="G88" t="n">
+        <v>4412</v>
+      </c>
+      <c r="H88" s="3" t="n">
+        <v>33</v>
+      </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>4913</t>
         </is>
       </c>
     </row>
@@ -3089,9 +3611,15 @@
       <c r="F89" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t>3052</t>
+      <c r="G89" t="n">
+        <v>3052</v>
+      </c>
+      <c r="H89" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>3150</t>
         </is>
       </c>
     </row>
@@ -3120,9 +3648,15 @@
       <c r="F90" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>3506</t>
+      <c r="G90" t="n">
+        <v>3506</v>
+      </c>
+      <c r="H90" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>3588</t>
         </is>
       </c>
     </row>
@@ -3151,9 +3685,15 @@
       <c r="F91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>2084</t>
+      <c r="G91" t="n">
+        <v>2084</v>
+      </c>
+      <c r="H91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>2087</t>
         </is>
       </c>
     </row>
@@ -3182,9 +3722,15 @@
       <c r="F92" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>2815</t>
+      <c r="G92" t="n">
+        <v>2815</v>
+      </c>
+      <c r="H92" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>2909</t>
         </is>
       </c>
     </row>
@@ -3213,9 +3759,15 @@
       <c r="F93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>2998</t>
+      <c r="G93" t="n">
+        <v>2998</v>
+      </c>
+      <c r="H93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>3112</t>
         </is>
       </c>
     </row>
@@ -3244,9 +3796,15 @@
       <c r="F94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G94" t="inlineStr">
-        <is>
-          <t>2280</t>
+      <c r="G94" t="n">
+        <v>2280</v>
+      </c>
+      <c r="H94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>2407</t>
         </is>
       </c>
     </row>
@@ -3270,6 +3828,8 @@
       <c r="E95" t="inlineStr"/>
       <c r="F95" s="4" t="inlineStr"/>
       <c r="G95" t="inlineStr"/>
+      <c r="H95" s="4" t="inlineStr"/>
+      <c r="I95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -3296,9 +3856,15 @@
       <c r="F96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>2415</t>
+      <c r="G96" t="n">
+        <v>2415</v>
+      </c>
+      <c r="H96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>2425</t>
         </is>
       </c>
     </row>
@@ -3327,9 +3893,15 @@
       <c r="F97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>3580</t>
+      <c r="G97" t="n">
+        <v>3580</v>
+      </c>
+      <c r="H97" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>3958</t>
         </is>
       </c>
     </row>
@@ -3358,9 +3930,15 @@
       <c r="F98" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>3743</t>
+      <c r="G98" t="n">
+        <v>3743</v>
+      </c>
+      <c r="H98" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>3995</t>
         </is>
       </c>
     </row>
@@ -3389,9 +3967,15 @@
       <c r="F99" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G99" t="inlineStr">
-        <is>
-          <t>4375</t>
+      <c r="G99" t="n">
+        <v>4375</v>
+      </c>
+      <c r="H99" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>4620</t>
         </is>
       </c>
     </row>
@@ -3420,9 +4004,15 @@
       <c r="F100" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G100" t="inlineStr">
-        <is>
-          <t>3873</t>
+      <c r="G100" t="n">
+        <v>3873</v>
+      </c>
+      <c r="H100" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>4183</t>
         </is>
       </c>
     </row>
@@ -3451,9 +4041,15 @@
       <c r="F101" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="G101" t="inlineStr">
-        <is>
-          <t>4082</t>
+      <c r="G101" t="n">
+        <v>4082</v>
+      </c>
+      <c r="H101" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>4290</t>
         </is>
       </c>
     </row>
@@ -3482,9 +4078,15 @@
       <c r="F102" s="3" t="n">
         <v>34</v>
       </c>
-      <c r="G102" t="inlineStr">
-        <is>
-          <t>4389</t>
+      <c r="G102" t="n">
+        <v>4389</v>
+      </c>
+      <c r="H102" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>4607</t>
         </is>
       </c>
     </row>
@@ -3513,9 +4115,15 @@
       <c r="F103" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="G103" t="inlineStr">
-        <is>
-          <t>4077</t>
+      <c r="G103" t="n">
+        <v>4077</v>
+      </c>
+      <c r="H103" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>4340</t>
         </is>
       </c>
     </row>
@@ -3544,9 +4152,15 @@
       <c r="F104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G104" t="inlineStr">
-        <is>
-          <t>2457</t>
+      <c r="G104" t="n">
+        <v>2457</v>
+      </c>
+      <c r="H104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>2492</t>
         </is>
       </c>
     </row>
@@ -3575,9 +4189,15 @@
       <c r="F105" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="G105" t="inlineStr">
-        <is>
-          <t>5241</t>
+      <c r="G105" t="n">
+        <v>5241</v>
+      </c>
+      <c r="H105" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>5825</t>
         </is>
       </c>
     </row>
@@ -3606,9 +4226,15 @@
       <c r="F106" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="G106" t="inlineStr">
-        <is>
-          <t>3946</t>
+      <c r="G106" t="n">
+        <v>3946</v>
+      </c>
+      <c r="H106" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>4082</t>
         </is>
       </c>
     </row>
@@ -3637,9 +4263,15 @@
       <c r="F107" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G107" t="inlineStr">
-        <is>
-          <t>3594</t>
+      <c r="G107" t="n">
+        <v>3594</v>
+      </c>
+      <c r="H107" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>3818</t>
         </is>
       </c>
     </row>
@@ -3668,9 +4300,15 @@
       <c r="F108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G108" t="inlineStr">
-        <is>
-          <t>2752</t>
+      <c r="G108" t="n">
+        <v>2752</v>
+      </c>
+      <c r="H108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>2804</t>
         </is>
       </c>
     </row>
@@ -3699,9 +4337,15 @@
       <c r="F109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G109" t="inlineStr">
-        <is>
-          <t>3483</t>
+      <c r="G109" t="n">
+        <v>3483</v>
+      </c>
+      <c r="H109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>3637</t>
         </is>
       </c>
     </row>
@@ -3730,9 +4374,15 @@
       <c r="F110" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G110" t="inlineStr">
-        <is>
-          <t>3574</t>
+      <c r="G110" t="n">
+        <v>3574</v>
+      </c>
+      <c r="H110" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>3655</t>
         </is>
       </c>
     </row>
@@ -3761,9 +4411,15 @@
       <c r="F111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G111" t="inlineStr">
-        <is>
-          <t>3698</t>
+      <c r="G111" t="n">
+        <v>3698</v>
+      </c>
+      <c r="H111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>3822</t>
         </is>
       </c>
     </row>
@@ -3792,9 +4448,15 @@
       <c r="F112" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="G112" t="inlineStr">
-        <is>
-          <t>4160</t>
+      <c r="G112" t="n">
+        <v>4160</v>
+      </c>
+      <c r="H112" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>4498</t>
         </is>
       </c>
     </row>
@@ -3823,9 +4485,15 @@
       <c r="F113" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="G113" t="inlineStr">
-        <is>
-          <t>2663</t>
+      <c r="G113" t="n">
+        <v>2663</v>
+      </c>
+      <c r="H113" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>2635</t>
         </is>
       </c>
     </row>
@@ -3854,9 +4522,15 @@
       <c r="F114" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="G114" t="inlineStr">
-        <is>
-          <t>2832</t>
+      <c r="G114" t="n">
+        <v>2832</v>
+      </c>
+      <c r="H114" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>3161</t>
         </is>
       </c>
     </row>
@@ -3885,9 +4559,15 @@
       <c r="F115" s="4" t="n">
         <v>28</v>
       </c>
-      <c r="G115" t="inlineStr">
-        <is>
-          <t>3710</t>
+      <c r="G115" t="n">
+        <v>3710</v>
+      </c>
+      <c r="H115" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>3806</t>
         </is>
       </c>
     </row>
@@ -3916,9 +4596,15 @@
       <c r="F116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G116" t="inlineStr">
-        <is>
-          <t>2946</t>
+      <c r="G116" t="n">
+        <v>2946</v>
+      </c>
+      <c r="H116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>3067</t>
         </is>
       </c>
     </row>
@@ -3947,9 +4633,15 @@
       <c r="F117" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G117" t="inlineStr">
-        <is>
-          <t>3733</t>
+      <c r="G117" t="n">
+        <v>3733</v>
+      </c>
+      <c r="H117" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>4111</t>
         </is>
       </c>
     </row>
@@ -3978,9 +4670,15 @@
       <c r="F118" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G118" t="inlineStr">
-        <is>
-          <t>3348</t>
+      <c r="G118" t="n">
+        <v>3348</v>
+      </c>
+      <c r="H118" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>3396</t>
         </is>
       </c>
     </row>
@@ -4009,9 +4707,15 @@
       <c r="F119" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="G119" t="inlineStr">
-        <is>
-          <t>3647</t>
+      <c r="G119" t="n">
+        <v>3647</v>
+      </c>
+      <c r="H119" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>3925</t>
         </is>
       </c>
     </row>
@@ -4040,9 +4744,15 @@
       <c r="F120" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="G120" t="inlineStr">
-        <is>
-          <t>3000</t>
+      <c r="G120" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H120" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>3077</t>
         </is>
       </c>
     </row>
@@ -4071,9 +4781,15 @@
       <c r="F121" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G121" t="inlineStr">
-        <is>
-          <t>3304</t>
+      <c r="G121" t="n">
+        <v>3304</v>
+      </c>
+      <c r="H121" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>3330</t>
         </is>
       </c>
     </row>
@@ -4102,9 +4818,15 @@
       <c r="F122" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G122" t="inlineStr">
-        <is>
-          <t>3309</t>
+      <c r="G122" t="n">
+        <v>3309</v>
+      </c>
+      <c r="H122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I122" t="inlineStr">
+        <is>
+          <t>3286</t>
         </is>
       </c>
     </row>
@@ -4133,9 +4855,15 @@
       <c r="F123" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G123" t="inlineStr">
-        <is>
-          <t>3676</t>
+      <c r="G123" t="n">
+        <v>3676</v>
+      </c>
+      <c r="H123" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>3908</t>
         </is>
       </c>
     </row>
@@ -4164,9 +4892,15 @@
       <c r="F124" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G124" t="inlineStr">
-        <is>
-          <t>3128</t>
+      <c r="G124" t="n">
+        <v>3128</v>
+      </c>
+      <c r="H124" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>3458</t>
         </is>
       </c>
     </row>
@@ -4195,9 +4929,15 @@
       <c r="F125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G125" t="inlineStr">
-        <is>
-          <t>2087</t>
+      <c r="G125" t="n">
+        <v>2087</v>
+      </c>
+      <c r="H125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I125" t="inlineStr">
+        <is>
+          <t>2097</t>
         </is>
       </c>
     </row>
@@ -4226,9 +4966,15 @@
       <c r="F126" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G126" t="inlineStr">
-        <is>
-          <t>2830</t>
+      <c r="G126" t="n">
+        <v>2830</v>
+      </c>
+      <c r="H126" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I126" t="inlineStr">
+        <is>
+          <t>2968</t>
         </is>
       </c>
     </row>
@@ -4257,9 +5003,15 @@
       <c r="F127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G127" t="inlineStr">
-        <is>
-          <t>2397</t>
+      <c r="G127" t="n">
+        <v>2397</v>
+      </c>
+      <c r="H127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I127" t="inlineStr">
+        <is>
+          <t>2442</t>
         </is>
       </c>
     </row>
@@ -4282,15 +5034,21 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F128" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G128" t="inlineStr">
-        <is>
-          <t>5025</t>
+      <c r="G128" t="n">
+        <v>5025</v>
+      </c>
+      <c r="H128" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I128" t="inlineStr">
+        <is>
+          <t>5573</t>
         </is>
       </c>
     </row>
@@ -4314,6 +5072,8 @@
       <c r="E129" t="inlineStr"/>
       <c r="F129" s="4" t="inlineStr"/>
       <c r="G129" t="inlineStr"/>
+      <c r="H129" s="4" t="inlineStr"/>
+      <c r="I129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="n">
@@ -4340,9 +5100,15 @@
       <c r="F130" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G130" t="inlineStr">
-        <is>
-          <t>2668</t>
+      <c r="G130" t="n">
+        <v>2668</v>
+      </c>
+      <c r="H130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I130" t="inlineStr">
+        <is>
+          <t>2755</t>
         </is>
       </c>
     </row>
@@ -4371,9 +5137,15 @@
       <c r="F131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G131" t="inlineStr">
-        <is>
-          <t>2798</t>
+      <c r="G131" t="n">
+        <v>2798</v>
+      </c>
+      <c r="H131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I131" t="inlineStr">
+        <is>
+          <t>2772</t>
         </is>
       </c>
     </row>
@@ -4402,9 +5174,15 @@
       <c r="F132" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G132" t="inlineStr">
-        <is>
-          <t>3763</t>
+      <c r="G132" t="n">
+        <v>3763</v>
+      </c>
+      <c r="H132" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="I132" t="inlineStr">
+        <is>
+          <t>3960</t>
         </is>
       </c>
     </row>
@@ -4428,6 +5206,8 @@
       <c r="E133" t="inlineStr"/>
       <c r="F133" s="4" t="inlineStr"/>
       <c r="G133" t="inlineStr"/>
+      <c r="H133" s="4" t="inlineStr"/>
+      <c r="I133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="n">
@@ -4454,9 +5234,15 @@
       <c r="F134" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="G134" t="inlineStr">
-        <is>
-          <t>2794</t>
+      <c r="G134" t="n">
+        <v>2794</v>
+      </c>
+      <c r="H134" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I134" t="inlineStr">
+        <is>
+          <t>2883</t>
         </is>
       </c>
     </row>
@@ -4485,9 +5271,15 @@
       <c r="F135" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G135" t="inlineStr">
-        <is>
-          <t>2492</t>
+      <c r="G135" t="n">
+        <v>2492</v>
+      </c>
+      <c r="H135" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I135" t="inlineStr">
+        <is>
+          <t>2471</t>
         </is>
       </c>
     </row>
@@ -4516,9 +5308,15 @@
       <c r="F136" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="G136" t="inlineStr">
-        <is>
-          <t>2932</t>
+      <c r="G136" t="n">
+        <v>2932</v>
+      </c>
+      <c r="H136" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="I136" t="inlineStr">
+        <is>
+          <t>2894</t>
         </is>
       </c>
     </row>
@@ -4547,9 +5345,15 @@
       <c r="F137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G137" t="inlineStr">
-        <is>
-          <t>2134</t>
+      <c r="G137" t="n">
+        <v>2134</v>
+      </c>
+      <c r="H137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I137" t="inlineStr">
+        <is>
+          <t>2154</t>
         </is>
       </c>
     </row>
@@ -4573,6 +5377,8 @@
       <c r="E138" t="inlineStr"/>
       <c r="F138" s="4" t="inlineStr"/>
       <c r="G138" t="inlineStr"/>
+      <c r="H138" s="4" t="inlineStr"/>
+      <c r="I138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -4594,6 +5400,8 @@
       <c r="E139" t="inlineStr"/>
       <c r="F139" s="4" t="inlineStr"/>
       <c r="G139" t="inlineStr"/>
+      <c r="H139" s="4" t="inlineStr"/>
+      <c r="I139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -4615,6 +5423,8 @@
       <c r="E140" t="inlineStr"/>
       <c r="F140" s="4" t="inlineStr"/>
       <c r="G140" t="inlineStr"/>
+      <c r="H140" s="4" t="inlineStr"/>
+      <c r="I140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="n">
@@ -4641,9 +5451,15 @@
       <c r="F141" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G141" t="inlineStr">
-        <is>
-          <t>2003</t>
+      <c r="G141" t="n">
+        <v>2003</v>
+      </c>
+      <c r="H141" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I141" t="inlineStr">
+        <is>
+          <t>2012</t>
         </is>
       </c>
     </row>
@@ -4667,6 +5483,8 @@
       <c r="E142" t="inlineStr"/>
       <c r="F142" s="4" t="inlineStr"/>
       <c r="G142" t="inlineStr"/>
+      <c r="H142" s="4" t="inlineStr"/>
+      <c r="I142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="n">
@@ -4688,6 +5506,8 @@
       <c r="E143" t="inlineStr"/>
       <c r="F143" s="4" t="inlineStr"/>
       <c r="G143" t="inlineStr"/>
+      <c r="H143" s="4" t="inlineStr"/>
+      <c r="I143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -4709,6 +5529,8 @@
       <c r="E144" t="inlineStr"/>
       <c r="F144" s="4" t="inlineStr"/>
       <c r="G144" t="inlineStr"/>
+      <c r="H144" s="4" t="inlineStr"/>
+      <c r="I144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -4730,6 +5552,8 @@
       <c r="E145" t="inlineStr"/>
       <c r="F145" s="4" t="inlineStr"/>
       <c r="G145" t="inlineStr"/>
+      <c r="H145" s="4" t="inlineStr"/>
+      <c r="I145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -4751,6 +5575,8 @@
       <c r="E146" t="inlineStr"/>
       <c r="F146" s="4" t="inlineStr"/>
       <c r="G146" t="inlineStr"/>
+      <c r="H146" s="4" t="inlineStr"/>
+      <c r="I146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -4772,6 +5598,8 @@
       <c r="E147" t="inlineStr"/>
       <c r="F147" s="4" t="inlineStr"/>
       <c r="G147" t="inlineStr"/>
+      <c r="H147" s="4" t="inlineStr"/>
+      <c r="I147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -4793,6 +5621,8 @@
       <c r="E148" t="inlineStr"/>
       <c r="F148" s="4" t="inlineStr"/>
       <c r="G148" t="inlineStr"/>
+      <c r="H148" s="4" t="inlineStr"/>
+      <c r="I148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="n">
@@ -4814,6 +5644,8 @@
       <c r="E149" t="inlineStr"/>
       <c r="F149" s="4" t="inlineStr"/>
       <c r="G149" t="inlineStr"/>
+      <c r="H149" s="4" t="inlineStr"/>
+      <c r="I149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="n">
@@ -4835,6 +5667,8 @@
       <c r="E150" t="inlineStr"/>
       <c r="F150" s="4" t="inlineStr"/>
       <c r="G150" t="inlineStr"/>
+      <c r="H150" s="4" t="inlineStr"/>
+      <c r="I150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="n">
@@ -4856,6 +5690,8 @@
       <c r="E151" t="inlineStr"/>
       <c r="F151" s="4" t="inlineStr"/>
       <c r="G151" t="inlineStr"/>
+      <c r="H151" s="4" t="inlineStr"/>
+      <c r="I151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="n">
@@ -4877,6 +5713,8 @@
       <c r="E152" t="inlineStr"/>
       <c r="F152" s="4" t="inlineStr"/>
       <c r="G152" t="inlineStr"/>
+      <c r="H152" s="4" t="inlineStr"/>
+      <c r="I152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" t="n">
@@ -4898,6 +5736,8 @@
       <c r="E153" t="inlineStr"/>
       <c r="F153" s="4" t="inlineStr"/>
       <c r="G153" t="inlineStr"/>
+      <c r="H153" s="4" t="inlineStr"/>
+      <c r="I153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" t="n">
@@ -4924,9 +5764,15 @@
       <c r="F154" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="G154" t="inlineStr">
-        <is>
-          <t>2381</t>
+      <c r="G154" t="n">
+        <v>2381</v>
+      </c>
+      <c r="H154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I154" t="inlineStr">
+        <is>
+          <t>2374</t>
         </is>
       </c>
     </row>
@@ -4950,6 +5796,8 @@
       <c r="E155" t="inlineStr"/>
       <c r="F155" s="4" t="inlineStr"/>
       <c r="G155" t="inlineStr"/>
+      <c r="H155" s="4" t="inlineStr"/>
+      <c r="I155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="n">
@@ -4976,9 +5824,15 @@
       <c r="F156" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="G156" t="inlineStr">
-        <is>
-          <t>5283</t>
+      <c r="G156" t="n">
+        <v>5283</v>
+      </c>
+      <c r="H156" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="I156" t="inlineStr">
+        <is>
+          <t>5718</t>
         </is>
       </c>
     </row>
@@ -5007,7 +5861,13 @@
       <c r="F157" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G157" t="inlineStr">
+      <c r="G157" t="n">
+        <v>0</v>
+      </c>
+      <c r="H157" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I157" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5038,9 +5898,15 @@
       <c r="F158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G158" t="inlineStr">
-        <is>
-          <t>2523</t>
+      <c r="G158" t="n">
+        <v>2523</v>
+      </c>
+      <c r="H158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I158" t="inlineStr">
+        <is>
+          <t>2550</t>
         </is>
       </c>
     </row>
@@ -5069,9 +5935,15 @@
       <c r="F159" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="G159" t="inlineStr">
-        <is>
-          <t>5498</t>
+      <c r="G159" t="n">
+        <v>5498</v>
+      </c>
+      <c r="H159" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="I159" t="inlineStr">
+        <is>
+          <t>5940</t>
         </is>
       </c>
     </row>
@@ -5100,7 +5972,13 @@
       <c r="F160" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G160" t="inlineStr">
+      <c r="G160" t="n">
+        <v>0</v>
+      </c>
+      <c r="H160" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I160" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5131,9 +6009,15 @@
       <c r="F161" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G161" t="inlineStr">
-        <is>
-          <t>3211</t>
+      <c r="G161" t="n">
+        <v>3211</v>
+      </c>
+      <c r="H161" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I161" t="inlineStr">
+        <is>
+          <t>3342</t>
         </is>
       </c>
     </row>
@@ -5162,7 +6046,13 @@
       <c r="F162" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G162" t="inlineStr">
+      <c r="G162" t="n">
+        <v>0</v>
+      </c>
+      <c r="H162" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I162" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5193,17 +6083,21 @@
       <c r="F163" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G163" t="inlineStr">
-        <is>
-          <t>3097</t>
+      <c r="G163" t="n">
+        <v>3097</v>
+      </c>
+      <c r="H163" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I163" t="inlineStr">
+        <is>
+          <t>3178</t>
         </is>
       </c>
     </row>
     <row r="164">
-      <c r="A164" t="inlineStr">
-        <is>
-          <t>56829330</t>
-        </is>
+      <c r="A164" t="n">
+        <v>56829330</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
@@ -5220,17 +6114,21 @@
       <c r="F164" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="G164" t="inlineStr">
-        <is>
-          <t>3125</t>
+      <c r="G164" t="n">
+        <v>3125</v>
+      </c>
+      <c r="H164" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="I164" t="inlineStr">
+        <is>
+          <t>3172</t>
         </is>
       </c>
     </row>
     <row r="165">
-      <c r="A165" t="inlineStr">
-        <is>
-          <t>9321819</t>
-        </is>
+      <c r="A165" t="n">
+        <v>9321819</v>
       </c>
       <c r="B165" t="inlineStr">
         <is>
@@ -5247,17 +6145,15 @@
       <c r="F165" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="G165" t="inlineStr">
-        <is>
-          <t>2966</t>
-        </is>
-      </c>
+      <c r="G165" t="n">
+        <v>2966</v>
+      </c>
+      <c r="H165" s="4" t="inlineStr"/>
+      <c r="I165" t="inlineStr"/>
     </row>
     <row r="166">
-      <c r="A166" t="inlineStr">
-        <is>
-          <t>15436348</t>
-        </is>
+      <c r="A166" t="n">
+        <v>15436348</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>
@@ -5274,17 +6170,21 @@
       <c r="F166" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G166" t="inlineStr">
-        <is>
-          <t>1779</t>
+      <c r="G166" t="n">
+        <v>1779</v>
+      </c>
+      <c r="H166" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I166" t="inlineStr">
+        <is>
+          <t>1770</t>
         </is>
       </c>
     </row>
     <row r="167">
-      <c r="A167" t="inlineStr">
-        <is>
-          <t>20372140</t>
-        </is>
+      <c r="A167" t="n">
+        <v>20372140</v>
       </c>
       <c r="B167" t="inlineStr">
         <is>
@@ -5301,17 +6201,21 @@
       <c r="F167" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="G167" t="inlineStr">
-        <is>
-          <t>2518</t>
+      <c r="G167" t="n">
+        <v>2518</v>
+      </c>
+      <c r="H167" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="I167" t="inlineStr">
+        <is>
+          <t>2595</t>
         </is>
       </c>
     </row>
     <row r="168">
-      <c r="A168" t="inlineStr">
-        <is>
-          <t>47928278</t>
-        </is>
+      <c r="A168" t="n">
+        <v>47928278</v>
       </c>
       <c r="B168" t="inlineStr">
         <is>
@@ -5322,23 +6226,27 @@
       <c r="D168" t="inlineStr"/>
       <c r="E168" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F168" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="G168" t="inlineStr">
-        <is>
-          <t>6129</t>
+      <c r="G168" t="n">
+        <v>6129</v>
+      </c>
+      <c r="H168" s="3" t="n">
+        <v>39</v>
+      </c>
+      <c r="I168" t="inlineStr">
+        <is>
+          <t>6924</t>
         </is>
       </c>
     </row>
     <row r="169">
-      <c r="A169" t="inlineStr">
-        <is>
-          <t>57442184</t>
-        </is>
+      <c r="A169" t="n">
+        <v>57442184</v>
       </c>
       <c r="B169" t="inlineStr">
         <is>
@@ -5355,17 +6263,15 @@
       <c r="F169" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="G169" t="inlineStr">
-        <is>
-          <t>2288</t>
-        </is>
-      </c>
+      <c r="G169" t="n">
+        <v>2288</v>
+      </c>
+      <c r="H169" s="4" t="inlineStr"/>
+      <c r="I169" t="inlineStr"/>
     </row>
     <row r="170">
-      <c r="A170" t="inlineStr">
-        <is>
-          <t>58615957</t>
-        </is>
+      <c r="A170" t="n">
+        <v>58615957</v>
       </c>
       <c r="B170" t="inlineStr">
         <is>
@@ -5382,17 +6288,21 @@
       <c r="F170" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G170" t="inlineStr">
+      <c r="G170" t="n">
+        <v>2608</v>
+      </c>
+      <c r="H170" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I170" t="inlineStr">
         <is>
           <t>2608</t>
         </is>
       </c>
     </row>
     <row r="171">
-      <c r="A171" t="inlineStr">
-        <is>
-          <t>12333251</t>
-        </is>
+      <c r="A171" t="n">
+        <v>12333251</v>
       </c>
       <c r="B171" t="inlineStr">
         <is>
@@ -5409,17 +6319,21 @@
       <c r="F171" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G171" t="inlineStr">
-        <is>
-          <t>3067</t>
+      <c r="G171" t="n">
+        <v>3067</v>
+      </c>
+      <c r="H171" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="I171" t="inlineStr">
+        <is>
+          <t>3567</t>
         </is>
       </c>
     </row>
     <row r="172">
-      <c r="A172" t="inlineStr">
-        <is>
-          <t>27113069</t>
-        </is>
+      <c r="A172" t="n">
+        <v>27113069</v>
       </c>
       <c r="B172" t="inlineStr">
         <is>
@@ -5430,23 +6344,27 @@
       <c r="D172" t="inlineStr"/>
       <c r="E172" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F172" s="3" t="n">
         <v>37</v>
       </c>
-      <c r="G172" t="inlineStr">
-        <is>
-          <t>5701</t>
+      <c r="G172" t="n">
+        <v>5701</v>
+      </c>
+      <c r="H172" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="I172" t="inlineStr">
+        <is>
+          <t>6023</t>
         </is>
       </c>
     </row>
     <row r="173">
-      <c r="A173" t="inlineStr">
-        <is>
-          <t>47533851</t>
-        </is>
+      <c r="A173" t="n">
+        <v>47533851</v>
       </c>
       <c r="B173" t="inlineStr">
         <is>
@@ -5463,17 +6381,21 @@
       <c r="F173" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="G173" t="inlineStr">
-        <is>
-          <t>2286</t>
+      <c r="G173" t="n">
+        <v>2286</v>
+      </c>
+      <c r="H173" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="I173" t="inlineStr">
+        <is>
+          <t>2336</t>
         </is>
       </c>
     </row>
     <row r="174">
-      <c r="A174" t="inlineStr">
-        <is>
-          <t>50742014</t>
-        </is>
+      <c r="A174" t="n">
+        <v>50742014</v>
       </c>
       <c r="B174" t="inlineStr">
         <is>
@@ -5490,17 +6412,21 @@
       <c r="F174" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G174" t="inlineStr">
+      <c r="G174" t="n">
+        <v>0</v>
+      </c>
+      <c r="H174" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I174" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
     </row>
     <row r="175">
-      <c r="A175" t="inlineStr">
-        <is>
-          <t>53269862</t>
-        </is>
+      <c r="A175" t="n">
+        <v>53269862</v>
       </c>
       <c r="B175" t="inlineStr">
         <is>
@@ -5517,17 +6443,21 @@
       <c r="F175" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G175" t="inlineStr">
-        <is>
-          <t>2062</t>
+      <c r="G175" t="n">
+        <v>2062</v>
+      </c>
+      <c r="H175" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I175" t="inlineStr">
+        <is>
+          <t>2057</t>
         </is>
       </c>
     </row>
     <row r="176">
-      <c r="A176" t="inlineStr">
-        <is>
-          <t>54924790</t>
-        </is>
+      <c r="A176" t="n">
+        <v>54924790</v>
       </c>
       <c r="B176" t="inlineStr">
         <is>
@@ -5544,17 +6474,21 @@
       <c r="F176" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G176" t="inlineStr">
-        <is>
-          <t>3019</t>
+      <c r="G176" t="n">
+        <v>3019</v>
+      </c>
+      <c r="H176" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I176" t="inlineStr">
+        <is>
+          <t>3054</t>
         </is>
       </c>
     </row>
     <row r="177">
-      <c r="A177" t="inlineStr">
-        <is>
-          <t>55963040</t>
-        </is>
+      <c r="A177" t="n">
+        <v>55963040</v>
       </c>
       <c r="B177" t="inlineStr">
         <is>
@@ -5571,17 +6505,21 @@
       <c r="F177" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G177" t="inlineStr">
-        <is>
-          <t>2399</t>
+      <c r="G177" t="n">
+        <v>2399</v>
+      </c>
+      <c r="H177" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I177" t="inlineStr">
+        <is>
+          <t>2386</t>
         </is>
       </c>
     </row>
     <row r="178">
-      <c r="A178" t="inlineStr">
-        <is>
-          <t>56691087</t>
-        </is>
+      <c r="A178" t="n">
+        <v>56691087</v>
       </c>
       <c r="B178" t="inlineStr">
         <is>
@@ -5598,17 +6536,21 @@
       <c r="F178" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G178" t="inlineStr">
-        <is>
-          <t>1882</t>
+      <c r="G178" t="n">
+        <v>1882</v>
+      </c>
+      <c r="H178" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I178" t="inlineStr">
+        <is>
+          <t>1891</t>
         </is>
       </c>
     </row>
     <row r="179">
-      <c r="A179" t="inlineStr">
-        <is>
-          <t>57339836</t>
-        </is>
+      <c r="A179" t="n">
+        <v>57339836</v>
       </c>
       <c r="B179" t="inlineStr">
         <is>
@@ -5625,17 +6567,21 @@
       <c r="F179" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="G179" t="inlineStr">
-        <is>
-          <t>1149</t>
+      <c r="G179" t="n">
+        <v>1149</v>
+      </c>
+      <c r="H179" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I179" t="inlineStr">
+        <is>
+          <t>1167</t>
         </is>
       </c>
     </row>
     <row r="180">
-      <c r="A180" t="inlineStr">
-        <is>
-          <t>57605565</t>
-        </is>
+      <c r="A180" t="n">
+        <v>57605565</v>
       </c>
       <c r="B180" t="inlineStr">
         <is>
@@ -5652,17 +6598,21 @@
       <c r="F180" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G180" t="inlineStr">
-        <is>
-          <t>1560</t>
+      <c r="G180" t="n">
+        <v>1560</v>
+      </c>
+      <c r="H180" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I180" t="inlineStr">
+        <is>
+          <t>1559</t>
         </is>
       </c>
     </row>
     <row r="181">
-      <c r="A181" t="inlineStr">
-        <is>
-          <t>58132159</t>
-        </is>
+      <c r="A181" t="n">
+        <v>58132159</v>
       </c>
       <c r="B181" t="inlineStr">
         <is>
@@ -5679,17 +6629,21 @@
       <c r="F181" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G181" t="inlineStr">
+      <c r="G181" t="n">
+        <v>0</v>
+      </c>
+      <c r="H181" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I181" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
     </row>
     <row r="182">
-      <c r="A182" t="inlineStr">
-        <is>
-          <t>58562596</t>
-        </is>
+      <c r="A182" t="n">
+        <v>58562596</v>
       </c>
       <c r="B182" t="inlineStr">
         <is>
@@ -5706,17 +6660,21 @@
       <c r="F182" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G182" t="inlineStr">
+      <c r="G182" t="n">
+        <v>0</v>
+      </c>
+      <c r="H182" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I182" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
     </row>
     <row r="183">
-      <c r="A183" t="inlineStr">
-        <is>
-          <t>58615925</t>
-        </is>
+      <c r="A183" t="n">
+        <v>58615925</v>
       </c>
       <c r="B183" t="inlineStr">
         <is>
@@ -5733,17 +6691,21 @@
       <c r="F183" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G183" t="inlineStr">
-        <is>
-          <t>2877</t>
+      <c r="G183" t="n">
+        <v>2877</v>
+      </c>
+      <c r="H183" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="I183" t="inlineStr">
+        <is>
+          <t>2968</t>
         </is>
       </c>
     </row>
     <row r="184">
-      <c r="A184" t="inlineStr">
-        <is>
-          <t>58635041</t>
-        </is>
+      <c r="A184" t="n">
+        <v>58635041</v>
       </c>
       <c r="B184" t="inlineStr">
         <is>
@@ -5760,17 +6722,21 @@
       <c r="F184" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="G184" t="inlineStr">
-        <is>
-          <t>1608</t>
+      <c r="G184" t="n">
+        <v>1608</v>
+      </c>
+      <c r="H184" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I184" t="inlineStr">
+        <is>
+          <t>1635</t>
         </is>
       </c>
     </row>
     <row r="185">
-      <c r="A185" t="inlineStr">
-        <is>
-          <t>58644547</t>
-        </is>
+      <c r="A185" t="n">
+        <v>58644547</v>
       </c>
       <c r="B185" t="inlineStr">
         <is>
@@ -5787,17 +6753,21 @@
       <c r="F185" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="G185" t="inlineStr">
-        <is>
-          <t>1632</t>
+      <c r="G185" t="n">
+        <v>1632</v>
+      </c>
+      <c r="H185" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I185" t="inlineStr">
+        <is>
+          <t>1712</t>
         </is>
       </c>
     </row>
     <row r="186">
-      <c r="A186" t="inlineStr">
-        <is>
-          <t>48005945</t>
-        </is>
+      <c r="A186" t="n">
+        <v>48005945</v>
       </c>
       <c r="B186" t="inlineStr">
         <is>
@@ -5814,9 +6784,102 @@
       <c r="F186" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G186" t="inlineStr">
-        <is>
-          <t>2668</t>
+      <c r="G186" t="n">
+        <v>2668</v>
+      </c>
+      <c r="H186" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I186" t="inlineStr">
+        <is>
+          <t>2661</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>54714516</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>ёмιいч</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr"/>
+      <c r="D187" t="inlineStr"/>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F187" s="4" t="inlineStr"/>
+      <c r="G187" t="inlineStr"/>
+      <c r="H187" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="I187" t="inlineStr">
+        <is>
+          <t>2890</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>58689512</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>Player-58689512</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr"/>
+      <c r="D188" t="inlineStr"/>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F188" s="4" t="inlineStr"/>
+      <c r="G188" t="inlineStr"/>
+      <c r="H188" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="I188" t="inlineStr">
+        <is>
+          <t>1441</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>58705573</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>Player-58705573</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr"/>
+      <c r="D189" t="inlineStr"/>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F189" s="4" t="inlineStr"/>
+      <c r="G189" t="inlineStr"/>
+      <c r="H189" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I189" t="inlineStr">
+        <is>
+          <t>1274</t>
         </is>
       </c>
     </row>

</xml_diff>